<commit_message>
General advancements, such as level screen improvement, level 3 added, and game over screen.
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="388">
   <si>
     <t>Difficulty</t>
   </si>
@@ -249,9 +249,6 @@
     <t>One hundred</t>
   </si>
   <si>
-    <t>What president signed the Executive order 6102</t>
-  </si>
-  <si>
     <t>Franklin D. Roosevelt</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>Nick Leeson</t>
   </si>
   <si>
-    <t>Jérôme Kerviel</t>
-  </si>
-  <si>
     <t>A rogue trader hid a loss of over $35 million</t>
   </si>
   <si>
@@ -1038,15 +1032,6 @@
     <t>Who was Moses Amschel Bauer?</t>
   </si>
   <si>
-    <t>Who was Mayer Amschel Rothschild's father?</t>
-  </si>
-  <si>
-    <t>The Judengasse foreign currency and bullion trader Moses Amschel Bauer</t>
-  </si>
-  <si>
-    <t>The banker and financier Nathaniel Rothschild</t>
-  </si>
-  <si>
     <t>The seal of the Finance Ministry of Hesse</t>
   </si>
   <si>
@@ -1168,6 +1153,33 @@
   </si>
   <si>
     <t>It was the Roman coin after the denarius</t>
+  </si>
+  <si>
+    <t>Amschel Mayer Rothschild's father</t>
+  </si>
+  <si>
+    <t>The 25th Secretary of the Treasury</t>
+  </si>
+  <si>
+    <t>The 3rd Chairman of the Federal Reserve</t>
+  </si>
+  <si>
+    <t>An obligation for its writer</t>
+  </si>
+  <si>
+    <t>An obligation to sell shares</t>
+  </si>
+  <si>
+    <t>An option to buy shares</t>
+  </si>
+  <si>
+    <t>Money based on trust</t>
+  </si>
+  <si>
+    <t>Jerome Kerviel</t>
+  </si>
+  <si>
+    <t>Which president signed the Executive order 6102</t>
   </si>
 </sst>
 </file>
@@ -1502,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1607,7 +1619,7 @@
         <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1621,7 +1633,7 @@
         <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
@@ -1635,7 +1647,7 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -1655,7 +1667,7 @@
         <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
         <v>46</v>
@@ -1681,7 +1693,7 @@
         <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1709,10 +1721,10 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
         <v>59</v>
@@ -1763,16 +1775,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
+        <v>387</v>
+      </c>
+      <c r="D14" t="s">
         <v>77</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>78</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>79</v>
-      </c>
-      <c r="F14" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1783,16 +1795,16 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" t="s">
         <v>86</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
         <v>87</v>
-      </c>
-      <c r="E15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1800,16 +1812,16 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
         <v>103</v>
       </c>
-      <c r="D16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>104</v>
-      </c>
-      <c r="F16" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1817,16 +1829,16 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
         <v>107</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>108</v>
-      </c>
-      <c r="F17" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1834,16 +1846,16 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" t="s">
         <v>111</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>112</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>113</v>
-      </c>
-      <c r="F18" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1851,19 +1863,19 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" t="s">
         <v>115</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>116</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>117</v>
-      </c>
-      <c r="F19" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1874,16 +1886,16 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" t="s">
         <v>125</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>126</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>127</v>
-      </c>
-      <c r="F20" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1891,16 +1903,16 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" t="s">
         <v>129</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>130</v>
-      </c>
-      <c r="F21" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1911,16 +1923,16 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" t="s">
         <v>139</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>140</v>
       </c>
-      <c r="E22" t="s">
-        <v>141</v>
-      </c>
       <c r="F22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1928,16 +1940,16 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" t="s">
         <v>165</v>
       </c>
-      <c r="D23" t="s">
-        <v>164</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>166</v>
-      </c>
-      <c r="F23" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1945,16 +1957,16 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" t="s">
         <v>168</v>
       </c>
-      <c r="E24" t="s">
-        <v>169</v>
-      </c>
       <c r="F24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1962,16 +1974,16 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" t="s">
         <v>167</v>
-      </c>
-      <c r="E25" t="s">
-        <v>169</v>
-      </c>
-      <c r="F25" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1979,19 +1991,19 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" t="s">
         <v>150</v>
       </c>
-      <c r="E26" t="s">
-        <v>151</v>
-      </c>
       <c r="F26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1999,16 +2011,16 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
+        <v>169</v>
+      </c>
+      <c r="D27" t="s">
         <v>170</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>171</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>172</v>
-      </c>
-      <c r="F27" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2016,16 +2028,16 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28" t="s">
+        <v>234</v>
+      </c>
+      <c r="F28" t="s">
         <v>235</v>
-      </c>
-      <c r="D28" t="s">
-        <v>234</v>
-      </c>
-      <c r="E28" t="s">
-        <v>236</v>
-      </c>
-      <c r="F28" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2033,13 +2045,13 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D29" t="s">
         <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F29" t="s">
         <v>47</v>
@@ -2050,16 +2062,16 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" t="s">
         <v>191</v>
       </c>
-      <c r="D30" t="s">
-        <v>192</v>
-      </c>
       <c r="E30" t="s">
-        <v>193</v>
+        <v>386</v>
       </c>
       <c r="F30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2067,16 +2079,16 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D31" t="s">
-        <v>193</v>
+        <v>386</v>
       </c>
       <c r="E31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2084,16 +2096,16 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
+        <v>203</v>
+      </c>
+      <c r="D32" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F32" t="s">
         <v>205</v>
-      </c>
-      <c r="D32" t="s">
-        <v>204</v>
-      </c>
-      <c r="E32" t="s">
-        <v>206</v>
-      </c>
-      <c r="F32" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2101,16 +2113,16 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
+        <v>206</v>
+      </c>
+      <c r="D33" t="s">
+        <v>207</v>
+      </c>
+      <c r="E33" t="s">
         <v>208</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>209</v>
-      </c>
-      <c r="E33" t="s">
-        <v>210</v>
-      </c>
-      <c r="F33" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2118,16 +2130,16 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
+        <v>217</v>
+      </c>
+      <c r="D34" t="s">
+        <v>218</v>
+      </c>
+      <c r="E34" t="s">
         <v>219</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F34" t="s">
         <v>220</v>
-      </c>
-      <c r="E34" t="s">
-        <v>221</v>
-      </c>
-      <c r="F34" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2135,16 +2147,16 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" t="s">
+        <v>225</v>
+      </c>
+      <c r="E35" t="s">
         <v>224</v>
       </c>
-      <c r="D35" t="s">
-        <v>227</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>226</v>
-      </c>
-      <c r="F35" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2152,16 +2164,16 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" t="s">
         <v>225</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
         <v>226</v>
-      </c>
-      <c r="E36" t="s">
-        <v>227</v>
-      </c>
-      <c r="F36" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2169,16 +2181,16 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D37" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E37" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2186,315 +2198,393 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E38" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" t="s">
         <v>238</v>
       </c>
-      <c r="E38" t="s">
-        <v>239</v>
-      </c>
-      <c r="F38" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="39" spans="1:6">
+      <c r="A39">
+        <v>10</v>
+      </c>
       <c r="B39" t="s">
+        <v>253</v>
+      </c>
+      <c r="D39" t="s">
+        <v>254</v>
+      </c>
+      <c r="E39" t="s">
         <v>255</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
         <v>256</v>
       </c>
-      <c r="E39" t="s">
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
         <v>257</v>
       </c>
-      <c r="F39" t="s">
+      <c r="D40" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="B40" t="s">
+      <c r="E40" t="s">
         <v>259</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" t="s">
         <v>260</v>
       </c>
-      <c r="E40" t="s">
-        <v>261</v>
-      </c>
-      <c r="F40" t="s">
-        <v>262</v>
-      </c>
     </row>
     <row r="41" spans="1:6">
+      <c r="A41">
+        <v>10</v>
+      </c>
       <c r="B41" t="s">
+        <v>263</v>
+      </c>
+      <c r="D41" t="s">
+        <v>258</v>
+      </c>
+      <c r="E41" t="s">
+        <v>259</v>
+      </c>
+      <c r="F41" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>268</v>
+      </c>
+      <c r="D42" t="s">
         <v>265</v>
       </c>
-      <c r="D41" t="s">
-        <v>260</v>
-      </c>
-      <c r="E41" t="s">
-        <v>261</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E42" t="s">
+        <v>267</v>
+      </c>
+      <c r="F42" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="B42" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>269</v>
+      </c>
+      <c r="D43" t="s">
         <v>270</v>
       </c>
-      <c r="D42" t="s">
-        <v>267</v>
-      </c>
-      <c r="E42" t="s">
-        <v>269</v>
-      </c>
-      <c r="F42" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="B43" t="s">
+      <c r="E43" t="s">
         <v>271</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F43" t="s">
         <v>272</v>
       </c>
-      <c r="E43" t="s">
-        <v>273</v>
-      </c>
-      <c r="F43" t="s">
-        <v>274</v>
-      </c>
     </row>
     <row r="44" spans="1:6">
+      <c r="A44">
+        <v>10</v>
+      </c>
       <c r="B44" t="s">
+        <v>291</v>
+      </c>
+      <c r="D44" t="s">
         <v>293</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
+        <v>292</v>
+      </c>
+      <c r="F44" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>286</v>
+      </c>
+      <c r="D45" t="s">
+        <v>279</v>
+      </c>
+      <c r="E45" t="s">
+        <v>280</v>
+      </c>
+      <c r="F45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>285</v>
+      </c>
+      <c r="D46" t="s">
+        <v>282</v>
+      </c>
+      <c r="E46" t="s">
+        <v>283</v>
+      </c>
+      <c r="F46" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>287</v>
+      </c>
+      <c r="D47" t="s">
+        <v>290</v>
+      </c>
+      <c r="E47" t="s">
+        <v>288</v>
+      </c>
+      <c r="F47" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
         <v>295</v>
       </c>
-      <c r="E44" t="s">
-        <v>294</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="C48" t="s">
+        <v>299</v>
+      </c>
+      <c r="D48" t="s">
+        <v>297</v>
+      </c>
+      <c r="E48" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="B45" t="s">
-        <v>288</v>
-      </c>
-      <c r="D45" t="s">
-        <v>281</v>
-      </c>
-      <c r="E45" t="s">
-        <v>282</v>
-      </c>
-      <c r="F45" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="B46" t="s">
-        <v>287</v>
-      </c>
-      <c r="D46" t="s">
-        <v>284</v>
-      </c>
-      <c r="E46" t="s">
-        <v>285</v>
-      </c>
-      <c r="F46" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="B47" t="s">
-        <v>289</v>
-      </c>
-      <c r="D47" t="s">
-        <v>292</v>
-      </c>
-      <c r="E47" t="s">
-        <v>290</v>
-      </c>
-      <c r="F47" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="B48" t="s">
-        <v>297</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="F48" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>303</v>
+      </c>
+      <c r="D49" t="s">
+        <v>300</v>
+      </c>
+      <c r="E49" t="s">
         <v>301</v>
       </c>
-      <c r="D48" t="s">
-        <v>299</v>
-      </c>
-      <c r="E48" t="s">
-        <v>298</v>
-      </c>
-      <c r="F48" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49" t="s">
+      <c r="F49" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>304</v>
+      </c>
+      <c r="D50" t="s">
         <v>305</v>
       </c>
-      <c r="D49" t="s">
-        <v>302</v>
-      </c>
-      <c r="E49" t="s">
-        <v>303</v>
-      </c>
-      <c r="F49" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50" t="s">
+      <c r="E50" t="s">
         <v>306</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>307</v>
       </c>
-      <c r="E50" t="s">
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>309</v>
+      </c>
+      <c r="D51" t="s">
         <v>308</v>
       </c>
-      <c r="F50" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="B51" t="s">
+      <c r="E51" t="s">
+        <v>310</v>
+      </c>
+      <c r="F51" t="s">
         <v>311</v>
       </c>
-      <c r="D51" t="s">
-        <v>310</v>
-      </c>
-      <c r="E51" t="s">
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
         <v>312</v>
       </c>
-      <c r="F51" t="s">
+      <c r="D52" t="s">
+        <v>323</v>
+      </c>
+      <c r="E52" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="B52" t="s">
+      <c r="F52" t="s">
         <v>314</v>
       </c>
-      <c r="D52" t="s">
-        <v>325</v>
-      </c>
-      <c r="E52" t="s">
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
         <v>315</v>
       </c>
-      <c r="F52" t="s">
+      <c r="D53" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="53" spans="2:6">
-      <c r="B53" t="s">
+      <c r="E53" t="s">
         <v>317</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>318</v>
       </c>
-      <c r="E53" t="s">
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
         <v>319</v>
       </c>
-      <c r="F53" t="s">
+      <c r="D54" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="54" spans="2:6">
-      <c r="B54" t="s">
+      <c r="E54" t="s">
         <v>321</v>
       </c>
-      <c r="D54" t="s">
+      <c r="F54" t="s">
         <v>322</v>
       </c>
-      <c r="E54" t="s">
-        <v>323</v>
-      </c>
-      <c r="F54" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6">
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>10</v>
+      </c>
       <c r="B55" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D55" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="E55" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F55" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>10</v>
+      </c>
       <c r="B56" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6">
+        <v>368</v>
+      </c>
+      <c r="D56" t="s">
+        <v>382</v>
+      </c>
+      <c r="E56" t="s">
+        <v>383</v>
+      </c>
+      <c r="F56" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>10</v>
+      </c>
       <c r="B57" t="s">
+        <v>354</v>
+      </c>
+      <c r="D57" t="s">
+        <v>355</v>
+      </c>
+      <c r="E57" t="s">
+        <v>356</v>
+      </c>
+      <c r="F57" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>358</v>
+      </c>
+      <c r="D58" t="s">
+        <v>361</v>
+      </c>
+      <c r="E58" t="s">
+        <v>360</v>
+      </c>
+      <c r="F58" t="s">
         <v>359</v>
       </c>
-      <c r="D57" t="s">
-        <v>360</v>
-      </c>
-      <c r="E57" t="s">
-        <v>361</v>
-      </c>
-      <c r="F57" t="s">
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="58" spans="2:6">
-      <c r="B58" t="s">
+      <c r="D59" t="s">
         <v>363</v>
       </c>
-      <c r="D58" t="s">
-        <v>366</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
+        <v>364</v>
+      </c>
+      <c r="F59" t="s">
         <v>365</v>
       </c>
-      <c r="F58" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6">
-      <c r="B59" t="s">
-        <v>367</v>
-      </c>
-      <c r="D59" t="s">
-        <v>368</v>
-      </c>
-      <c r="E59" t="s">
-        <v>369</v>
-      </c>
-      <c r="F59" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6">
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>10</v>
+      </c>
       <c r="B60" t="s">
-        <v>381</v>
+        <v>376</v>
+      </c>
+      <c r="D60" t="s">
+        <v>385</v>
       </c>
       <c r="E60" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F60" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -2504,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2631,7 +2721,7 @@
         <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2676,7 +2766,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
         <v>50</v>
@@ -2710,16 +2800,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" t="s">
         <v>81</v>
       </c>
-      <c r="D11" t="s">
-        <v>280</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>82</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2727,16 +2817,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
         <v>90</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>91</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>92</v>
-      </c>
-      <c r="F12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2744,16 +2834,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" t="s">
         <v>94</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>95</v>
-      </c>
-      <c r="F13" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2761,16 +2851,16 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
         <v>121</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>122</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>123</v>
-      </c>
-      <c r="F14" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2778,16 +2868,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
         <v>132</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>133</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>134</v>
-      </c>
-      <c r="F15" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2795,16 +2885,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" t="s">
         <v>144</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>145</v>
-      </c>
-      <c r="F16" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2812,16 +2902,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" t="s">
         <v>154</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>155</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>156</v>
-      </c>
-      <c r="F17" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2829,16 +2919,16 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" t="s">
         <v>158</v>
       </c>
-      <c r="D18" t="s">
-        <v>157</v>
-      </c>
-      <c r="E18" t="s">
-        <v>159</v>
-      </c>
       <c r="F18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2846,16 +2936,16 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19" t="s">
         <v>160</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>161</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>162</v>
-      </c>
-      <c r="F19" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2863,16 +2953,16 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" t="s">
         <v>176</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>177</v>
-      </c>
-      <c r="F20" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2880,13 +2970,13 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" t="s">
         <v>180</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>181</v>
-      </c>
-      <c r="E21" t="s">
-        <v>182</v>
       </c>
       <c r="F21" t="s">
         <v>46</v>
@@ -2897,16 +2987,16 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" t="s">
         <v>189</v>
       </c>
-      <c r="E22" t="s">
-        <v>190</v>
-      </c>
       <c r="F22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2914,16 +3004,16 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" t="s">
+        <v>194</v>
+      </c>
+      <c r="F23" t="s">
         <v>195</v>
-      </c>
-      <c r="D23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E23" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2931,75 +3021,90 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" t="s">
         <v>198</v>
       </c>
-      <c r="D24" t="s">
-        <v>200</v>
-      </c>
       <c r="E24" t="s">
+        <v>197</v>
+      </c>
+      <c r="F24" t="s">
         <v>199</v>
       </c>
-      <c r="F24" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="25" spans="1:6">
+      <c r="A25">
+        <v>15</v>
+      </c>
       <c r="B25" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D25" t="s">
+        <v>332</v>
+      </c>
+      <c r="E25" t="s">
+        <v>261</v>
+      </c>
+      <c r="F25" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>277</v>
+      </c>
+      <c r="D26" t="s">
+        <v>273</v>
+      </c>
+      <c r="E26" t="s">
+        <v>274</v>
+      </c>
+      <c r="F26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>328</v>
+      </c>
+      <c r="D27" t="s">
+        <v>329</v>
+      </c>
+      <c r="E27" t="s">
+        <v>330</v>
+      </c>
+      <c r="F27" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
         <v>334</v>
       </c>
-      <c r="E25" t="s">
-        <v>263</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="D28" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="B26" t="s">
-        <v>279</v>
-      </c>
-      <c r="D26" t="s">
-        <v>275</v>
-      </c>
-      <c r="E26" t="s">
-        <v>276</v>
-      </c>
-      <c r="F26" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="B27" t="s">
-        <v>330</v>
-      </c>
-      <c r="D27" t="s">
-        <v>331</v>
-      </c>
-      <c r="E27" t="s">
-        <v>332</v>
-      </c>
-      <c r="F27" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="B28" t="s">
+      <c r="E28" t="s">
+        <v>198</v>
+      </c>
+      <c r="F28" t="s">
         <v>336</v>
       </c>
-      <c r="D28" t="s">
-        <v>337</v>
-      </c>
-      <c r="E28" t="s">
-        <v>200</v>
-      </c>
-      <c r="F28" t="s">
-        <v>338</v>
-      </c>
     </row>
     <row r="29" spans="1:6">
+      <c r="A29">
+        <v>15</v>
+      </c>
       <c r="B29" t="s">
         <v>340</v>
       </c>
@@ -3007,91 +3112,95 @@
         <v>341</v>
       </c>
       <c r="E29" t="s">
+        <v>338</v>
+      </c>
+      <c r="F29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="B30" t="s">
+      <c r="D30" t="s">
+        <v>343</v>
+      </c>
+      <c r="E30" t="s">
+        <v>344</v>
+      </c>
+      <c r="F30" t="s">
         <v>345</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>349</v>
+      </c>
+      <c r="D31" t="s">
         <v>346</v>
       </c>
-      <c r="E30" t="s">
-        <v>343</v>
-      </c>
-      <c r="F30" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>347</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>348</v>
       </c>
-      <c r="E31" t="s">
-        <v>349</v>
-      </c>
-      <c r="F31" t="s">
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>352</v>
+      </c>
+      <c r="D32" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="B32" t="s">
-        <v>354</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>351</v>
-      </c>
-      <c r="E32" t="s">
-        <v>352</v>
       </c>
       <c r="F32" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>15</v>
+      </c>
       <c r="B33" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="D33" t="s">
-        <v>355</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>356</v>
+        <v>63</v>
       </c>
       <c r="F33" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>15</v>
+      </c>
       <c r="B34" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>373</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>374</v>
       </c>
       <c r="F34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" t="s">
-        <v>377</v>
-      </c>
-      <c r="D35" t="s">
-        <v>378</v>
-      </c>
-      <c r="E35" t="s">
-        <v>379</v>
-      </c>
-      <c r="F35" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -3104,7 +3213,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3158,16 +3267,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3175,16 +3284,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
         <v>99</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
         <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3192,16 +3301,16 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
         <v>136</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>137</v>
-      </c>
-      <c r="F5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3209,7 +3318,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="1">
         <v>485165195</v>
@@ -3226,16 +3335,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" t="s">
         <v>184</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>185</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>186</v>
-      </c>
-      <c r="F7" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3243,16 +3352,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
         <v>214</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>215</v>
-      </c>
-      <c r="E8" t="s">
-        <v>216</v>
-      </c>
-      <c r="F8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3260,16 +3369,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E9" t="s">
         <v>229</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>230</v>
-      </c>
-      <c r="E9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F9" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3277,16 +3386,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" t="s">
         <v>243</v>
       </c>
-      <c r="D10" t="s">
-        <v>245</v>
-      </c>
       <c r="E10" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" t="s">
         <v>244</v>
-      </c>
-      <c r="F10" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3294,49 +3403,67 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D11" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" t="s">
         <v>250</v>
       </c>
-      <c r="D11" t="s">
-        <v>247</v>
-      </c>
-      <c r="E11" t="s">
-        <v>248</v>
-      </c>
-      <c r="F11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>251</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>252</v>
       </c>
-      <c r="E12" t="s">
-        <v>253</v>
-      </c>
-      <c r="F12" t="s">
-        <v>254</v>
-      </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="A13">
+        <v>20</v>
+      </c>
       <c r="B13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E13" t="s">
+        <v>326</v>
+      </c>
+      <c r="F13" t="s">
         <v>327</v>
       </c>
-      <c r="D13" t="s">
-        <v>326</v>
-      </c>
-      <c r="E13" t="s">
-        <v>328</v>
-      </c>
-      <c r="F13" t="s">
-        <v>329</v>
-      </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14">
+        <v>20</v>
+      </c>
       <c r="B14" t="s">
-        <v>339</v>
+        <v>337</v>
+      </c>
+      <c r="D14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E14" t="s">
+        <v>380</v>
+      </c>
+      <c r="F14" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New images added and general game impromevements
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="654">
   <si>
     <t>Difficulty</t>
   </si>
@@ -75,9 +75,6 @@
     <t>JP Morgan Chase</t>
   </si>
   <si>
-    <t>Lloid Blankfein</t>
-  </si>
-  <si>
     <t>Merril Linch</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>A zero correlation portfolio optimization method</t>
   </si>
   <si>
-    <t>20mark1</t>
-  </si>
-  <si>
     <t>A 20-Reichsmark gold coin</t>
   </si>
   <si>
@@ -279,12 +273,6 @@
     <t>A British Sovereign</t>
   </si>
   <si>
-    <t>A Tudor 1588 gold coin</t>
-  </si>
-  <si>
-    <t>A French imperial coin</t>
-  </si>
-  <si>
     <t>Which countries formed the Latin Monetary Union?</t>
   </si>
   <si>
@@ -306,9 +294,6 @@
     <t>France</t>
   </si>
   <si>
-    <t>The gold Vrenelli was legal tender in which country?</t>
-  </si>
-  <si>
     <t>According to the euroskeptic Nigel Farage, H. van Rompuy resembles. . .</t>
   </si>
   <si>
@@ -618,9 +603,6 @@
     <t>Napoleon's purchase of former French Lousiana</t>
   </si>
   <si>
-    <t>Which one of these traders was accused of losing €4900 million in 2008?</t>
-  </si>
-  <si>
     <t>Mohamed El-Erian</t>
   </si>
   <si>
@@ -765,12 +747,6 @@
     <t>What is the growth function of the compound interest with fixed rate r?</t>
   </si>
   <si>
-    <t>According to Voltaire, the art of government. . .</t>
-  </si>
-  <si>
-    <t>consists in taking as much money as possible from one party of the citizens to give to the other</t>
-  </si>
-  <si>
     <t>building an efficient bureaucracy</t>
   </si>
   <si>
@@ -804,9 +780,6 @@
     <t>The Spanish Santiago Matamoros design</t>
   </si>
   <si>
-    <t>In 2012, the EU vetoed which €2 coin design?</t>
-  </si>
-  <si>
     <t>Who is the statesman depiced on the $100 notes?</t>
   </si>
   <si>
@@ -942,9 +915,6 @@
     <t>The international speculator was attacking the Dollar</t>
   </si>
   <si>
-    <t>Governments were fearful that the US was financing the Vietnam costs at their expense and demanded hard money</t>
-  </si>
-  <si>
     <t>Why did foreign countries withdraw tons of gold at $35 per ounce at the NY Fed in 1971?</t>
   </si>
   <si>
@@ -957,9 +927,6 @@
     <t>After interrumpting "The House on the Prairie", Nixon pronounced a famous speech in 1971 about. . .</t>
   </si>
   <si>
-    <t>The end of the Bretton Woods Accords because of the Vietnam war</t>
-  </si>
-  <si>
     <t>Closing the New Yok Fed</t>
   </si>
   <si>
@@ -987,9 +954,6 @@
     <t>Expand the monetary supply to purchase hard assets</t>
   </si>
   <si>
-    <t>The closing of the gold window because of the international currency speculator</t>
-  </si>
-  <si>
     <t>Stored subprime gold bars in the prime Bundesbank vault</t>
   </si>
   <si>
@@ -1180,6 +1144,840 @@
   </si>
   <si>
     <t>Which president signed the Executive order 6102</t>
+  </si>
+  <si>
+    <t>A Greek gold coin</t>
+  </si>
+  <si>
+    <t>A French "Napoleon" coin</t>
+  </si>
+  <si>
+    <t>The gold Vreneli was legal tender in which country?</t>
+  </si>
+  <si>
+    <t>vreneli1</t>
+  </si>
+  <si>
+    <t>A Swiss 20 francs gold coin "Vreneli"</t>
+  </si>
+  <si>
+    <t>A French 20 francs gold coin "Napoleon"</t>
+  </si>
+  <si>
+    <t>rooster1</t>
+  </si>
+  <si>
+    <t>A 20 French francs Napoleon "rooster"</t>
+  </si>
+  <si>
+    <t>A French 20 Francs 2nd republic gold coin</t>
+  </si>
+  <si>
+    <t>A French 20 Francs 5th republic gold coin</t>
+  </si>
+  <si>
+    <t>According to Jim Rogers, if a single person were to be blamed for the crisis, it would be. . .</t>
+  </si>
+  <si>
+    <t>Alan Greenspan</t>
+  </si>
+  <si>
+    <t>greenspan1</t>
+  </si>
+  <si>
+    <t>Henry Kissinger</t>
+  </si>
+  <si>
+    <t>volcker1</t>
+  </si>
+  <si>
+    <t>What was LTCM?</t>
+  </si>
+  <si>
+    <t>A hedge fund that collapsed in 1998 and was bailed out by the Fed</t>
+  </si>
+  <si>
+    <t>A hedge fund that caused the 1997 Asian currency collapse</t>
+  </si>
+  <si>
+    <t>The hedge fund that Soros used to break the BoE's currency reserves</t>
+  </si>
+  <si>
+    <t>Who founded LTCM?</t>
+  </si>
+  <si>
+    <t>John Meriwether</t>
+  </si>
+  <si>
+    <t>Nobel Laureate Myron Scholes</t>
+  </si>
+  <si>
+    <t>LTCM bailout is famous for being. . .</t>
+  </si>
+  <si>
+    <t>Russian bankruptcy</t>
+  </si>
+  <si>
+    <t>Myron Scholes and Robert Merton</t>
+  </si>
+  <si>
+    <t>Myron Scholes and Fisher Black</t>
+  </si>
+  <si>
+    <t>Robert Merton and Fisher Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first huge bailout and the one that gave name to the Greenspan's put </t>
+  </si>
+  <si>
+    <t>What is a currency swap?</t>
+  </si>
+  <si>
+    <t>What is the Bank of International Settlements?</t>
+  </si>
+  <si>
+    <t>What is Rentec?</t>
+  </si>
+  <si>
+    <t>What does HSBC stand for?</t>
+  </si>
+  <si>
+    <t>Santander</t>
+  </si>
+  <si>
+    <t>What is the current name of the Abbey Bank in the UK?</t>
+  </si>
+  <si>
+    <t>Abbey Northern Rock</t>
+  </si>
+  <si>
+    <t>BBVA Abbey</t>
+  </si>
+  <si>
+    <t>How does the BIS operate?</t>
+  </si>
+  <si>
+    <t>It is the central bank of central banks</t>
+  </si>
+  <si>
+    <t>It is an international bank focused on large capitalized corporations</t>
+  </si>
+  <si>
+    <t>It is one of the international institutions that extends credit to troubled coutries</t>
+  </si>
+  <si>
+    <t>What is the bid price?</t>
+  </si>
+  <si>
+    <t>What is the ask price?</t>
+  </si>
+  <si>
+    <t>What is the last price in an electronic quote?</t>
+  </si>
+  <si>
+    <t>What does NASDAQ stand for?</t>
+  </si>
+  <si>
+    <t>What is the NASDAQ?</t>
+  </si>
+  <si>
+    <t>In a trading terminal, a level 2 quote contains. . .</t>
+  </si>
+  <si>
+    <t>maple1</t>
+  </si>
+  <si>
+    <t>A 1 Oz. Canadian "Maple"</t>
+  </si>
+  <si>
+    <t>A Canadian 1960 gold coin</t>
+  </si>
+  <si>
+    <t>A 1 Oz. Canadian "Mountie"</t>
+  </si>
+  <si>
+    <t>What is leverage?</t>
+  </si>
+  <si>
+    <t>The first bailout in the 2008 crisis</t>
+  </si>
+  <si>
+    <t>Bearn Stearns' bailout was. . .</t>
+  </si>
+  <si>
+    <t>The first in the 2008 financial crisis</t>
+  </si>
+  <si>
+    <t>Sponsored by the Fed and Merryl Lynch</t>
+  </si>
+  <si>
+    <t>Sponsored by the Treasury and Merryl Lynch</t>
+  </si>
+  <si>
+    <t>In 2008, Bearn Stearns was. . .</t>
+  </si>
+  <si>
+    <t>Bought by JP Morgan Chase with a credit from the Fed at ultra low levels</t>
+  </si>
+  <si>
+    <t>Bought by JP Morgan Chase and Merryl Lynch</t>
+  </si>
+  <si>
+    <t>National Association of Securities Dealers Automated Quotation</t>
+  </si>
+  <si>
+    <t>National Association of Shares Dealers with Automated Quotations</t>
+  </si>
+  <si>
+    <t>National Association of Shares Dealers with Automated Queries</t>
+  </si>
+  <si>
+    <t>What is the IMF?</t>
+  </si>
+  <si>
+    <t>How does the IMF operate?</t>
+  </si>
+  <si>
+    <t>How does the World Bank operate?</t>
+  </si>
+  <si>
+    <t>Bailed out with taxpayer money</t>
+  </si>
+  <si>
+    <t>A Belgian 20 francs LMU gold coin</t>
+  </si>
+  <si>
+    <t>mark1</t>
+  </si>
+  <si>
+    <t>Spanish "Real de a 8" minted in Spain</t>
+  </si>
+  <si>
+    <t>Spanish "Real de a 8" minted in the Phillipines</t>
+  </si>
+  <si>
+    <t>According to the most accepted research, the dollar symbol comes from. . .</t>
+  </si>
+  <si>
+    <t>The snake and stick of the medical profession</t>
+  </si>
+  <si>
+    <t>The German Thaler snake</t>
+  </si>
+  <si>
+    <t>Why did LTCM collapse?</t>
+  </si>
+  <si>
+    <t>taking as much money as possible from one party of the citizens to give to the other</t>
+  </si>
+  <si>
+    <t>According to Voltaire, the art of government consists in. . .</t>
+  </si>
+  <si>
+    <t>Renaissance Technologies: a hedge fund based on Fliud Dynamic equations</t>
+  </si>
+  <si>
+    <t>Renewable Technologies: a hedge fund based on Statistical Arbitrage</t>
+  </si>
+  <si>
+    <t>Renewable Techniques: a hedge fund based on Portfolio Optimization</t>
+  </si>
+  <si>
+    <t>A hedge fund</t>
+  </si>
+  <si>
+    <t>A financial tends research institution</t>
+  </si>
+  <si>
+    <t>What is Gloucester Research?</t>
+  </si>
+  <si>
+    <t>A financial consulting firm</t>
+  </si>
+  <si>
+    <t>Hong Kong Shanghai Banking Corporation</t>
+  </si>
+  <si>
+    <t>Hamilton Schoeneberg Banking Corporation</t>
+  </si>
+  <si>
+    <t>Hong Kong Singapore Banking Corporation</t>
+  </si>
+  <si>
+    <t>Factor Analysis</t>
+  </si>
+  <si>
+    <t>Stochastic Flows</t>
+  </si>
+  <si>
+    <t>PAMR moving average reversal rebalancing</t>
+  </si>
+  <si>
+    <t>kelly1</t>
+  </si>
+  <si>
+    <t>The Kelly criterion for investing</t>
+  </si>
+  <si>
+    <t>A directional betting formula</t>
+  </si>
+  <si>
+    <t>The Shannon criterion for investing</t>
+  </si>
+  <si>
+    <t>Modern Portfolio Theory is due to. . .</t>
+  </si>
+  <si>
+    <t>Harry Markowitz</t>
+  </si>
+  <si>
+    <t>Myron Scholes</t>
+  </si>
+  <si>
+    <t>Edward Thorp</t>
+  </si>
+  <si>
+    <t>Who was the DA prosecuting the case that forced Princeton Newport Partners to liquidate?</t>
+  </si>
+  <si>
+    <t>Rudolph Giuliani</t>
+  </si>
+  <si>
+    <t>Kenneth Starr</t>
+  </si>
+  <si>
+    <t>Eric Holder</t>
+  </si>
+  <si>
+    <t>President Kennedy's Executive Order 11110 allowed the Secretary of the Treasury to. . .</t>
+  </si>
+  <si>
+    <t>Issue as many silver certificates as necessary</t>
+  </si>
+  <si>
+    <t>Recall silver certificates</t>
+  </si>
+  <si>
+    <t>Mint one million American Silver Eagles</t>
+  </si>
+  <si>
+    <t>eagle1</t>
+  </si>
+  <si>
+    <t>An American Silver Eagle</t>
+  </si>
+  <si>
+    <t>A British Silver pound</t>
+  </si>
+  <si>
+    <t>An American half-dollar of 1964</t>
+  </si>
+  <si>
+    <t>to the rest</t>
+  </si>
+  <si>
+    <t>to the rich</t>
+  </si>
+  <si>
+    <t>to the companies</t>
+  </si>
+  <si>
+    <t>According to popular financial sites, gold is flowing from the West. . .</t>
+  </si>
+  <si>
+    <t>It is an electronic market focused on trading shares of technology companies</t>
+  </si>
+  <si>
+    <t>It is an electronic market system</t>
+  </si>
+  <si>
+    <t>It is a an Amercian electronic market focused on start-ups</t>
+  </si>
+  <si>
+    <t>What is the similarity between compound interest with fixed rate and the carbon-14 test?</t>
+  </si>
+  <si>
+    <t>They are described by essentially the same differential equation</t>
+  </si>
+  <si>
+    <t>They grow at the same rate</t>
+  </si>
+  <si>
+    <t>They were characterized in the same research paper</t>
+  </si>
+  <si>
+    <t>The Asian currency crisis consisted of. . .</t>
+  </si>
+  <si>
+    <t>The dollar-pegged Chinese Yuan affected the competitivenes of its neighbors</t>
+  </si>
+  <si>
+    <t>The housing collapse in Japan affected manufacturing in its neighbors</t>
+  </si>
+  <si>
+    <t>Thailand's debt and lack of reserves led to a bath collapse, with an unclear extension to its neighbors</t>
+  </si>
+  <si>
+    <t>Their financial models didn't account for tail events such as the Russian and Asian bankruptcies</t>
+  </si>
+  <si>
+    <t>High leverage on mortgage-backed securities</t>
+  </si>
+  <si>
+    <t>High leverage on Japan's housing market</t>
+  </si>
+  <si>
+    <t>Best bid, best ask, number of buyers and sellers, last traded price and contracts traded</t>
+  </si>
+  <si>
+    <t>Bid, ask and their sizes up to six levels plus the last traded information</t>
+  </si>
+  <si>
+    <t>Technical indicators plus the last trade information</t>
+  </si>
+  <si>
+    <t>What is Fundamental Analysis?</t>
+  </si>
+  <si>
+    <t>What is Technical Analysis?</t>
+  </si>
+  <si>
+    <t>Who was a pioneering mathematical investor?</t>
+  </si>
+  <si>
+    <t>Ed Thorp</t>
+  </si>
+  <si>
+    <t>Blythe Masters</t>
+  </si>
+  <si>
+    <t>Jim Simons</t>
+  </si>
+  <si>
+    <t>George Soros</t>
+  </si>
+  <si>
+    <t>Who is Rentec's founder?</t>
+  </si>
+  <si>
+    <t>Hold possession of physical silver either by buying bullion or taking delivery</t>
+  </si>
+  <si>
+    <t>Hold possession of physical gold either by buying bullion or taking delivery</t>
+  </si>
+  <si>
+    <t>The 2010 campaign by TV host Max Kaiser consisted of. . .</t>
+  </si>
+  <si>
+    <t>Buying up the metals futures market</t>
+  </si>
+  <si>
+    <t>Which bank was the target of the 2010 Max Kaiser's campaign?</t>
+  </si>
+  <si>
+    <t>Scotia Moccata</t>
+  </si>
+  <si>
+    <t>A trader buys cattle futures and forgets to close its position so he has to go and feed the cattle himself</t>
+  </si>
+  <si>
+    <t>Hillary Clinton turned $1,000 into $99,540 trading cattle futures</t>
+  </si>
+  <si>
+    <t>Which story appears in Hull's "Options, Futures and other derivatives" book?</t>
+  </si>
+  <si>
+    <t>Ed Thorp was the first to come up with the Black Scholes formula</t>
+  </si>
+  <si>
+    <t>real1</t>
+  </si>
+  <si>
+    <t>Fanny Mae</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>What is the LBMA?</t>
+  </si>
+  <si>
+    <t>A London-based cartel that sets the gold's price</t>
+  </si>
+  <si>
+    <t>What is a bitcoin?</t>
+  </si>
+  <si>
+    <t>What is the FOMC's Commitments of Traders report?</t>
+  </si>
+  <si>
+    <t>Who is the costodian of the ETF iShares SLV silver vault?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLV doesn'r rely on third parties when it comes to the custody of the metal </t>
+  </si>
+  <si>
+    <t>Which bank is not a CME licensed gold depository?</t>
+  </si>
+  <si>
+    <t>Scotiamocatta</t>
+  </si>
+  <si>
+    <t>What is known as a "quant"?</t>
+  </si>
+  <si>
+    <t>What is an "actuary"?</t>
+  </si>
+  <si>
+    <t>What is the best known mortgage lender after Fannie Mae?</t>
+  </si>
+  <si>
+    <t>Freddie Mac</t>
+  </si>
+  <si>
+    <t>Dodd-Frank Act</t>
+  </si>
+  <si>
+    <t>Glass-Steagal</t>
+  </si>
+  <si>
+    <t>QE</t>
+  </si>
+  <si>
+    <t>It is the best offered price</t>
+  </si>
+  <si>
+    <t>It is the best selling price</t>
+  </si>
+  <si>
+    <t>It is a level II quote field but not a level III field</t>
+  </si>
+  <si>
+    <t>It is the last traded price appearing to the seller</t>
+  </si>
+  <si>
+    <t>It is the price that the seller and buyer of the last operation agreed upon</t>
+  </si>
+  <si>
+    <t>It is the last outstanding selling price</t>
+  </si>
+  <si>
+    <t>It refers to using resources one does not own</t>
+  </si>
+  <si>
+    <t>Using a lever system in the markets</t>
+  </si>
+  <si>
+    <t>Betting large amounts of money</t>
+  </si>
+  <si>
+    <t>Spanish "Real de a 8" minted in Potosi</t>
+  </si>
+  <si>
+    <t>A decentralized virtual currency</t>
+  </si>
+  <si>
+    <t>A world currency replacement for the dollar</t>
+  </si>
+  <si>
+    <t>A coin made of two bits</t>
+  </si>
+  <si>
+    <t>Papandeou</t>
+  </si>
+  <si>
+    <t>papandeou1</t>
+  </si>
+  <si>
+    <t>Papademos</t>
+  </si>
+  <si>
+    <t>lagarde1</t>
+  </si>
+  <si>
+    <t>Christine Lagarde</t>
+  </si>
+  <si>
+    <t>Angela Merkel</t>
+  </si>
+  <si>
+    <t>merkel1</t>
+  </si>
+  <si>
+    <t>rompuy1</t>
+  </si>
+  <si>
+    <t>Herman van Rompuy</t>
+  </si>
+  <si>
+    <t>Neil Farage</t>
+  </si>
+  <si>
+    <t>barroso1</t>
+  </si>
+  <si>
+    <t>Durao-Barroso</t>
+  </si>
+  <si>
+    <t>What is the SEC?</t>
+  </si>
+  <si>
+    <t>What does SEC stand for?</t>
+  </si>
+  <si>
+    <t>Securities and Exchanges Commision</t>
+  </si>
+  <si>
+    <t>What is PIMCO?</t>
+  </si>
+  <si>
+    <t>Who are the two best known partners at PIMCO?</t>
+  </si>
+  <si>
+    <t>Bill Gross and Muhammed El-Erian</t>
+  </si>
+  <si>
+    <t>Jim Rogers and Marc Faber</t>
+  </si>
+  <si>
+    <t>Lawrence Livermore and Nathan Rothschild</t>
+  </si>
+  <si>
+    <t>Who was Lawrence Livermore?</t>
+  </si>
+  <si>
+    <t>In the 80's Ed Thorp employed a portfolio selection method using. . .</t>
+  </si>
+  <si>
+    <t>Which one of these traders was accused of losing 4900 million euro in 2008?</t>
+  </si>
+  <si>
+    <t>The US purchase of Fench Lousiana, in the middle of Napoleon wars</t>
+  </si>
+  <si>
+    <t>In 2012, the EU vetoed which 2 euro coin design?</t>
+  </si>
+  <si>
+    <t>The publication of the names of politicians having bank accounts in Switzerland</t>
+  </si>
+  <si>
+    <t>Bribing government officials to disclose the decision of staying in the euro</t>
+  </si>
+  <si>
+    <t>The publication of a list of tax evading politicians</t>
+  </si>
+  <si>
+    <t>In late 2012, a Greek journalist was arrested over. . .</t>
+  </si>
+  <si>
+    <t>What does LTCM stand for?</t>
+  </si>
+  <si>
+    <t>Long-Term Capital Management</t>
+  </si>
+  <si>
+    <t>Large Trading and Capitalization Market</t>
+  </si>
+  <si>
+    <t>Large Trading and Capitalization Management</t>
+  </si>
+  <si>
+    <t>Which two of these were partners at LTCM?</t>
+  </si>
+  <si>
+    <t>Silver Exchange Corporation</t>
+  </si>
+  <si>
+    <t>Secure Electronic Connections</t>
+  </si>
+  <si>
+    <t>Lawrence Livermore</t>
+  </si>
+  <si>
+    <t>What is the Black Friday?</t>
+  </si>
+  <si>
+    <t>A day with heavy discounts in retail sales</t>
+  </si>
+  <si>
+    <t>A special day for the black community</t>
+  </si>
+  <si>
+    <t>A day in which the Dow Jones dropped 6%</t>
+  </si>
+  <si>
+    <t>Monday October 19, 1987</t>
+  </si>
+  <si>
+    <t>When did the Black Monday happen?</t>
+  </si>
+  <si>
+    <t>Monday October 23, 1929</t>
+  </si>
+  <si>
+    <t>Monday September 27, 2010</t>
+  </si>
+  <si>
+    <t>Who was J.P. Morgan's head of Global Commodities from 2006 to 2012?</t>
+  </si>
+  <si>
+    <t>Emmanuel Derman</t>
+  </si>
+  <si>
+    <t>What is compound interest?</t>
+  </si>
+  <si>
+    <t>Which is not supportive of the temporary existence of compound interest?</t>
+  </si>
+  <si>
+    <t>Inflation</t>
+  </si>
+  <si>
+    <t>What are the BRICs?</t>
+  </si>
+  <si>
+    <t>A group of former emergent countries</t>
+  </si>
+  <si>
+    <t>Credit derivatives</t>
+  </si>
+  <si>
+    <t>A group of investment banks</t>
+  </si>
+  <si>
+    <t>Trust in the currency and cheap energy</t>
+  </si>
+  <si>
+    <t>High interest rates</t>
+  </si>
+  <si>
+    <t>A pyramidal scheme</t>
+  </si>
+  <si>
+    <t>What was the Billionaire Boys Club?</t>
+  </si>
+  <si>
+    <t>A club for high-income individuals</t>
+  </si>
+  <si>
+    <t>A sucressful investment club</t>
+  </si>
+  <si>
+    <t>What is Skull &amp; Bones?</t>
+  </si>
+  <si>
+    <t>skull1</t>
+  </si>
+  <si>
+    <t>Freemasons gather together in. . .</t>
+  </si>
+  <si>
+    <t>Lodges</t>
+  </si>
+  <si>
+    <t>Building sites</t>
+  </si>
+  <si>
+    <t>Hardware stores</t>
+  </si>
+  <si>
+    <t>The closing of the gold window</t>
+  </si>
+  <si>
+    <t>The multilateral end of the Bretton Woods Accords</t>
+  </si>
+  <si>
+    <t>Which was was to blame of the dollar devaluation according to Nixon?</t>
+  </si>
+  <si>
+    <t>The international currency speculator</t>
+  </si>
+  <si>
+    <t>The businessmen</t>
+  </si>
+  <si>
+    <t>The layman</t>
+  </si>
+  <si>
+    <t>Governments were fearful that the US was financing the Vietnam costs at their expense</t>
+  </si>
+  <si>
+    <t>A transgressive rock band</t>
+  </si>
+  <si>
+    <t>A high-seas pirate syndicate</t>
+  </si>
+  <si>
+    <t>A selected group of students</t>
+  </si>
+  <si>
+    <t>Angela Merkel studied in. . .</t>
+  </si>
+  <si>
+    <t>The DDR</t>
+  </si>
+  <si>
+    <t>The BDR</t>
+  </si>
+  <si>
+    <t>Moscow</t>
+  </si>
+  <si>
+    <t>Who was Angela Merkel's mentor?</t>
+  </si>
+  <si>
+    <t>Helmut Kohl</t>
+  </si>
+  <si>
+    <t>Gerhard Schroeder</t>
+  </si>
+  <si>
+    <t>Willy Brandt</t>
+  </si>
+  <si>
+    <t>Who said "I will never trust in paper money"?</t>
+  </si>
+  <si>
+    <t>Napoleon Bonaparte</t>
+  </si>
+  <si>
+    <t>Hjalmar Schacht</t>
+  </si>
+  <si>
+    <t>John Law</t>
+  </si>
+  <si>
+    <t>Dutch tulips</t>
+  </si>
+  <si>
+    <t>French 1st republic assignants</t>
+  </si>
+  <si>
+    <t>The French 1st republic raised funds by. . .</t>
+  </si>
+  <si>
+    <t>Issuing rapidly-inflationary paper money</t>
+  </si>
+  <si>
+    <t>Selling the French Louisiana to the US</t>
+  </si>
+  <si>
+    <t>Taking loans from the Florentian families</t>
+  </si>
+  <si>
+    <t>Who is Durao-Barroso</t>
+  </si>
+  <si>
+    <t>In 2012, the Serbian envoy to NATO Branislav Milinkovic's body was found. . .</t>
+  </si>
+  <si>
+    <t>Crashed on the ground at Brussel's airport in unkown circumstances</t>
+  </si>
+  <si>
+    <t>Exhaust to death because of waiting at Brussel's airport</t>
+  </si>
+  <si>
+    <t>Poisoned at Brussel's airport</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1524,7 +2322,7 @@
     <col min="2" max="2" width="43.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1573,10 +2371,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1590,16 +2388,16 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1607,19 +2405,19 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1627,16 +2425,16 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>173</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1644,16 +2442,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
         <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1664,16 +2462,16 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1684,16 +2482,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1701,16 +2499,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
         <v>54</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>55</v>
-      </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1718,19 +2516,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1741,16 +2539,16 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1758,16 +2556,16 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>74</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1775,16 +2573,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" t="s">
         <v>77</v>
-      </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1792,19 +2590,19 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>377</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1812,16 +2610,16 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1829,16 +2627,16 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1846,16 +2644,16 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1863,19 +2661,19 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1886,16 +2684,16 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1903,16 +2701,16 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1923,16 +2721,16 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1940,16 +2738,16 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D23" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E23" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F23" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1957,16 +2755,16 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D24" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E24" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F24" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1974,16 +2772,16 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E25" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F25" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1991,19 +2789,19 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F26" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2011,16 +2809,16 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E27" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F27" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2028,16 +2826,16 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D28" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E28" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="F28" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2045,16 +2843,16 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2062,16 +2860,16 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D30" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E30" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="F30" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2079,16 +2877,16 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>577</v>
       </c>
       <c r="D31" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="E31" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F31" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2096,16 +2894,16 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E32" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F32" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2113,16 +2911,16 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D33" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E33" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F33" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2130,16 +2928,16 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D34" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E34" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F34" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2147,16 +2945,16 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D35" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="F35" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2164,16 +2962,16 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D36" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E36" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F36" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2181,16 +2979,16 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D37" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E37" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F37" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2198,16 +2996,16 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D38" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E38" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F38" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2215,16 +3013,16 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D39" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="E39" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F39" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2232,16 +3030,16 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D40" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E40" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F40" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2249,16 +3047,16 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="D41" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E41" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F41" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2266,16 +3064,16 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D42" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E42" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="F42" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2283,16 +3081,16 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D43" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="E43" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="F43" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2300,16 +3098,16 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="D44" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="E44" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="F44" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2317,16 +3115,16 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D45" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="E45" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="F45" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2334,16 +3132,16 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D46" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E46" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="F46" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2351,16 +3149,16 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D47" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E47" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="F47" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2368,19 +3166,19 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C48" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D48" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="E48" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="F48" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2388,16 +3186,16 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D49" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="E49" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F49" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2405,16 +3203,16 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D50" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="E50" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F50" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2422,16 +3220,16 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="D51" t="s">
-        <v>308</v>
+        <v>627</v>
       </c>
       <c r="E51" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="F51" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2439,16 +3237,16 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="D52" t="s">
-        <v>323</v>
+        <v>621</v>
       </c>
       <c r="E52" t="s">
-        <v>313</v>
+        <v>622</v>
       </c>
       <c r="F52" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2456,16 +3254,16 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="D53" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="E53" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F53" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2473,16 +3271,16 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D54" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="E54" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F54" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2490,16 +3288,16 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="D55" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="E55" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="F55" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2507,16 +3305,16 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="D56" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="E56" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="F56" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2524,16 +3322,16 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="D57" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="E57" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="F57" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2541,16 +3339,16 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="D58" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="E58" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="F58" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2558,16 +3356,16 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="D59" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="E59" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="F59" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2575,16 +3373,775 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="D60" t="s">
+        <v>373</v>
+      </c>
+      <c r="E60" t="s">
+        <v>365</v>
+      </c>
+      <c r="F60" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" t="s">
+        <v>382</v>
+      </c>
+      <c r="D61" t="s">
+        <v>383</v>
+      </c>
+      <c r="E61" t="s">
+        <v>384</v>
+      </c>
+      <c r="F61" t="s">
         <v>385</v>
       </c>
-      <c r="E60" t="s">
-        <v>377</v>
-      </c>
-      <c r="F60" t="s">
-        <v>378</v>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>388</v>
+      </c>
+      <c r="D62" t="s">
+        <v>387</v>
+      </c>
+      <c r="E62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>391</v>
+      </c>
+      <c r="D63" t="s">
+        <v>392</v>
+      </c>
+      <c r="E63" t="s">
+        <v>393</v>
+      </c>
+      <c r="F63" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
+        <v>395</v>
+      </c>
+      <c r="D64" t="s">
+        <v>396</v>
+      </c>
+      <c r="E64" t="s">
+        <v>134</v>
+      </c>
+      <c r="F64" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>398</v>
+      </c>
+      <c r="D65" t="s">
+        <v>403</v>
+      </c>
+      <c r="F65" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>416</v>
+      </c>
+      <c r="D66" t="s">
+        <v>542</v>
+      </c>
+      <c r="E66" t="s">
+        <v>544</v>
+      </c>
+      <c r="F66" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>417</v>
+      </c>
+      <c r="D67" t="s">
+        <v>543</v>
+      </c>
+      <c r="E67" t="s">
+        <v>545</v>
+      </c>
+      <c r="F67" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>418</v>
+      </c>
+      <c r="D68" t="s">
+        <v>546</v>
+      </c>
+      <c r="E68" t="s">
+        <v>547</v>
+      </c>
+      <c r="F68" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>420</v>
+      </c>
+      <c r="D69" t="s">
+        <v>489</v>
+      </c>
+      <c r="E69" t="s">
+        <v>490</v>
+      </c>
+      <c r="F69" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" t="s">
+        <v>422</v>
+      </c>
+      <c r="D70" t="s">
+        <v>423</v>
+      </c>
+      <c r="E70" t="s">
+        <v>424</v>
+      </c>
+      <c r="F70" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>426</v>
+      </c>
+      <c r="D71" t="s">
+        <v>548</v>
+      </c>
+      <c r="E71" t="s">
+        <v>549</v>
+      </c>
+      <c r="F71" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>428</v>
+      </c>
+      <c r="D72" t="s">
+        <v>429</v>
+      </c>
+      <c r="E72" t="s">
+        <v>430</v>
+      </c>
+      <c r="F72" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>10</v>
+      </c>
+      <c r="B73" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <v>10</v>
+      </c>
+      <c r="B74" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" t="s">
+        <v>481</v>
+      </c>
+      <c r="D74" t="s">
+        <v>482</v>
+      </c>
+      <c r="E74" t="s">
+        <v>483</v>
+      </c>
+      <c r="F74" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <v>10</v>
+      </c>
+      <c r="B75" t="s">
+        <v>488</v>
+      </c>
+      <c r="D75" t="s">
+        <v>485</v>
+      </c>
+      <c r="E75" t="s">
+        <v>486</v>
+      </c>
+      <c r="F75" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>10</v>
+      </c>
+      <c r="B76" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>10</v>
+      </c>
+      <c r="B77" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>10</v>
+      </c>
+      <c r="B78" t="s">
+        <v>516</v>
+      </c>
+      <c r="D78" t="s">
+        <v>514</v>
+      </c>
+      <c r="E78" t="s">
+        <v>515</v>
+      </c>
+      <c r="F78" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79">
+        <v>10</v>
+      </c>
+      <c r="B79" t="s">
+        <v>518</v>
+      </c>
+      <c r="D79" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" t="s">
+        <v>519</v>
+      </c>
+      <c r="F79" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80">
+        <v>10</v>
+      </c>
+      <c r="B80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D80" t="s">
+        <v>509</v>
+      </c>
+      <c r="E80" t="s">
+        <v>510</v>
+      </c>
+      <c r="F80" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>10</v>
+      </c>
+      <c r="B82" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>10</v>
+      </c>
+      <c r="B83" t="s">
+        <v>527</v>
+      </c>
+      <c r="D83" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <v>10</v>
+      </c>
+      <c r="B84" t="s">
+        <v>533</v>
+      </c>
+      <c r="D84" t="s">
+        <v>17</v>
+      </c>
+      <c r="E84" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85">
+        <v>10</v>
+      </c>
+      <c r="B85" t="s">
+        <v>529</v>
+      </c>
+      <c r="D85" t="s">
+        <v>552</v>
+      </c>
+      <c r="E85" t="s">
+        <v>553</v>
+      </c>
+      <c r="F85" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86">
+        <v>10</v>
+      </c>
+      <c r="B86" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s">
+        <v>531</v>
+      </c>
+      <c r="D87" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88">
+        <v>10</v>
+      </c>
+      <c r="B88" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89">
+        <v>10</v>
+      </c>
+      <c r="B89" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90">
+        <v>10</v>
+      </c>
+      <c r="B90" t="s">
+        <v>537</v>
+      </c>
+      <c r="D90" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>10</v>
+      </c>
+      <c r="B91" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>10</v>
+      </c>
+      <c r="B92" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <v>10</v>
+      </c>
+      <c r="B93" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>10</v>
+      </c>
+      <c r="B94" t="s">
+        <v>571</v>
+      </c>
+      <c r="D94" t="s">
+        <v>572</v>
+      </c>
+      <c r="E94" t="s">
+        <v>573</v>
+      </c>
+      <c r="F94" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>10</v>
+      </c>
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>556</v>
+      </c>
+      <c r="D95" t="s">
+        <v>555</v>
+      </c>
+      <c r="E95" t="s">
+        <v>557</v>
+      </c>
+      <c r="F95" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>10</v>
+      </c>
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>565</v>
+      </c>
+      <c r="D96" t="s">
+        <v>566</v>
+      </c>
+      <c r="E96" t="s">
+        <v>557</v>
+      </c>
+      <c r="F96" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>10</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>561</v>
+      </c>
+      <c r="D97" t="s">
+        <v>560</v>
+      </c>
+      <c r="E97" t="s">
+        <v>510</v>
+      </c>
+      <c r="F97" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>10</v>
+      </c>
+      <c r="B98" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>10</v>
+      </c>
+      <c r="B99" t="s">
+        <v>568</v>
+      </c>
+      <c r="D99" t="s">
+        <v>569</v>
+      </c>
+      <c r="E99" t="s">
+        <v>589</v>
+      </c>
+      <c r="F99" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>10</v>
+      </c>
+      <c r="B100" t="s">
+        <v>584</v>
+      </c>
+      <c r="D100" t="s">
+        <v>585</v>
+      </c>
+      <c r="E100" t="s">
+        <v>586</v>
+      </c>
+      <c r="F100" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>10</v>
+      </c>
+      <c r="B101" t="s">
+        <v>592</v>
+      </c>
+      <c r="D101" t="s">
+        <v>593</v>
+      </c>
+      <c r="E101" t="s">
+        <v>594</v>
+      </c>
+      <c r="F101" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>10</v>
+      </c>
+      <c r="B102" t="s">
+        <v>597</v>
+      </c>
+      <c r="D102" t="s">
+        <v>596</v>
+      </c>
+      <c r="E102" t="s">
+        <v>598</v>
+      </c>
+      <c r="F102" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>10</v>
+      </c>
+      <c r="B103" t="s">
+        <v>605</v>
+      </c>
+      <c r="D103" t="s">
+        <v>606</v>
+      </c>
+      <c r="E103" t="s">
+        <v>607</v>
+      </c>
+      <c r="F103" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="B104" t="s">
+        <v>612</v>
+      </c>
+      <c r="D104" t="s">
+        <v>611</v>
+      </c>
+      <c r="E104" t="s">
+        <v>613</v>
+      </c>
+      <c r="F104" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="B105" t="s">
+        <v>615</v>
+      </c>
+      <c r="C105" t="s">
+        <v>616</v>
+      </c>
+      <c r="D105" t="s">
+        <v>630</v>
+      </c>
+      <c r="E105" t="s">
+        <v>628</v>
+      </c>
+      <c r="F105" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="B106" t="s">
+        <v>617</v>
+      </c>
+      <c r="D106" t="s">
+        <v>618</v>
+      </c>
+      <c r="E106" t="s">
+        <v>619</v>
+      </c>
+      <c r="F106" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="B107" t="s">
+        <v>623</v>
+      </c>
+      <c r="D107" t="s">
+        <v>624</v>
+      </c>
+      <c r="E107" t="s">
+        <v>625</v>
+      </c>
+      <c r="F107" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="B108" t="s">
+        <v>635</v>
+      </c>
+      <c r="D108" t="s">
+        <v>636</v>
+      </c>
+      <c r="E108" t="s">
+        <v>637</v>
+      </c>
+      <c r="F108" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="B109" t="s">
+        <v>639</v>
+      </c>
+      <c r="D109" t="s">
+        <v>640</v>
+      </c>
+      <c r="E109" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="B110" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="B111" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="B112" t="s">
+        <v>645</v>
+      </c>
+      <c r="D112" t="s">
+        <v>646</v>
+      </c>
+      <c r="E112" t="s">
+        <v>648</v>
+      </c>
+      <c r="F112" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6">
+      <c r="B113" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="B114" t="s">
+        <v>650</v>
+      </c>
+      <c r="D114" t="s">
+        <v>651</v>
+      </c>
+      <c r="E114" t="s">
+        <v>652</v>
+      </c>
+      <c r="F114" t="s">
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -2594,10 +4151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2644,7 +4201,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2664,7 +4221,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2675,16 +4232,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2692,19 +4249,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
+        <v>443</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2712,16 +4269,16 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
       <c r="F6" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2729,7 +4286,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -2738,7 +4295,7 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2752,10 +4309,10 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -2766,16 +4323,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2783,16 +4340,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
         <v>70</v>
-      </c>
-      <c r="F10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2800,16 +4357,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s">
         <v>80</v>
-      </c>
-      <c r="D11" t="s">
-        <v>278</v>
-      </c>
-      <c r="E11" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2817,16 +4374,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2834,16 +4391,16 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>378</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2851,16 +4408,16 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2868,16 +4425,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2885,16 +4442,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2902,16 +4459,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F17" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2919,16 +4476,16 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F18" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2936,16 +4493,16 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F19" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2953,16 +4510,16 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2970,16 +4527,16 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2987,16 +4544,16 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D22" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3004,16 +4561,16 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F23" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3021,16 +4578,16 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>198</v>
+        <v>578</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3038,16 +4595,16 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>262</v>
+        <v>579</v>
       </c>
       <c r="D25" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="E25" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="F25" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3055,16 +4612,16 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="E26" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="F26" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3072,16 +4629,16 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="D27" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="E27" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="F27" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3089,16 +4646,16 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="D28" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F28" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3106,16 +4663,16 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="D29" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="E29" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="F29" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3123,16 +4680,16 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="D30" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="E30" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="F30" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3140,16 +4697,16 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="D31" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="E31" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="F31" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3157,16 +4714,16 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="D32" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="E32" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F32" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3174,16 +4731,16 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F33" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3191,16 +4748,416 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="D34" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="E34" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="F34" t="s">
-        <v>375</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>379</v>
+      </c>
+      <c r="D35" t="s">
+        <v>380</v>
+      </c>
+      <c r="E35" t="s">
+        <v>381</v>
+      </c>
+      <c r="F35" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>386</v>
+      </c>
+      <c r="D36" t="s">
+        <v>387</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>390</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>387</v>
+      </c>
+      <c r="F37" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>496</v>
+      </c>
+      <c r="D38" t="s">
+        <v>499</v>
+      </c>
+      <c r="E38" t="s">
+        <v>497</v>
+      </c>
+      <c r="F38" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>409</v>
+      </c>
+      <c r="D40" t="s">
+        <v>408</v>
+      </c>
+      <c r="E40" t="s">
+        <v>410</v>
+      </c>
+      <c r="F40" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>405</v>
+      </c>
+      <c r="D41" t="s">
+        <v>413</v>
+      </c>
+      <c r="E41" t="s">
+        <v>414</v>
+      </c>
+      <c r="F41" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>419</v>
+      </c>
+      <c r="D42" t="s">
+        <v>435</v>
+      </c>
+      <c r="E42" t="s">
+        <v>436</v>
+      </c>
+      <c r="F42" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>421</v>
+      </c>
+      <c r="D43" t="s">
+        <v>503</v>
+      </c>
+      <c r="E43" t="s">
+        <v>504</v>
+      </c>
+      <c r="F43" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>432</v>
+      </c>
+      <c r="D44" t="s">
+        <v>433</v>
+      </c>
+      <c r="E44" t="s">
+        <v>441</v>
+      </c>
+      <c r="F44" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>524</v>
+      </c>
+      <c r="D47" t="s">
+        <v>551</v>
+      </c>
+      <c r="E47" t="s">
+        <v>444</v>
+      </c>
+      <c r="F47" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48" t="s">
+        <v>446</v>
+      </c>
+      <c r="D48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" t="s">
+        <v>447</v>
+      </c>
+      <c r="F48" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>15</v>
+      </c>
+      <c r="B49" t="s">
+        <v>469</v>
+      </c>
+      <c r="D49" t="s">
+        <v>470</v>
+      </c>
+      <c r="E49" t="s">
+        <v>471</v>
+      </c>
+      <c r="F49" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>15</v>
+      </c>
+      <c r="B50" t="s">
+        <v>477</v>
+      </c>
+      <c r="D50" t="s">
+        <v>478</v>
+      </c>
+      <c r="E50" t="s">
+        <v>479</v>
+      </c>
+      <c r="F50" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>522</v>
+      </c>
+      <c r="D51" t="s">
+        <v>520</v>
+      </c>
+      <c r="E51" t="s">
+        <v>521</v>
+      </c>
+      <c r="F51" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>513</v>
+      </c>
+      <c r="D52" t="s">
+        <v>511</v>
+      </c>
+      <c r="E52" t="s">
+        <v>509</v>
+      </c>
+      <c r="F52" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>15</v>
+      </c>
+      <c r="B53" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>558</v>
+      </c>
+      <c r="D54" t="s">
+        <v>559</v>
+      </c>
+      <c r="E54" t="s">
+        <v>510</v>
+      </c>
+      <c r="F54" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>15</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>562</v>
+      </c>
+      <c r="D55" t="s">
+        <v>563</v>
+      </c>
+      <c r="E55" t="s">
+        <v>564</v>
+      </c>
+      <c r="F55" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>583</v>
+      </c>
+      <c r="D56" t="s">
+        <v>580</v>
+      </c>
+      <c r="E56" t="s">
+        <v>581</v>
+      </c>
+      <c r="F56" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>603</v>
+      </c>
+      <c r="D58" t="s">
+        <v>610</v>
+      </c>
+      <c r="E58" t="s">
+        <v>604</v>
+      </c>
+      <c r="F58" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>15</v>
+      </c>
+      <c r="B59" t="s">
+        <v>631</v>
+      </c>
+      <c r="D59" t="s">
+        <v>632</v>
+      </c>
+      <c r="E59" t="s">
+        <v>633</v>
+      </c>
+      <c r="F59" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="B60" t="s">
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -3210,16 +5167,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="63.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="5" width="31.85546875" customWidth="1"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
@@ -3250,16 +5208,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3267,16 +5225,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3284,16 +5242,16 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3301,16 +5259,16 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3318,7 +5276,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1">
         <v>485165195</v>
@@ -3335,16 +5293,16 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3352,16 +5310,16 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F8" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3369,16 +5327,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E9" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F9" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3386,16 +5344,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D10" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E10" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3403,16 +5361,16 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E11" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3420,16 +5378,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>451</v>
       </c>
       <c r="D12" t="s">
-        <v>250</v>
+        <v>450</v>
       </c>
       <c r="E12" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3437,16 +5395,16 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="D13" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="E13" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="F13" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3454,16 +5412,213 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D14" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="E14" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="F14" t="s">
-        <v>381</v>
+        <v>369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>406</v>
+      </c>
+      <c r="D17" t="s">
+        <v>452</v>
+      </c>
+      <c r="E17" t="s">
+        <v>453</v>
+      </c>
+      <c r="F17" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>457</v>
+      </c>
+      <c r="D18" t="s">
+        <v>455</v>
+      </c>
+      <c r="E18" t="s">
+        <v>456</v>
+      </c>
+      <c r="F18" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>407</v>
+      </c>
+      <c r="D19" t="s">
+        <v>459</v>
+      </c>
+      <c r="E19" t="s">
+        <v>460</v>
+      </c>
+      <c r="F19" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>449</v>
+      </c>
+      <c r="D20" t="s">
+        <v>500</v>
+      </c>
+      <c r="E20" t="s">
+        <v>501</v>
+      </c>
+      <c r="F20" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>588</v>
+      </c>
+      <c r="D21" t="s">
+        <v>400</v>
+      </c>
+      <c r="E21" t="s">
+        <v>401</v>
+      </c>
+      <c r="F21" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>576</v>
+      </c>
+      <c r="D22" t="s">
+        <v>462</v>
+      </c>
+      <c r="E22" t="s">
+        <v>463</v>
+      </c>
+      <c r="F22" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>465</v>
+      </c>
+      <c r="D23" t="s">
+        <v>466</v>
+      </c>
+      <c r="E23" t="s">
+        <v>467</v>
+      </c>
+      <c r="F23" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>473</v>
+      </c>
+      <c r="D24" t="s">
+        <v>474</v>
+      </c>
+      <c r="E24" t="s">
+        <v>475</v>
+      </c>
+      <c r="F24" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>492</v>
+      </c>
+      <c r="D25" t="s">
+        <v>493</v>
+      </c>
+      <c r="E25" t="s">
+        <v>494</v>
+      </c>
+      <c r="F25" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>600</v>
+      </c>
+      <c r="D27" t="s">
+        <v>510</v>
+      </c>
+      <c r="E27" t="s">
+        <v>511</v>
+      </c>
+      <c r="F27" t="s">
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Flash round and made some minor modifications.
More questions added.
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="818">
   <si>
     <t>Difficulty</t>
   </si>
@@ -684,9 +684,6 @@
     <t>What important work did Mayer Amschel Rothschild do for Wilhelm IX, Landgrave of Hesse-Kassel?</t>
   </si>
   <si>
-    <t>He handled paymends from renting males from or passing through Hesse as soldiers, including the American indpendence war</t>
-  </si>
-  <si>
     <t>He provided him with useful tips in the Paris stock market</t>
   </si>
   <si>
@@ -1215,9 +1212,6 @@
     <t>LTCM bailout is famous for being. . .</t>
   </si>
   <si>
-    <t>Russian bankruptcy</t>
-  </si>
-  <si>
     <t>Myron Scholes and Robert Merton</t>
   </si>
   <si>
@@ -1338,9 +1332,6 @@
     <t>How does the IMF operate?</t>
   </si>
   <si>
-    <t>How does the World Bank operate?</t>
-  </si>
-  <si>
     <t>Bailed out with taxpayer money</t>
   </si>
   <si>
@@ -1374,15 +1365,6 @@
     <t>According to Voltaire, the art of government consists in. . .</t>
   </si>
   <si>
-    <t>Renaissance Technologies: a hedge fund based on Fliud Dynamic equations</t>
-  </si>
-  <si>
-    <t>Renewable Technologies: a hedge fund based on Statistical Arbitrage</t>
-  </si>
-  <si>
-    <t>Renewable Techniques: a hedge fund based on Portfolio Optimization</t>
-  </si>
-  <si>
     <t>A hedge fund</t>
   </si>
   <si>
@@ -1593,9 +1575,6 @@
     <t>real1</t>
   </si>
   <si>
-    <t>Fanny Mae</t>
-  </si>
-  <si>
     <t>AIG</t>
   </si>
   <si>
@@ -1635,15 +1614,6 @@
     <t>Freddie Mac</t>
   </si>
   <si>
-    <t>Dodd-Frank Act</t>
-  </si>
-  <si>
-    <t>Glass-Steagal</t>
-  </si>
-  <si>
-    <t>QE</t>
-  </si>
-  <si>
     <t>It is the best offered price</t>
   </si>
   <si>
@@ -1947,12 +1917,6 @@
     <t>John Law</t>
   </si>
   <si>
-    <t>Dutch tulips</t>
-  </si>
-  <si>
-    <t>French 1st republic assignants</t>
-  </si>
-  <si>
     <t>The French 1st republic raised funds by. . .</t>
   </si>
   <si>
@@ -1965,9 +1929,6 @@
     <t>Taking loans from the Florentian families</t>
   </si>
   <si>
-    <t>Who is Durao-Barroso</t>
-  </si>
-  <si>
     <t>In 2012, the Serbian envoy to NATO Branislav Milinkovic's body was found. . .</t>
   </si>
   <si>
@@ -1978,6 +1939,537 @@
   </si>
   <si>
     <t>Poisoned at Brussel's airport</t>
+  </si>
+  <si>
+    <t>Henry Ford</t>
+  </si>
+  <si>
+    <t>Nathan Mayer Rothschild</t>
+  </si>
+  <si>
+    <t>J. Rockefeller</t>
+  </si>
+  <si>
+    <t>Who said the following quote "It is well enough that people of the nation do not understand our banking and monetary system, for if they did, I believe there would be a revolution before tomorrow morning"</t>
+  </si>
+  <si>
+    <t>What is AIG?</t>
+  </si>
+  <si>
+    <t>An insurance broker</t>
+  </si>
+  <si>
+    <t>American Insurance Group</t>
+  </si>
+  <si>
+    <t>A bank</t>
+  </si>
+  <si>
+    <t>Dutch tulips are an example of. . .</t>
+  </si>
+  <si>
+    <t>A financial bubble</t>
+  </si>
+  <si>
+    <t>Beauty</t>
+  </si>
+  <si>
+    <t>Stock trading</t>
+  </si>
+  <si>
+    <t>A beloved silver coin in Fance is. . .</t>
+  </si>
+  <si>
+    <t>The Hercules</t>
+  </si>
+  <si>
+    <t>The Alfonsina</t>
+  </si>
+  <si>
+    <t>20 Euro</t>
+  </si>
+  <si>
+    <t>Renaissance Technologies</t>
+  </si>
+  <si>
+    <t>Renewable Technologies</t>
+  </si>
+  <si>
+    <t>Renowned Technicians</t>
+  </si>
+  <si>
+    <t>Who is credited for creating the infamous Credit Default Swaps?</t>
+  </si>
+  <si>
+    <t>Paul Wilmott</t>
+  </si>
+  <si>
+    <t>Chardinal Richelieu's economic policy was named. . .</t>
+  </si>
+  <si>
+    <t>Merchantilism</t>
+  </si>
+  <si>
+    <t>Richelenian</t>
+  </si>
+  <si>
+    <t>Capitalism</t>
+  </si>
+  <si>
+    <t>What is Merchantilism?</t>
+  </si>
+  <si>
+    <t>Importing less that exporting</t>
+  </si>
+  <si>
+    <t>Remove taxes to trading</t>
+  </si>
+  <si>
+    <t>Remove taxes to production</t>
+  </si>
+  <si>
+    <t>Ron Paul promotes. . .</t>
+  </si>
+  <si>
+    <t>Libertarism</t>
+  </si>
+  <si>
+    <t>Socialism</t>
+  </si>
+  <si>
+    <t>What is liberalism?</t>
+  </si>
+  <si>
+    <t>In a liberal system, if a bank fails, it. . .</t>
+  </si>
+  <si>
+    <t>Files for bankrupt</t>
+  </si>
+  <si>
+    <t>Is bailed-out by the government</t>
+  </si>
+  <si>
+    <t>Receives an assistance package from its central bank</t>
+  </si>
+  <si>
+    <t>Those who steal rule</t>
+  </si>
+  <si>
+    <t>Those who vote rule</t>
+  </si>
+  <si>
+    <t>A cleptocracy is a system in which. . .</t>
+  </si>
+  <si>
+    <t>One can vote his/her own laws directly</t>
+  </si>
+  <si>
+    <t>Santander and BBVA are two large banks from. . .</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>As of the end of 2012, what percentage of the newly-issued debt would be bought by the Fed?</t>
+  </si>
+  <si>
+    <t>What is socialism?</t>
+  </si>
+  <si>
+    <t>What is comunism?</t>
+  </si>
+  <si>
+    <t>As budget-cutting politicians in the European institutions</t>
+  </si>
+  <si>
+    <t>In Western Europe, the students who organized the pro-rights revolts in Spring '68 ended up. . .</t>
+  </si>
+  <si>
+    <t>As bankers</t>
+  </si>
+  <si>
+    <t>As expensive hippie clothing manufacturers</t>
+  </si>
+  <si>
+    <t>What is capitalism?</t>
+  </si>
+  <si>
+    <t>Who is Emilio Botin?</t>
+  </si>
+  <si>
+    <t>Head of Santander and of the Botin family</t>
+  </si>
+  <si>
+    <t>Head of the Botin Bank</t>
+  </si>
+  <si>
+    <t>Head of BBVA and the Botin Family</t>
+  </si>
+  <si>
+    <t>In his famous Speech, Kennedy was opposed to. . .</t>
+  </si>
+  <si>
+    <t>Secret societies</t>
+  </si>
+  <si>
+    <t>Banking excesses</t>
+  </si>
+  <si>
+    <t>Excessive monetary expansion</t>
+  </si>
+  <si>
+    <t>The Brithish Northern Rock collapsed in. . .</t>
+  </si>
+  <si>
+    <t>British Northern Rock</t>
+  </si>
+  <si>
+    <t>French Societé Generale</t>
+  </si>
+  <si>
+    <t>American Goldman Sachs</t>
+  </si>
+  <si>
+    <t>The subprime crisis severily affected. . .</t>
+  </si>
+  <si>
+    <t>He handled payments from renting males from or passing through Hesse as soldiers</t>
+  </si>
+  <si>
+    <t>After the communism, Russia underwent a financial crisis in the year. . .</t>
+  </si>
+  <si>
+    <t>The IMF was created. . .</t>
+  </si>
+  <si>
+    <t>At the Bretton Woods conference</t>
+  </si>
+  <si>
+    <t>In 1949</t>
+  </si>
+  <si>
+    <t>In 1951</t>
+  </si>
+  <si>
+    <t>Countries contribute money to a pool from which countries with imbalances temporarily borrow</t>
+  </si>
+  <si>
+    <t>Banks contribute money to a pool from which countries with imbalances temporarily borrow</t>
+  </si>
+  <si>
+    <t>Banks contribute money to a pool from which banks with imbalances temporarily borrow</t>
+  </si>
+  <si>
+    <t>Which one is a main point in the Dodd-Frank Act?</t>
+  </si>
+  <si>
+    <t>Closing the OTC market</t>
+  </si>
+  <si>
+    <t>Separation between investment and commercial banking</t>
+  </si>
+  <si>
+    <t>Elimination of regulations</t>
+  </si>
+  <si>
+    <t>Bringing opaque products to open exchanges</t>
+  </si>
+  <si>
+    <t>Which one is a main point in the Glass-Steagal Act?</t>
+  </si>
+  <si>
+    <t>Extension of the FDIC</t>
+  </si>
+  <si>
+    <t>What does QE stand for?</t>
+  </si>
+  <si>
+    <t>Quantitative Easing</t>
+  </si>
+  <si>
+    <t>Quantitative Economics</t>
+  </si>
+  <si>
+    <t>Quadratic Extension</t>
+  </si>
+  <si>
+    <t>The largest active global fixed income managers in the world</t>
+  </si>
+  <si>
+    <t>A Japanese morgage brokerage</t>
+  </si>
+  <si>
+    <t>An agency that regulates and enforces federal laws in the securities industry</t>
+  </si>
+  <si>
+    <t>An exchange</t>
+  </si>
+  <si>
+    <t>International Monetary Fund</t>
+  </si>
+  <si>
+    <t>International Market Funding</t>
+  </si>
+  <si>
+    <t>International Money Forwarders</t>
+  </si>
+  <si>
+    <t>An Italian ex Goldman Sachs who served as Italian PM for over 1 year</t>
+  </si>
+  <si>
+    <t>The Italian ex Goldman Sachs who served as ECB's president</t>
+  </si>
+  <si>
+    <t>The president of the Italian Plumbing Company (IPC)</t>
+  </si>
+  <si>
+    <t>Who is Mario Monti?</t>
+  </si>
+  <si>
+    <t>Spanish financial problems come from. . .</t>
+  </si>
+  <si>
+    <t>A 13-year long housing bubble</t>
+  </si>
+  <si>
+    <t>A weak financial system</t>
+  </si>
+  <si>
+    <t>Constantly forgiving debt to other countries</t>
+  </si>
+  <si>
+    <t>Forecasting the direction of prices through the study of past market data</t>
+  </si>
+  <si>
+    <t>Quantitative management of portfolio</t>
+  </si>
+  <si>
+    <t>Forecasting the direction of prices based on a company's circumstances and macroeconomic variables</t>
+  </si>
+  <si>
+    <t>Forecasting the direction of prices based on mathematical techniques</t>
+  </si>
+  <si>
+    <t>Amalysis of the conformity of a bank books to the applicable law</t>
+  </si>
+  <si>
+    <t>What is Fanny Mae?</t>
+  </si>
+  <si>
+    <t>A mortgate brokerage</t>
+  </si>
+  <si>
+    <t>A Latin-American commerce association</t>
+  </si>
+  <si>
+    <t>A Libanese trading post</t>
+  </si>
+  <si>
+    <t>In most countries, the retirement funds are, by definition. . .</t>
+  </si>
+  <si>
+    <t>A robust scheme</t>
+  </si>
+  <si>
+    <t>An investment</t>
+  </si>
+  <si>
+    <t>What was the currency in Italy before the euro?</t>
+  </si>
+  <si>
+    <t>The lira</t>
+  </si>
+  <si>
+    <t>The Italian pound</t>
+  </si>
+  <si>
+    <t>The Italian franc</t>
+  </si>
+  <si>
+    <t>What was the currency in France before the euro?</t>
+  </si>
+  <si>
+    <t>The French franc</t>
+  </si>
+  <si>
+    <t>The French pound</t>
+  </si>
+  <si>
+    <t>The French mark</t>
+  </si>
+  <si>
+    <t>What was the currency in the Rep. of Ireland before the euro?</t>
+  </si>
+  <si>
+    <t>The Irish pound</t>
+  </si>
+  <si>
+    <t>The Irish dollar</t>
+  </si>
+  <si>
+    <t>The morrigan</t>
+  </si>
+  <si>
+    <t>Irish financial problems come from. . .</t>
+  </si>
+  <si>
+    <t>A housing bubble</t>
+  </si>
+  <si>
+    <t>An overextended financial system</t>
+  </si>
+  <si>
+    <t>Lack of industrial activity</t>
+  </si>
+  <si>
+    <t>After the credit froze in 2008 and the unemployment soared, the 2012 Spanish housing market fell. . .</t>
+  </si>
+  <si>
+    <t>An enumeration of the holdings of participants in various futures markets</t>
+  </si>
+  <si>
+    <t>The list of participants in the major US markets</t>
+  </si>
+  <si>
+    <t>The list of participants in all the US markets</t>
+  </si>
+  <si>
+    <t>A business professional who deals with the financial impact of risk and uncertainty</t>
+  </si>
+  <si>
+    <t>A financial professional who evaluates current economic events</t>
+  </si>
+  <si>
+    <t>A financial professional who makes derivatives</t>
+  </si>
+  <si>
+    <t>A form of government in which the State heavily intervenes the economy</t>
+  </si>
+  <si>
+    <t>A form of government in which the State owns almost everything and plans every aspect of the economy</t>
+  </si>
+  <si>
+    <t>A form of government in which the State provides everything for free</t>
+  </si>
+  <si>
+    <t>A form of government in which the State subsidizes everything</t>
+  </si>
+  <si>
+    <t>What is keynesianism?</t>
+  </si>
+  <si>
+    <t>An economic system based on private ownership of the means of production and selling the production for profit</t>
+  </si>
+  <si>
+    <t>An economic system in which the rich always accumulates wealth</t>
+  </si>
+  <si>
+    <t>A form of government in which the State subsidizes nothing</t>
+  </si>
+  <si>
+    <t>A political philosophy supporting civil and individual rights, freedom of the press, of religion, trade</t>
+  </si>
+  <si>
+    <t>How may grams is a troy ounce?</t>
+  </si>
+  <si>
+    <t>A financial professional that employs advanced mathematical techniques to profit from the market</t>
+  </si>
+  <si>
+    <t>A quantitative trading strategy</t>
+  </si>
+  <si>
+    <t>A technical analyst</t>
+  </si>
+  <si>
+    <t>Wells Fargo</t>
+  </si>
+  <si>
+    <t>Who is J.M. Durao-Barroso?</t>
+  </si>
+  <si>
+    <t>The Portuguese PM as of 2012</t>
+  </si>
+  <si>
+    <t>The Portuguese finance minister</t>
+  </si>
+  <si>
+    <t>An economic view that advocates public intervention to compensate alleged inefficiencies of the private sector</t>
+  </si>
+  <si>
+    <t>An economic theory that promotes subsidies of key industries</t>
+  </si>
+  <si>
+    <t>An economic theory that establishes when to intervene a market</t>
+  </si>
+  <si>
+    <t>Who is John Maynard Keynes?</t>
+  </si>
+  <si>
+    <t>The 1st Baron Keynes, of Tilton in the County of Sussex</t>
+  </si>
+  <si>
+    <t>The leading figure of the Chicago School of thought</t>
+  </si>
+  <si>
+    <t>A recent proponent of the Austrian School</t>
+  </si>
+  <si>
+    <t>An international financial institution that provides loans to developing countries</t>
+  </si>
+  <si>
+    <t>A bank that provides liquidity for internatinal commerce</t>
+  </si>
+  <si>
+    <t>What is the World Bank operate?</t>
+  </si>
+  <si>
+    <t>A bank that provides settlement services between central banks</t>
+  </si>
+  <si>
+    <t>It arises when interest is added to the principal and generates interest</t>
+  </si>
+  <si>
+    <t>It is exactly equivalent to having infinite energy</t>
+  </si>
+  <si>
+    <t>It is the interest offered by a kind of stocks</t>
+  </si>
+  <si>
+    <t>What were the French 1st republic assignats?</t>
+  </si>
+  <si>
+    <t>Paper money issued by the National Assembly in France from 1789 to 1796</t>
+  </si>
+  <si>
+    <t>Treasury bonds that financed Robespiere</t>
+  </si>
+  <si>
+    <t>A check corresponding to one pound of silver payable to the bearer on demand</t>
+  </si>
+  <si>
+    <t>Bank of International Settlements</t>
+  </si>
+  <si>
+    <t>What does BIS stand for?</t>
+  </si>
+  <si>
+    <t>Bank of International Stocks</t>
+  </si>
+  <si>
+    <t>Bank of the Islamic Sharia</t>
+  </si>
+  <si>
+    <t>Credit is to the economy as. . .</t>
+  </si>
+  <si>
+    <t>Drugs to sports</t>
+  </si>
+  <si>
+    <t>Inflation to deflation</t>
+  </si>
+  <si>
+    <t>Gold to money</t>
   </si>
 </sst>
 </file>
@@ -2013,9 +2505,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2310,10 +2803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2573,7 +3066,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D14" t="s">
         <v>75</v>
@@ -2599,10 +3092,10 @@
         <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2826,16 +3319,16 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" t="s">
         <v>227</v>
       </c>
-      <c r="D28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>228</v>
-      </c>
-      <c r="F28" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2866,7 +3359,7 @@
         <v>186</v>
       </c>
       <c r="E30" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F30" t="s">
         <v>135</v>
@@ -2877,10 +3370,10 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="D31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E31" t="s">
         <v>186</v>
@@ -2979,7 +3472,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D37" t="s">
         <v>220</v>
@@ -2996,16 +3489,16 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D38" t="s">
+        <v>229</v>
+      </c>
+      <c r="E38" t="s">
         <v>230</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>231</v>
-      </c>
-      <c r="F38" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3013,16 +3506,16 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
+        <v>244</v>
+      </c>
+      <c r="D39" t="s">
         <v>245</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>246</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>247</v>
-      </c>
-      <c r="F39" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3030,16 +3523,16 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40" t="s">
         <v>249</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>250</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>251</v>
-      </c>
-      <c r="F40" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3047,16 +3540,16 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
+        <v>253</v>
+      </c>
+      <c r="D41" t="s">
+        <v>249</v>
+      </c>
+      <c r="E41" t="s">
+        <v>250</v>
+      </c>
+      <c r="F41" t="s">
         <v>254</v>
-      </c>
-      <c r="D41" t="s">
-        <v>250</v>
-      </c>
-      <c r="E41" t="s">
-        <v>251</v>
-      </c>
-      <c r="F41" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3064,16 +3557,16 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D42" t="s">
+        <v>255</v>
+      </c>
+      <c r="E42" t="s">
+        <v>257</v>
+      </c>
+      <c r="F42" t="s">
         <v>256</v>
-      </c>
-      <c r="E42" t="s">
-        <v>258</v>
-      </c>
-      <c r="F42" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3081,16 +3574,16 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" t="s">
         <v>260</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>261</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>262</v>
-      </c>
-      <c r="F43" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3098,16 +3591,16 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
+        <v>281</v>
+      </c>
+      <c r="D44" t="s">
+        <v>283</v>
+      </c>
+      <c r="E44" t="s">
         <v>282</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F44" t="s">
         <v>284</v>
-      </c>
-      <c r="E44" t="s">
-        <v>283</v>
-      </c>
-      <c r="F44" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3115,16 +3608,16 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D45" t="s">
+        <v>269</v>
+      </c>
+      <c r="E45" t="s">
         <v>270</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>271</v>
-      </c>
-      <c r="F45" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3132,16 +3625,16 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D46" t="s">
+        <v>272</v>
+      </c>
+      <c r="E46" t="s">
         <v>273</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>274</v>
-      </c>
-      <c r="F46" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3149,16 +3642,16 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
+        <v>277</v>
+      </c>
+      <c r="D47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E47" t="s">
         <v>278</v>
       </c>
-      <c r="D47" t="s">
-        <v>281</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>279</v>
-      </c>
-      <c r="F47" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3166,19 +3659,19 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
+        <v>285</v>
+      </c>
+      <c r="C48" t="s">
+        <v>289</v>
+      </c>
+      <c r="D48" t="s">
+        <v>287</v>
+      </c>
+      <c r="E48" t="s">
         <v>286</v>
       </c>
-      <c r="C48" t="s">
-        <v>290</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="F48" t="s">
         <v>288</v>
-      </c>
-      <c r="E48" t="s">
-        <v>287</v>
-      </c>
-      <c r="F48" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3186,16 +3679,16 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D49" t="s">
+        <v>290</v>
+      </c>
+      <c r="E49" t="s">
         <v>291</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>292</v>
-      </c>
-      <c r="F49" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3203,16 +3696,16 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
+        <v>294</v>
+      </c>
+      <c r="D50" t="s">
         <v>295</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>296</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>297</v>
-      </c>
-      <c r="F50" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3220,16 +3713,16 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
+        <v>298</v>
+      </c>
+      <c r="D51" t="s">
+        <v>617</v>
+      </c>
+      <c r="E51" t="s">
         <v>299</v>
       </c>
-      <c r="D51" t="s">
-        <v>627</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>300</v>
-      </c>
-      <c r="F51" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3237,16 +3730,16 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
+        <v>301</v>
+      </c>
+      <c r="D52" t="s">
+        <v>611</v>
+      </c>
+      <c r="E52" t="s">
+        <v>612</v>
+      </c>
+      <c r="F52" t="s">
         <v>302</v>
-      </c>
-      <c r="D52" t="s">
-        <v>621</v>
-      </c>
-      <c r="E52" t="s">
-        <v>622</v>
-      </c>
-      <c r="F52" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3254,16 +3747,16 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
+        <v>303</v>
+      </c>
+      <c r="D53" t="s">
         <v>304</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>305</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>306</v>
-      </c>
-      <c r="F53" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3271,16 +3764,16 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
+        <v>307</v>
+      </c>
+      <c r="D54" t="s">
         <v>308</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>309</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>310</v>
-      </c>
-      <c r="F54" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3288,16 +3781,16 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D55" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E55" t="s">
+        <v>356</v>
+      </c>
+      <c r="F55" t="s">
         <v>357</v>
-      </c>
-      <c r="F55" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3305,16 +3798,16 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D56" t="s">
+        <v>369</v>
+      </c>
+      <c r="E56" t="s">
         <v>370</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>371</v>
-      </c>
-      <c r="F56" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3322,16 +3815,16 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
+        <v>341</v>
+      </c>
+      <c r="D57" t="s">
         <v>342</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>343</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>344</v>
-      </c>
-      <c r="F57" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3339,16 +3832,16 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
+        <v>345</v>
+      </c>
+      <c r="D58" t="s">
+        <v>348</v>
+      </c>
+      <c r="E58" t="s">
+        <v>347</v>
+      </c>
+      <c r="F58" t="s">
         <v>346</v>
-      </c>
-      <c r="D58" t="s">
-        <v>349</v>
-      </c>
-      <c r="E58" t="s">
-        <v>348</v>
-      </c>
-      <c r="F58" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3356,16 +3849,16 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
+        <v>349</v>
+      </c>
+      <c r="D59" t="s">
         <v>350</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>351</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>352</v>
-      </c>
-      <c r="F59" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3373,16 +3866,16 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
+        <v>363</v>
+      </c>
+      <c r="D60" t="s">
+        <v>372</v>
+      </c>
+      <c r="E60" t="s">
         <v>364</v>
       </c>
-      <c r="D60" t="s">
-        <v>373</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>365</v>
-      </c>
-      <c r="F60" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3393,16 +3886,16 @@
         <v>25</v>
       </c>
       <c r="C61" t="s">
+        <v>381</v>
+      </c>
+      <c r="D61" t="s">
         <v>382</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>383</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>384</v>
-      </c>
-      <c r="F61" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3413,10 +3906,10 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D62" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E62" t="s">
         <v>121</v>
@@ -3430,16 +3923,16 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
+        <v>390</v>
+      </c>
+      <c r="D63" t="s">
         <v>391</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>392</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>393</v>
-      </c>
-      <c r="F63" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3447,16 +3940,16 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
+        <v>394</v>
+      </c>
+      <c r="D64" t="s">
         <v>395</v>
-      </c>
-      <c r="D64" t="s">
-        <v>396</v>
       </c>
       <c r="E64" t="s">
         <v>134</v>
       </c>
       <c r="F64" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3464,13 +3957,13 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D65" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F65" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3478,16 +3971,16 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D66" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="E66" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="F66" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3495,16 +3988,16 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D67" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="E67" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="F67" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3512,16 +4005,16 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D68" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="E68" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="F68" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3529,16 +4022,16 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D69" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="E69" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="F69" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3549,16 +4042,16 @@
         <v>25</v>
       </c>
       <c r="C70" t="s">
+        <v>420</v>
+      </c>
+      <c r="D70" t="s">
+        <v>421</v>
+      </c>
+      <c r="E70" t="s">
         <v>422</v>
       </c>
-      <c r="D70" t="s">
+      <c r="F70" t="s">
         <v>423</v>
-      </c>
-      <c r="E70" t="s">
-        <v>424</v>
-      </c>
-      <c r="F70" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -3566,16 +4059,16 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D71" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="E71" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="F71" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -3583,16 +4076,16 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
+        <v>426</v>
+      </c>
+      <c r="D72" t="s">
+        <v>427</v>
+      </c>
+      <c r="E72" t="s">
         <v>428</v>
       </c>
-      <c r="D72" t="s">
+      <c r="F72" t="s">
         <v>429</v>
-      </c>
-      <c r="E72" t="s">
-        <v>430</v>
-      </c>
-      <c r="F72" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -3600,7 +4093,16 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>438</v>
+        <v>436</v>
+      </c>
+      <c r="D73" t="s">
+        <v>729</v>
+      </c>
+      <c r="E73" t="s">
+        <v>730</v>
+      </c>
+      <c r="F73" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3611,16 +4113,16 @@
         <v>25</v>
       </c>
       <c r="C74" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D74" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="E74" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="F74" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3628,16 +4130,16 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="D75" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="E75" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="F75" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3645,7 +4147,16 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>507</v>
+        <v>501</v>
+      </c>
+      <c r="D76" t="s">
+        <v>740</v>
+      </c>
+      <c r="E76" t="s">
+        <v>743</v>
+      </c>
+      <c r="F76" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3653,7 +4164,16 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>506</v>
+        <v>500</v>
+      </c>
+      <c r="D77" t="s">
+        <v>742</v>
+      </c>
+      <c r="E77" t="s">
+        <v>743</v>
+      </c>
+      <c r="F77" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3661,16 +4181,16 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="D78" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="E78" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="F78" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3678,13 +4198,13 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -3695,16 +4215,16 @@
         <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="D80" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="E80" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="F80" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3712,7 +4232,16 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>525</v>
+        <v>745</v>
+      </c>
+      <c r="D81" t="s">
+        <v>746</v>
+      </c>
+      <c r="E81" t="s">
+        <v>648</v>
+      </c>
+      <c r="F81" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3720,7 +4249,16 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>526</v>
+        <v>645</v>
+      </c>
+      <c r="D82" t="s">
+        <v>646</v>
+      </c>
+      <c r="E82" t="s">
+        <v>647</v>
+      </c>
+      <c r="F82" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3728,10 +4266,16 @@
         <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="D83" t="s">
-        <v>528</v>
+        <v>521</v>
+      </c>
+      <c r="E83" t="s">
+        <v>747</v>
+      </c>
+      <c r="F83" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3739,7 +4283,7 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="D84" t="s">
         <v>17</v>
@@ -3748,7 +4292,7 @@
         <v>18</v>
       </c>
       <c r="F84" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3756,16 +4300,16 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="D85" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="E85" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="F85" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3773,7 +4317,16 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>530</v>
+        <v>523</v>
+      </c>
+      <c r="D86" t="s">
+        <v>769</v>
+      </c>
+      <c r="E86" t="s">
+        <v>770</v>
+      </c>
+      <c r="F86" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3781,7 +4334,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -3790,7 +4343,7 @@
         <v>17</v>
       </c>
       <c r="F87" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3798,7 +4351,16 @@
         <v>10</v>
       </c>
       <c r="B88" t="s">
-        <v>536</v>
+        <v>529</v>
+      </c>
+      <c r="D88" t="s">
+        <v>772</v>
+      </c>
+      <c r="E88" t="s">
+        <v>773</v>
+      </c>
+      <c r="F88" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -3806,7 +4368,16 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>535</v>
+        <v>528</v>
+      </c>
+      <c r="D89" t="s">
+        <v>785</v>
+      </c>
+      <c r="E89" t="s">
+        <v>786</v>
+      </c>
+      <c r="F89" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3814,10 +4385,16 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="D90" t="s">
-        <v>538</v>
+        <v>531</v>
+      </c>
+      <c r="E90" t="s">
+        <v>519</v>
+      </c>
+      <c r="F90" t="s">
+        <v>788</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3825,7 +4402,16 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>540</v>
+        <v>719</v>
+      </c>
+      <c r="D91" t="s">
+        <v>716</v>
+      </c>
+      <c r="E91" t="s">
+        <v>718</v>
+      </c>
+      <c r="F91" t="s">
+        <v>720</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3833,7 +4419,16 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>541</v>
+        <v>721</v>
+      </c>
+      <c r="D92" t="s">
+        <v>722</v>
+      </c>
+      <c r="E92" t="s">
+        <v>723</v>
+      </c>
+      <c r="F92" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3841,7 +4436,16 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>570</v>
+        <v>560</v>
+      </c>
+      <c r="D93" t="s">
+        <v>725</v>
+      </c>
+      <c r="E93" t="s">
+        <v>726</v>
+      </c>
+      <c r="F93" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -3849,16 +4453,16 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="D94" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="E94" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="F94" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3869,13 +4473,13 @@
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="D95" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="E95" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="F95" t="s">
         <v>45</v>
@@ -3889,13 +4493,13 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="D96" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="E96" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="F96" t="s">
         <v>45</v>
@@ -3909,16 +4513,16 @@
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="D97" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="E97" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="F97" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3926,7 +4530,16 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>567</v>
+        <v>557</v>
+      </c>
+      <c r="D98" t="s">
+        <v>727</v>
+      </c>
+      <c r="E98" t="s">
+        <v>449</v>
+      </c>
+      <c r="F98" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3934,16 +4547,16 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="D99" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="E99" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="F99" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3951,16 +4564,16 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="D100" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
       <c r="E100" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="F100" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3968,16 +4581,16 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="D101" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="E101" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="F101" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3985,16 +4598,16 @@
         <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="D102" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="E102" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="F102" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4002,146 +4615,580 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
+        <v>595</v>
+      </c>
+      <c r="D103" t="s">
+        <v>596</v>
+      </c>
+      <c r="E103" t="s">
+        <v>597</v>
+      </c>
+      <c r="F103" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>10</v>
+      </c>
+      <c r="B104" t="s">
+        <v>602</v>
+      </c>
+      <c r="D104" t="s">
+        <v>601</v>
+      </c>
+      <c r="E104" t="s">
+        <v>603</v>
+      </c>
+      <c r="F104" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105">
+        <v>10</v>
+      </c>
+      <c r="B105" t="s">
         <v>605</v>
       </c>
-      <c r="D103" t="s">
+      <c r="C105" t="s">
         <v>606</v>
       </c>
-      <c r="E103" t="s">
+      <c r="D105" t="s">
+        <v>620</v>
+      </c>
+      <c r="E105" t="s">
+        <v>618</v>
+      </c>
+      <c r="F105" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106">
+        <v>10</v>
+      </c>
+      <c r="B106" t="s">
         <v>607</v>
       </c>
-      <c r="F103" t="s">
+      <c r="D106" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="B104" t="s">
-        <v>612</v>
-      </c>
-      <c r="D104" t="s">
-        <v>611</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="E106" t="s">
+        <v>609</v>
+      </c>
+      <c r="F106" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107">
+        <v>10</v>
+      </c>
+      <c r="B107" t="s">
         <v>613</v>
       </c>
-      <c r="F104" t="s">
+      <c r="D107" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="B105" t="s">
+      <c r="E107" t="s">
         <v>615</v>
       </c>
-      <c r="C105" t="s">
+      <c r="F107" t="s">
         <v>616</v>
       </c>
-      <c r="D105" t="s">
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
+        <v>10</v>
+      </c>
+      <c r="B108" t="s">
+        <v>625</v>
+      </c>
+      <c r="D108" t="s">
+        <v>626</v>
+      </c>
+      <c r="E108" t="s">
+        <v>627</v>
+      </c>
+      <c r="F108" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
+        <v>10</v>
+      </c>
+      <c r="B109" t="s">
+        <v>629</v>
+      </c>
+      <c r="D109" t="s">
         <v>630</v>
-      </c>
-      <c r="E105" t="s">
-        <v>628</v>
-      </c>
-      <c r="F105" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="B106" t="s">
-        <v>617</v>
-      </c>
-      <c r="D106" t="s">
-        <v>618</v>
-      </c>
-      <c r="E106" t="s">
-        <v>619</v>
-      </c>
-      <c r="F106" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="B107" t="s">
-        <v>623</v>
-      </c>
-      <c r="D107" t="s">
-        <v>624</v>
-      </c>
-      <c r="E107" t="s">
-        <v>625</v>
-      </c>
-      <c r="F107" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="B108" t="s">
-        <v>635</v>
-      </c>
-      <c r="D108" t="s">
-        <v>636</v>
-      </c>
-      <c r="E108" t="s">
-        <v>637</v>
-      </c>
-      <c r="F108" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="B109" t="s">
-        <v>639</v>
-      </c>
-      <c r="D109" t="s">
-        <v>640</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
       </c>
       <c r="F109" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110">
+        <v>10</v>
+      </c>
+      <c r="B110" t="s">
+        <v>696</v>
+      </c>
+      <c r="D110" t="s">
+        <v>697</v>
+      </c>
+      <c r="E110" t="s">
+        <v>698</v>
+      </c>
+      <c r="F110" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111">
+        <v>10</v>
+      </c>
+      <c r="B111" t="s">
+        <v>649</v>
+      </c>
+      <c r="D111" t="s">
+        <v>650</v>
+      </c>
+      <c r="E111" t="s">
+        <v>651</v>
+      </c>
+      <c r="F111" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112">
+        <v>10</v>
+      </c>
+      <c r="B112" t="s">
+        <v>633</v>
+      </c>
+      <c r="D112" t="s">
+        <v>634</v>
+      </c>
+      <c r="E112" t="s">
+        <v>636</v>
+      </c>
+      <c r="F112" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>10</v>
+      </c>
+      <c r="B113" t="s">
+        <v>789</v>
+      </c>
+      <c r="D113" t="s">
+        <v>279</v>
+      </c>
+      <c r="E113" t="s">
+        <v>791</v>
+      </c>
+      <c r="F113" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
+        <v>10</v>
+      </c>
+      <c r="B114" t="s">
+        <v>644</v>
+      </c>
+      <c r="D114" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="B110" t="s">
+      <c r="E114" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="B111" t="s">
+      <c r="F114" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
-      <c r="B112" t="s">
-        <v>645</v>
-      </c>
-      <c r="D112" t="s">
-        <v>646</v>
-      </c>
-      <c r="E112" t="s">
-        <v>648</v>
-      </c>
-      <c r="F112" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6">
-      <c r="B113" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6">
-      <c r="B114" t="s">
-        <v>650</v>
-      </c>
-      <c r="D114" t="s">
-        <v>651</v>
-      </c>
-      <c r="E114" t="s">
-        <v>652</v>
-      </c>
-      <c r="F114" t="s">
-        <v>653</v>
+    <row r="115" spans="1:6">
+      <c r="A115">
+        <v>10</v>
+      </c>
+      <c r="B115" t="s">
+        <v>662</v>
+      </c>
+      <c r="D115" t="s">
+        <v>663</v>
+      </c>
+      <c r="E115" t="s">
+        <v>664</v>
+      </c>
+      <c r="F115" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
+        <v>10</v>
+      </c>
+      <c r="B116" t="s">
+        <v>666</v>
+      </c>
+      <c r="D116" t="s">
+        <v>667</v>
+      </c>
+      <c r="E116" t="s">
+        <v>668</v>
+      </c>
+      <c r="F116" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117">
+        <v>10</v>
+      </c>
+      <c r="B117" t="s">
+        <v>670</v>
+      </c>
+      <c r="D117" t="s">
+        <v>671</v>
+      </c>
+      <c r="E117" t="s">
+        <v>663</v>
+      </c>
+      <c r="F117" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118">
+        <v>10</v>
+      </c>
+      <c r="B118" t="s">
+        <v>673</v>
+      </c>
+      <c r="D118" t="s">
+        <v>783</v>
+      </c>
+      <c r="E118" t="s">
+        <v>780</v>
+      </c>
+      <c r="F118" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119">
+        <v>10</v>
+      </c>
+      <c r="B119" t="s">
+        <v>674</v>
+      </c>
+      <c r="D119" t="s">
+        <v>675</v>
+      </c>
+      <c r="E119" t="s">
+        <v>676</v>
+      </c>
+      <c r="F119" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120">
+        <v>10</v>
+      </c>
+      <c r="B120" t="s">
+        <v>680</v>
+      </c>
+      <c r="D120" t="s">
+        <v>678</v>
+      </c>
+      <c r="E120" t="s">
+        <v>679</v>
+      </c>
+      <c r="F120" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
+        <v>10</v>
+      </c>
+      <c r="B121" t="s">
+        <v>684</v>
+      </c>
+      <c r="D121" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E121" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="F121" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122">
+        <v>10</v>
+      </c>
+      <c r="B122" t="s">
+        <v>685</v>
+      </c>
+      <c r="D122" t="s">
+        <v>775</v>
+      </c>
+      <c r="E122" t="s">
+        <v>776</v>
+      </c>
+      <c r="F122" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
+        <v>10</v>
+      </c>
+      <c r="B123" t="s">
+        <v>686</v>
+      </c>
+      <c r="D123" t="s">
+        <v>776</v>
+      </c>
+      <c r="E123" t="s">
+        <v>775</v>
+      </c>
+      <c r="F123" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124">
+        <v>10</v>
+      </c>
+      <c r="B124" t="s">
+        <v>691</v>
+      </c>
+      <c r="D124" t="s">
+        <v>780</v>
+      </c>
+      <c r="E124" t="s">
+        <v>781</v>
+      </c>
+      <c r="F124" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
+        <v>10</v>
+      </c>
+      <c r="B125" t="s">
+        <v>736</v>
+      </c>
+      <c r="D125" t="s">
+        <v>737</v>
+      </c>
+      <c r="E125" t="s">
+        <v>738</v>
+      </c>
+      <c r="F125" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
+        <v>10</v>
+      </c>
+      <c r="B126" t="s">
+        <v>688</v>
+      </c>
+      <c r="D126" t="s">
+        <v>687</v>
+      </c>
+      <c r="E126" t="s">
+        <v>689</v>
+      </c>
+      <c r="F126" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127">
+        <v>10</v>
+      </c>
+      <c r="B127" t="s">
+        <v>749</v>
+      </c>
+      <c r="D127" t="s">
+        <v>601</v>
+      </c>
+      <c r="E127" t="s">
+        <v>750</v>
+      </c>
+      <c r="F127" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128">
+        <v>10</v>
+      </c>
+      <c r="B128" t="s">
+        <v>752</v>
+      </c>
+      <c r="D128" t="s">
+        <v>753</v>
+      </c>
+      <c r="E128" t="s">
+        <v>754</v>
+      </c>
+      <c r="F128" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129">
+        <v>10</v>
+      </c>
+      <c r="B129" t="s">
+        <v>756</v>
+      </c>
+      <c r="D129" t="s">
+        <v>757</v>
+      </c>
+      <c r="E129" t="s">
+        <v>758</v>
+      </c>
+      <c r="F129" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130">
+        <v>10</v>
+      </c>
+      <c r="B130" t="s">
+        <v>760</v>
+      </c>
+      <c r="D130" t="s">
+        <v>761</v>
+      </c>
+      <c r="E130" t="s">
+        <v>762</v>
+      </c>
+      <c r="F130" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131">
+        <v>10</v>
+      </c>
+      <c r="B131" t="s">
+        <v>764</v>
+      </c>
+      <c r="D131" t="s">
+        <v>765</v>
+      </c>
+      <c r="E131" t="s">
+        <v>766</v>
+      </c>
+      <c r="F131" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132">
+        <v>10</v>
+      </c>
+      <c r="B132" t="s">
+        <v>768</v>
+      </c>
+      <c r="D132" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E132" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F132" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133">
+        <v>10</v>
+      </c>
+      <c r="B133" t="s">
+        <v>779</v>
+      </c>
+      <c r="D133" t="s">
+        <v>792</v>
+      </c>
+      <c r="E133" t="s">
+        <v>793</v>
+      </c>
+      <c r="F133" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134">
+        <v>10</v>
+      </c>
+      <c r="B134" t="s">
+        <v>795</v>
+      </c>
+      <c r="D134" t="s">
+        <v>796</v>
+      </c>
+      <c r="E134" t="s">
+        <v>797</v>
+      </c>
+      <c r="F134" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135">
+        <v>10</v>
+      </c>
+      <c r="B135" t="s">
+        <v>811</v>
+      </c>
+      <c r="D135" t="s">
+        <v>810</v>
+      </c>
+      <c r="E135" t="s">
+        <v>812</v>
+      </c>
+      <c r="F135" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136">
+        <v>10</v>
+      </c>
+      <c r="B136" t="s">
+        <v>814</v>
+      </c>
+      <c r="D136" t="s">
+        <v>815</v>
+      </c>
+      <c r="E136" t="s">
+        <v>817</v>
+      </c>
+      <c r="F136" t="s">
+        <v>816</v>
       </c>
     </row>
   </sheetData>
@@ -4151,10 +5198,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4252,7 +5299,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -4278,7 +5325,7 @@
         <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4360,7 +5407,7 @@
         <v>78</v>
       </c>
       <c r="D11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E11" t="s">
         <v>79</v>
@@ -4391,7 +5438,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -4581,7 +5628,7 @@
         <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="E24" t="s">
         <v>192</v>
@@ -4595,16 +5642,16 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="D25" t="s">
+        <v>319</v>
+      </c>
+      <c r="E25" t="s">
+        <v>252</v>
+      </c>
+      <c r="F25" t="s">
         <v>320</v>
-      </c>
-      <c r="E25" t="s">
-        <v>253</v>
-      </c>
-      <c r="F25" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -4612,16 +5659,16 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26" t="s">
         <v>264</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>265</v>
-      </c>
-      <c r="F26" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -4629,16 +5676,16 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
+        <v>315</v>
+      </c>
+      <c r="D27" t="s">
         <v>316</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>317</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>318</v>
-      </c>
-      <c r="F27" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -4646,16 +5693,16 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
+        <v>321</v>
+      </c>
+      <c r="D28" t="s">
         <v>322</v>
-      </c>
-      <c r="D28" t="s">
-        <v>323</v>
       </c>
       <c r="E28" t="s">
         <v>193</v>
       </c>
       <c r="F28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -4663,16 +5710,16 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
+        <v>327</v>
+      </c>
+      <c r="D29" t="s">
         <v>328</v>
       </c>
-      <c r="D29" t="s">
-        <v>329</v>
-      </c>
       <c r="E29" t="s">
+        <v>325</v>
+      </c>
+      <c r="F29" t="s">
         <v>326</v>
-      </c>
-      <c r="F29" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -4680,16 +5727,16 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
+        <v>329</v>
+      </c>
+      <c r="D30" t="s">
         <v>330</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>331</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>332</v>
-      </c>
-      <c r="F30" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -4697,16 +5744,16 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D31" t="s">
+        <v>333</v>
+      </c>
+      <c r="E31" t="s">
         <v>334</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>335</v>
-      </c>
-      <c r="F31" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -4714,16 +5761,16 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
+        <v>339</v>
+      </c>
+      <c r="D32" t="s">
+        <v>337</v>
+      </c>
+      <c r="E32" t="s">
+        <v>338</v>
+      </c>
+      <c r="F32" t="s">
         <v>340</v>
-      </c>
-      <c r="D32" t="s">
-        <v>338</v>
-      </c>
-      <c r="E32" t="s">
-        <v>339</v>
-      </c>
-      <c r="F32" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -4731,7 +5778,7 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -4748,16 +5795,16 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
+        <v>359</v>
+      </c>
+      <c r="D34" t="s">
         <v>360</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>361</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>362</v>
-      </c>
-      <c r="F34" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -4768,16 +5815,16 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
+        <v>378</v>
+      </c>
+      <c r="D35" t="s">
         <v>379</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>380</v>
       </c>
-      <c r="E35" t="s">
-        <v>381</v>
-      </c>
       <c r="F35" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -4785,16 +5832,16 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
+        <v>385</v>
+      </c>
+      <c r="D36" t="s">
         <v>386</v>
       </c>
-      <c r="D36" t="s">
-        <v>387</v>
-      </c>
       <c r="E36" t="s">
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -4805,16 +5852,16 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -4822,16 +5869,16 @@
         <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="D38" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="E38" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F38" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -4839,7 +5886,16 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>399</v>
+        <v>706</v>
+      </c>
+      <c r="D39">
+        <v>1998</v>
+      </c>
+      <c r="E39">
+        <v>1992</v>
+      </c>
+      <c r="F39">
+        <v>2000</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -4847,16 +5903,16 @@
         <v>15</v>
       </c>
       <c r="B40" t="s">
+        <v>407</v>
+      </c>
+      <c r="D40" t="s">
+        <v>406</v>
+      </c>
+      <c r="E40" t="s">
+        <v>408</v>
+      </c>
+      <c r="F40" t="s">
         <v>409</v>
-      </c>
-      <c r="D40" t="s">
-        <v>408</v>
-      </c>
-      <c r="E40" t="s">
-        <v>410</v>
-      </c>
-      <c r="F40" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -4864,16 +5920,16 @@
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D41" t="s">
+        <v>411</v>
+      </c>
+      <c r="E41" t="s">
+        <v>412</v>
+      </c>
+      <c r="F41" t="s">
         <v>413</v>
-      </c>
-      <c r="E41" t="s">
-        <v>414</v>
-      </c>
-      <c r="F41" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -4881,16 +5937,16 @@
         <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D42" t="s">
+        <v>433</v>
+      </c>
+      <c r="E42" t="s">
+        <v>434</v>
+      </c>
+      <c r="F42" t="s">
         <v>435</v>
-      </c>
-      <c r="E42" t="s">
-        <v>436</v>
-      </c>
-      <c r="F42" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -4898,16 +5954,16 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D43" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="E43" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="F43" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -4915,16 +5971,16 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
+        <v>430</v>
+      </c>
+      <c r="D44" t="s">
+        <v>431</v>
+      </c>
+      <c r="E44" t="s">
+        <v>438</v>
+      </c>
+      <c r="F44" t="s">
         <v>432</v>
-      </c>
-      <c r="D44" t="s">
-        <v>433</v>
-      </c>
-      <c r="E44" t="s">
-        <v>441</v>
-      </c>
-      <c r="F44" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -4932,7 +5988,16 @@
         <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>439</v>
+        <v>437</v>
+      </c>
+      <c r="D45" t="s">
+        <v>711</v>
+      </c>
+      <c r="E45" t="s">
+        <v>712</v>
+      </c>
+      <c r="F45" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4940,7 +6005,16 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>440</v>
+        <v>801</v>
+      </c>
+      <c r="D46" t="s">
+        <v>799</v>
+      </c>
+      <c r="E46" t="s">
+        <v>800</v>
+      </c>
+      <c r="F46" t="s">
+        <v>802</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -4951,16 +6025,16 @@
         <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="D47" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="E47" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F47" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -4968,16 +6042,16 @@
         <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D48" t="s">
         <v>138</v>
       </c>
       <c r="E48" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F48" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -4985,16 +6059,16 @@
         <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="D49" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E49" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="F49" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -5002,16 +6076,16 @@
         <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D50" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E50" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="F50" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -5019,16 +6093,16 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="D51" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E51" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="F51" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -5036,16 +6110,16 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="D52" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="E52" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="F52" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -5053,7 +6127,16 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>539</v>
+        <v>714</v>
+      </c>
+      <c r="D53" t="s">
+        <v>715</v>
+      </c>
+      <c r="E53" t="s">
+        <v>716</v>
+      </c>
+      <c r="F53" t="s">
+        <v>717</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -5064,16 +6147,16 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="D54" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="E54" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="F54" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -5084,16 +6167,16 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="D55" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="E55" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="F55" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -5101,16 +6184,16 @@
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
       <c r="D56" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="E56" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="F56" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -5118,7 +6201,16 @@
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>602</v>
+        <v>592</v>
+      </c>
+      <c r="D57" t="s">
+        <v>803</v>
+      </c>
+      <c r="E57" t="s">
+        <v>804</v>
+      </c>
+      <c r="F57" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -5126,16 +6218,16 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="D58" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="E58" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="F58" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -5143,21 +6235,169 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="D59" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="E59" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="F59" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
     </row>
     <row r="60" spans="1:6">
+      <c r="A60">
+        <v>15</v>
+      </c>
       <c r="B60" t="s">
-        <v>644</v>
+        <v>806</v>
+      </c>
+      <c r="D60" t="s">
+        <v>807</v>
+      </c>
+      <c r="E60" t="s">
+        <v>808</v>
+      </c>
+      <c r="F60" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>15</v>
+      </c>
+      <c r="B61" t="s">
+        <v>637</v>
+      </c>
+      <c r="D61" t="s">
+        <v>638</v>
+      </c>
+      <c r="E61" t="s">
+        <v>639</v>
+      </c>
+      <c r="F61" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>15</v>
+      </c>
+      <c r="B62" t="s">
+        <v>653</v>
+      </c>
+      <c r="D62" t="s">
+        <v>654</v>
+      </c>
+      <c r="E62" t="s">
+        <v>655</v>
+      </c>
+      <c r="F62" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>15</v>
+      </c>
+      <c r="B63" t="s">
+        <v>682</v>
+      </c>
+      <c r="D63" t="s">
+        <v>683</v>
+      </c>
+      <c r="E63" t="s">
+        <v>91</v>
+      </c>
+      <c r="F63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>15</v>
+      </c>
+      <c r="B64" t="s">
+        <v>700</v>
+      </c>
+      <c r="D64">
+        <v>2007</v>
+      </c>
+      <c r="E64">
+        <v>2008</v>
+      </c>
+      <c r="F64">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>15</v>
+      </c>
+      <c r="B65" t="s">
+        <v>704</v>
+      </c>
+      <c r="D65" t="s">
+        <v>701</v>
+      </c>
+      <c r="E65" t="s">
+        <v>702</v>
+      </c>
+      <c r="F65" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>15</v>
+      </c>
+      <c r="B66" t="s">
+        <v>707</v>
+      </c>
+      <c r="D66" t="s">
+        <v>708</v>
+      </c>
+      <c r="E66" t="s">
+        <v>709</v>
+      </c>
+      <c r="F66" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>15</v>
+      </c>
+      <c r="B67" t="s">
+        <v>735</v>
+      </c>
+      <c r="D67" t="s">
+        <v>732</v>
+      </c>
+      <c r="E67" t="s">
+        <v>733</v>
+      </c>
+      <c r="F67" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>692</v>
+      </c>
+      <c r="D68" t="s">
+        <v>693</v>
+      </c>
+      <c r="E68" t="s">
+        <v>694</v>
+      </c>
+      <c r="F68" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -5167,10 +6407,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5259,7 +6499,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>130</v>
@@ -5330,13 +6570,13 @@
         <v>221</v>
       </c>
       <c r="D9" t="s">
+        <v>705</v>
+      </c>
+      <c r="E9" t="s">
         <v>222</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>223</v>
-      </c>
-      <c r="F9" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5344,16 +6584,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" t="s">
         <v>235</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>237</v>
-      </c>
-      <c r="E10" t="s">
-        <v>236</v>
-      </c>
-      <c r="F10" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5361,16 +6601,16 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" t="s">
+        <v>238</v>
+      </c>
+      <c r="E11" t="s">
         <v>239</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>240</v>
-      </c>
-      <c r="F11" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5378,16 +6618,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D12" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" t="s">
         <v>243</v>
-      </c>
-      <c r="F12" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5395,16 +6635,16 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" t="s">
+        <v>311</v>
+      </c>
+      <c r="E13" t="s">
         <v>313</v>
       </c>
-      <c r="D13" t="s">
-        <v>312</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>314</v>
-      </c>
-      <c r="F13" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5412,16 +6652,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D14" t="s">
+        <v>366</v>
+      </c>
+      <c r="E14" t="s">
         <v>367</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>368</v>
-      </c>
-      <c r="F14" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5429,7 +6669,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5437,7 +6677,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -5445,16 +6685,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D17" t="s">
-        <v>452</v>
+        <v>657</v>
       </c>
       <c r="E17" t="s">
-        <v>453</v>
+        <v>658</v>
       </c>
       <c r="F17" t="s">
-        <v>454</v>
+        <v>659</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -5462,16 +6702,16 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D18" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E18" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="F18" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -5479,16 +6719,16 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D19" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="E19" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="F19" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -5496,16 +6736,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D20" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="E20" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="F20" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -5513,16 +6753,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="D21" t="s">
+        <v>398</v>
+      </c>
+      <c r="E21" t="s">
+        <v>399</v>
+      </c>
+      <c r="F21" t="s">
         <v>400</v>
-      </c>
-      <c r="E21" t="s">
-        <v>401</v>
-      </c>
-      <c r="F21" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -5530,16 +6770,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="D22" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E22" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F22" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -5550,16 +6790,16 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="D23" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="E23" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="F23" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -5567,16 +6807,16 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="D24" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="E24" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="F24" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -5584,16 +6824,16 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="D25" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="E25" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F25" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -5601,7 +6841,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -5609,16 +6849,49 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="D27" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="E27" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="F27" t="s">
-        <v>601</v>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>660</v>
+      </c>
+      <c r="D28" t="s">
+        <v>504</v>
+      </c>
+      <c r="E28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed activity transitions into within-activity transitions
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="883">
   <si>
     <t>Difficulty</t>
   </si>
@@ -2470,6 +2470,201 @@
   </si>
   <si>
     <t>Gold to money</t>
+  </si>
+  <si>
+    <t>John Corzine</t>
+  </si>
+  <si>
+    <t>Hunt Brothers</t>
+  </si>
+  <si>
+    <t>Bernie Madoff performed duties as. . .</t>
+  </si>
+  <si>
+    <t>NASDAQ CEO</t>
+  </si>
+  <si>
+    <t>White-collar stealing</t>
+  </si>
+  <si>
+    <t>Stock analyst</t>
+  </si>
+  <si>
+    <t>Bernie Madoff</t>
+  </si>
+  <si>
+    <t>Who was the head of a pyramidal scheme that notoriously blew up in 2011?</t>
+  </si>
+  <si>
+    <t>WTI futures</t>
+  </si>
+  <si>
+    <t>Brent futures</t>
+  </si>
+  <si>
+    <t>Cushing spot swaps</t>
+  </si>
+  <si>
+    <t>What contracts are traded at NYMEX?</t>
+  </si>
+  <si>
+    <t>Where does the Brent future contract trade?</t>
+  </si>
+  <si>
+    <t>ICE</t>
+  </si>
+  <si>
+    <t>NYMEX</t>
+  </si>
+  <si>
+    <t>CBOE</t>
+  </si>
+  <si>
+    <t>What does Brent oil mean?</t>
+  </si>
+  <si>
+    <t>Oil pumped from the Norwegian North Sea coast</t>
+  </si>
+  <si>
+    <t>Oil mixed with heavy sands</t>
+  </si>
+  <si>
+    <t>Oil from the OPEC</t>
+  </si>
+  <si>
+    <t>What is the oil that sets gas prices in Europe?</t>
+  </si>
+  <si>
+    <t>Brent oil</t>
+  </si>
+  <si>
+    <t>OPEC oil</t>
+  </si>
+  <si>
+    <t>WTI oil</t>
+  </si>
+  <si>
+    <t>Brent oil contracts are traded. . .</t>
+  </si>
+  <si>
+    <t>In London and priced in dollars</t>
+  </si>
+  <si>
+    <t>In London and priced in pounds sterling</t>
+  </si>
+  <si>
+    <t>In New York City and priced in dollars</t>
+  </si>
+  <si>
+    <t>What can I pick up in Cushing, Ocklahoma?</t>
+  </si>
+  <si>
+    <t>WTI barrels</t>
+  </si>
+  <si>
+    <t>Live cattle</t>
+  </si>
+  <si>
+    <t>Wheat bushels</t>
+  </si>
+  <si>
+    <t>Where is the strait of Hormuz?</t>
+  </si>
+  <si>
+    <t>In the Persial gulf</t>
+  </si>
+  <si>
+    <t>In Southern Spain</t>
+  </si>
+  <si>
+    <t>What is the OPEC?</t>
+  </si>
+  <si>
+    <t>An oil cartel composed mostly of Arab nations with headquartes in Vienna</t>
+  </si>
+  <si>
+    <t>An oil company</t>
+  </si>
+  <si>
+    <t>An oil cartel with headquartes in Qatar</t>
+  </si>
+  <si>
+    <t>In Northern Iran</t>
+  </si>
+  <si>
+    <t>I believe that banking institutions are more dangerous to our liberties than standing armies</t>
+  </si>
+  <si>
+    <t>Who said "I believe that banking institutions are more dangerous to our liberties than standing armies"?</t>
+  </si>
+  <si>
+    <t>John Adams</t>
+  </si>
+  <si>
+    <t>Who said "The modern theory of the perpetuation of debt has drenched the earth with blood, and crushed its inhabitants under burdens ever accumulating"?</t>
+  </si>
+  <si>
+    <t>James Madison</t>
+  </si>
+  <si>
+    <t>Andrew Jackson</t>
+  </si>
+  <si>
+    <t>In his speech against the 1809 recharter of the First Bank, Thomas Jefferson said. . .</t>
+  </si>
+  <si>
+    <t>. . .The issuing power should be taken from the banks and restored to the people, to whom it properly belongs</t>
+  </si>
+  <si>
+    <t>"Congress was given the reight to issue paper money themselves, not to delegate it to individuals or corporations"</t>
+  </si>
+  <si>
+    <t>Who said "Issue of currency should be lodged with the government and be protected from domination by Wall Street"?</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt</t>
+  </si>
+  <si>
+    <t>Who said "If congress has the right under the Constitution to issue paper money, it was  given them to use themselves, not to be delegated to individuals or corporations"?</t>
+  </si>
+  <si>
+    <t>The words "I am a most unhappy man. I have unwittingly ruined my country…" were written by. . .</t>
+  </si>
+  <si>
+    <t>Woodrow Wilson</t>
+  </si>
+  <si>
+    <t>Theodor Roosevelt</t>
+  </si>
+  <si>
+    <t>Who said "The real truth of the matter is that a financial element in the large centers has owned the government ever since the days of Andrew Jackson"?</t>
+  </si>
+  <si>
+    <t>Who said "Money has no motherland; financiers are without patriotism and without decency; their sole object is gain"?</t>
+  </si>
+  <si>
+    <t>Who said "I fear that foreign bankers will entirely control the exuberant riches of America and use them to systematically corrupt civilization"?</t>
+  </si>
+  <si>
+    <t>Otto von Bismarck</t>
+  </si>
+  <si>
+    <t>Where can you read the following text? "Money plays the largest part in determining the course of history"</t>
+  </si>
+  <si>
+    <t>The Communist Manifesto</t>
+  </si>
+  <si>
+    <t>The Republic</t>
+  </si>
+  <si>
+    <t>The Wealth of Nations</t>
+  </si>
+  <si>
+    <t>Who said "Banks lend by creating credit. They create the means of payment out of nothing"?</t>
+  </si>
+  <si>
+    <t>Ralph M. Hawtry</t>
   </si>
 </sst>
 </file>
@@ -2803,10 +2998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5191,6 +5386,357 @@
         <v>816</v>
       </c>
     </row>
+    <row r="137" spans="1:6">
+      <c r="A137">
+        <v>10</v>
+      </c>
+      <c r="B137" t="s">
+        <v>820</v>
+      </c>
+      <c r="D137" t="s">
+        <v>821</v>
+      </c>
+      <c r="E137" t="s">
+        <v>822</v>
+      </c>
+      <c r="F137" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138">
+        <v>10</v>
+      </c>
+      <c r="B138" t="s">
+        <v>825</v>
+      </c>
+      <c r="D138" t="s">
+        <v>824</v>
+      </c>
+      <c r="E138" t="s">
+        <v>41</v>
+      </c>
+      <c r="F138" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139">
+        <v>10</v>
+      </c>
+      <c r="B139" t="s">
+        <v>829</v>
+      </c>
+      <c r="D139" t="s">
+        <v>826</v>
+      </c>
+      <c r="E139" t="s">
+        <v>827</v>
+      </c>
+      <c r="F139" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140">
+        <v>10</v>
+      </c>
+      <c r="B140" t="s">
+        <v>830</v>
+      </c>
+      <c r="D140" t="s">
+        <v>831</v>
+      </c>
+      <c r="E140" t="s">
+        <v>832</v>
+      </c>
+      <c r="F140" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141">
+        <v>10</v>
+      </c>
+      <c r="B141" t="s">
+        <v>834</v>
+      </c>
+      <c r="D141" t="s">
+        <v>835</v>
+      </c>
+      <c r="E141" t="s">
+        <v>836</v>
+      </c>
+      <c r="F141" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142">
+        <v>10</v>
+      </c>
+      <c r="B142" t="s">
+        <v>838</v>
+      </c>
+      <c r="D142" t="s">
+        <v>839</v>
+      </c>
+      <c r="E142" t="s">
+        <v>840</v>
+      </c>
+      <c r="F142" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143">
+        <v>10</v>
+      </c>
+      <c r="B143" t="s">
+        <v>842</v>
+      </c>
+      <c r="D143" t="s">
+        <v>843</v>
+      </c>
+      <c r="E143" t="s">
+        <v>844</v>
+      </c>
+      <c r="F143" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144">
+        <v>10</v>
+      </c>
+      <c r="B144" t="s">
+        <v>846</v>
+      </c>
+      <c r="D144" t="s">
+        <v>847</v>
+      </c>
+      <c r="E144" t="s">
+        <v>848</v>
+      </c>
+      <c r="F144" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145">
+        <v>10</v>
+      </c>
+      <c r="B145" t="s">
+        <v>850</v>
+      </c>
+      <c r="D145" t="s">
+        <v>851</v>
+      </c>
+      <c r="E145" t="s">
+        <v>852</v>
+      </c>
+      <c r="F145" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146">
+        <v>10</v>
+      </c>
+      <c r="B146" t="s">
+        <v>853</v>
+      </c>
+      <c r="D146" t="s">
+        <v>854</v>
+      </c>
+      <c r="E146" t="s">
+        <v>855</v>
+      </c>
+      <c r="F146" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147">
+        <v>10</v>
+      </c>
+      <c r="B147" t="s">
+        <v>859</v>
+      </c>
+      <c r="D147" t="s">
+        <v>250</v>
+      </c>
+      <c r="E147" t="s">
+        <v>249</v>
+      </c>
+      <c r="F147" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148">
+        <v>10</v>
+      </c>
+      <c r="B148" t="s">
+        <v>861</v>
+      </c>
+      <c r="D148" t="s">
+        <v>250</v>
+      </c>
+      <c r="E148" t="s">
+        <v>862</v>
+      </c>
+      <c r="F148" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149">
+        <v>10</v>
+      </c>
+      <c r="B149" t="s">
+        <v>864</v>
+      </c>
+      <c r="D149" t="s">
+        <v>865</v>
+      </c>
+      <c r="E149" t="s">
+        <v>858</v>
+      </c>
+      <c r="F149" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150">
+        <v>10</v>
+      </c>
+      <c r="B150" t="s">
+        <v>867</v>
+      </c>
+      <c r="D150" t="s">
+        <v>868</v>
+      </c>
+      <c r="E150" t="s">
+        <v>862</v>
+      </c>
+      <c r="F150" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151">
+        <v>10</v>
+      </c>
+      <c r="B151" t="s">
+        <v>869</v>
+      </c>
+      <c r="D151" t="s">
+        <v>863</v>
+      </c>
+      <c r="E151" t="s">
+        <v>862</v>
+      </c>
+      <c r="F151" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152">
+        <v>10</v>
+      </c>
+      <c r="B152" t="s">
+        <v>870</v>
+      </c>
+      <c r="D152" t="s">
+        <v>871</v>
+      </c>
+      <c r="E152" t="s">
+        <v>872</v>
+      </c>
+      <c r="F152" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153">
+        <v>10</v>
+      </c>
+      <c r="B153" t="s">
+        <v>873</v>
+      </c>
+      <c r="D153" t="s">
+        <v>75</v>
+      </c>
+      <c r="E153" t="s">
+        <v>871</v>
+      </c>
+      <c r="F153" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154">
+        <v>10</v>
+      </c>
+      <c r="B154" t="s">
+        <v>874</v>
+      </c>
+      <c r="D154" t="s">
+        <v>630</v>
+      </c>
+      <c r="E154" t="s">
+        <v>250</v>
+      </c>
+      <c r="F154" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155">
+        <v>10</v>
+      </c>
+      <c r="B155" t="s">
+        <v>875</v>
+      </c>
+      <c r="D155" t="s">
+        <v>876</v>
+      </c>
+      <c r="E155" t="s">
+        <v>630</v>
+      </c>
+      <c r="F155" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="B156" t="s">
+        <v>877</v>
+      </c>
+      <c r="D156" t="s">
+        <v>878</v>
+      </c>
+      <c r="E156" t="s">
+        <v>879</v>
+      </c>
+      <c r="F156" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="B157" t="s">
+        <v>881</v>
+      </c>
+      <c r="D157" t="s">
+        <v>882</v>
+      </c>
+      <c r="E157" t="s">
+        <v>876</v>
+      </c>
+      <c r="F157" t="s">
+        <v>630</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5198,10 +5744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6400,6 +6946,16 @@
         <v>695</v>
       </c>
     </row>
+    <row r="69" spans="1:6">
+      <c r="B69" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="B70" t="s">
+        <v>819</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6409,7 +6965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Questions updated up to 172 questions at level 1
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="883">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="907">
   <si>
     <t>Difficulty</t>
   </si>
@@ -885,9 +885,6 @@
     <t>In the French colonies and Quebec</t>
   </si>
   <si>
-    <t>8reales1</t>
-  </si>
-  <si>
     <t>European powers needed to finance the costs of WWI</t>
   </si>
   <si>
@@ -1224,9 +1221,6 @@
     <t xml:space="preserve">The first huge bailout and the one that gave name to the Greenspan's put </t>
   </si>
   <si>
-    <t>What is a currency swap?</t>
-  </si>
-  <si>
     <t>What is the Bank of International Settlements?</t>
   </si>
   <si>
@@ -1248,9 +1242,6 @@
     <t>BBVA Abbey</t>
   </si>
   <si>
-    <t>How does the BIS operate?</t>
-  </si>
-  <si>
     <t>It is the central bank of central banks</t>
   </si>
   <si>
@@ -1713,9 +1704,6 @@
     <t>Lawrence Livermore and Nathan Rothschild</t>
   </si>
   <si>
-    <t>Who was Lawrence Livermore?</t>
-  </si>
-  <si>
     <t>In the 80's Ed Thorp employed a portfolio selection method using. . .</t>
   </si>
   <si>
@@ -1914,9 +1902,6 @@
     <t>Hjalmar Schacht</t>
   </si>
   <si>
-    <t>John Law</t>
-  </si>
-  <si>
     <t>The French 1st republic raised funds by. . .</t>
   </si>
   <si>
@@ -2475,9 +2460,6 @@
     <t>John Corzine</t>
   </si>
   <si>
-    <t>Hunt Brothers</t>
-  </si>
-  <si>
     <t>Bernie Madoff performed duties as. . .</t>
   </si>
   <si>
@@ -2613,12 +2595,6 @@
     <t>In his speech against the 1809 recharter of the First Bank, Thomas Jefferson said. . .</t>
   </si>
   <si>
-    <t>. . .The issuing power should be taken from the banks and restored to the people, to whom it properly belongs</t>
-  </si>
-  <si>
-    <t>"Congress was given the reight to issue paper money themselves, not to delegate it to individuals or corporations"</t>
-  </si>
-  <si>
     <t>Who said "Issue of currency should be lodged with the government and be protected from domination by Wall Street"?</t>
   </si>
   <si>
@@ -2665,6 +2641,102 @@
   </si>
   <si>
     <t>Ralph M. Hawtry</t>
+  </si>
+  <si>
+    <t>Bernard Madoff</t>
+  </si>
+  <si>
+    <t>madoff1</t>
+  </si>
+  <si>
+    <t>corzine1</t>
+  </si>
+  <si>
+    <t>Gary Gensler</t>
+  </si>
+  <si>
+    <t>hunt1</t>
+  </si>
+  <si>
+    <t>Nelson Bunker Hunt</t>
+  </si>
+  <si>
+    <t>The Hunt Brothers were infamous for. . .</t>
+  </si>
+  <si>
+    <t>Trying to corner the silver market</t>
+  </si>
+  <si>
+    <t>Setting up the largest pyramidal scheme in the 70s</t>
+  </si>
+  <si>
+    <t>Trying to corner the oil market</t>
+  </si>
+  <si>
+    <t>Congress was given the reight to issue paper money themselves, not to delegate it to individuals or corporations</t>
+  </si>
+  <si>
+    <t>The issuing power should be taken from the banks and restored to the people, to whom it properly belongs</t>
+  </si>
+  <si>
+    <t>Who was John Law?</t>
+  </si>
+  <si>
+    <t>A Scottish economist</t>
+  </si>
+  <si>
+    <t>An English financier</t>
+  </si>
+  <si>
+    <t>An Irish trader</t>
+  </si>
+  <si>
+    <t>What is a currency liquidity swap?</t>
+  </si>
+  <si>
+    <t>A swap used by a country's central bank to provide liquidity of its currency to another country's central bank</t>
+  </si>
+  <si>
+    <t>An instrument in which two parties agree to exchange interest rate cash flows but not the principal</t>
+  </si>
+  <si>
+    <t>A derivative traded on exchanges</t>
+  </si>
+  <si>
+    <t>Bank of Illinois-Springfield</t>
+  </si>
+  <si>
+    <t>Bank of International Shippings</t>
+  </si>
+  <si>
+    <t>A banker</t>
+  </si>
+  <si>
+    <t>A finance minister</t>
+  </si>
+  <si>
+    <t>Who was Jesse Livermore?</t>
+  </si>
+  <si>
+    <t>An American stock trader</t>
+  </si>
+  <si>
+    <t>Which was Jesse Livermore's nickname?</t>
+  </si>
+  <si>
+    <t>Boy Plunger</t>
+  </si>
+  <si>
+    <t>Killerboy</t>
+  </si>
+  <si>
+    <t>Dr. Bear</t>
+  </si>
+  <si>
+    <t>The first of a series of bailouts starting in 2007</t>
+  </si>
+  <si>
+    <t>reales1</t>
   </si>
 </sst>
 </file>
@@ -2998,10 +3070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3261,7 +3333,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D14" t="s">
         <v>75</v>
@@ -3287,10 +3359,10 @@
         <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3554,7 +3626,7 @@
         <v>186</v>
       </c>
       <c r="E30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F30" t="s">
         <v>135</v>
@@ -3565,10 +3637,10 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D31" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E31" t="s">
         <v>186</v>
@@ -3857,7 +3929,7 @@
         <v>285</v>
       </c>
       <c r="C48" t="s">
-        <v>289</v>
+        <v>906</v>
       </c>
       <c r="D48" t="s">
         <v>287</v>
@@ -3874,16 +3946,16 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D49" t="s">
+        <v>289</v>
+      </c>
+      <c r="E49" t="s">
         <v>290</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>291</v>
-      </c>
-      <c r="F49" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3891,16 +3963,16 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
+        <v>293</v>
+      </c>
+      <c r="D50" t="s">
         <v>294</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>295</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>296</v>
-      </c>
-      <c r="F50" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3908,16 +3980,16 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
+        <v>297</v>
+      </c>
+      <c r="D51" t="s">
+        <v>613</v>
+      </c>
+      <c r="E51" t="s">
         <v>298</v>
       </c>
-      <c r="D51" t="s">
-        <v>617</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>299</v>
-      </c>
-      <c r="F51" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3925,16 +3997,16 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
+        <v>300</v>
+      </c>
+      <c r="D52" t="s">
+        <v>607</v>
+      </c>
+      <c r="E52" t="s">
+        <v>608</v>
+      </c>
+      <c r="F52" t="s">
         <v>301</v>
-      </c>
-      <c r="D52" t="s">
-        <v>611</v>
-      </c>
-      <c r="E52" t="s">
-        <v>612</v>
-      </c>
-      <c r="F52" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3942,16 +4014,16 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
+        <v>302</v>
+      </c>
+      <c r="D53" t="s">
         <v>303</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>304</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>305</v>
-      </c>
-      <c r="F53" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3959,16 +4031,16 @@
         <v>10</v>
       </c>
       <c r="B54" t="s">
+        <v>306</v>
+      </c>
+      <c r="D54" t="s">
         <v>307</v>
       </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>308</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>309</v>
-      </c>
-      <c r="F54" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3976,16 +4048,16 @@
         <v>10</v>
       </c>
       <c r="B55" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D55" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E55" t="s">
+        <v>355</v>
+      </c>
+      <c r="F55" t="s">
         <v>356</v>
-      </c>
-      <c r="F55" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3993,16 +4065,16 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D56" t="s">
+        <v>368</v>
+      </c>
+      <c r="E56" t="s">
         <v>369</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>370</v>
-      </c>
-      <c r="F56" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -4010,16 +4082,16 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
+        <v>340</v>
+      </c>
+      <c r="D57" t="s">
         <v>341</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>342</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>343</v>
-      </c>
-      <c r="F57" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -4027,16 +4099,16 @@
         <v>10</v>
       </c>
       <c r="B58" t="s">
+        <v>344</v>
+      </c>
+      <c r="D58" t="s">
+        <v>347</v>
+      </c>
+      <c r="E58" t="s">
+        <v>346</v>
+      </c>
+      <c r="F58" t="s">
         <v>345</v>
-      </c>
-      <c r="D58" t="s">
-        <v>348</v>
-      </c>
-      <c r="E58" t="s">
-        <v>347</v>
-      </c>
-      <c r="F58" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -4044,16 +4116,16 @@
         <v>10</v>
       </c>
       <c r="B59" t="s">
+        <v>348</v>
+      </c>
+      <c r="D59" t="s">
         <v>349</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>350</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>351</v>
-      </c>
-      <c r="F59" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -4061,16 +4133,16 @@
         <v>10</v>
       </c>
       <c r="B60" t="s">
+        <v>362</v>
+      </c>
+      <c r="D60" t="s">
+        <v>371</v>
+      </c>
+      <c r="E60" t="s">
         <v>363</v>
       </c>
-      <c r="D60" t="s">
-        <v>372</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>364</v>
-      </c>
-      <c r="F60" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -4081,16 +4153,16 @@
         <v>25</v>
       </c>
       <c r="C61" t="s">
+        <v>380</v>
+      </c>
+      <c r="D61" t="s">
         <v>381</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>382</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>383</v>
-      </c>
-      <c r="F61" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -4101,10 +4173,10 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D62" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E62" t="s">
         <v>121</v>
@@ -4118,16 +4190,16 @@
         <v>10</v>
       </c>
       <c r="B63" t="s">
+        <v>389</v>
+      </c>
+      <c r="D63" t="s">
         <v>390</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>391</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>392</v>
-      </c>
-      <c r="F63" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -4135,16 +4207,16 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
+        <v>393</v>
+      </c>
+      <c r="D64" t="s">
         <v>394</v>
-      </c>
-      <c r="D64" t="s">
-        <v>395</v>
       </c>
       <c r="E64" t="s">
         <v>134</v>
       </c>
       <c r="F64" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -4152,13 +4224,16 @@
         <v>10</v>
       </c>
       <c r="B65" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D65" t="s">
-        <v>401</v>
+        <v>400</v>
+      </c>
+      <c r="E65" t="s">
+        <v>905</v>
       </c>
       <c r="F65" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -4166,16 +4241,16 @@
         <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D66" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E66" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F66" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4183,16 +4258,16 @@
         <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D67" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E67" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F67" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4200,16 +4275,16 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D68" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E68" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F68" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4217,16 +4292,16 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D69" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E69" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F69" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4237,16 +4312,16 @@
         <v>25</v>
       </c>
       <c r="C70" t="s">
+        <v>417</v>
+      </c>
+      <c r="D70" t="s">
+        <v>418</v>
+      </c>
+      <c r="E70" t="s">
+        <v>419</v>
+      </c>
+      <c r="F70" t="s">
         <v>420</v>
-      </c>
-      <c r="D70" t="s">
-        <v>421</v>
-      </c>
-      <c r="E70" t="s">
-        <v>422</v>
-      </c>
-      <c r="F70" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4254,16 +4329,16 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D71" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E71" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F71" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4271,16 +4346,16 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
+        <v>423</v>
+      </c>
+      <c r="D72" t="s">
+        <v>424</v>
+      </c>
+      <c r="E72" t="s">
+        <v>425</v>
+      </c>
+      <c r="F72" t="s">
         <v>426</v>
-      </c>
-      <c r="D72" t="s">
-        <v>427</v>
-      </c>
-      <c r="E72" t="s">
-        <v>428</v>
-      </c>
-      <c r="F72" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4288,16 +4363,16 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D73" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="E73" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="F73" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4308,16 +4383,16 @@
         <v>25</v>
       </c>
       <c r="C74" t="s">
+        <v>472</v>
+      </c>
+      <c r="D74" t="s">
+        <v>473</v>
+      </c>
+      <c r="E74" t="s">
+        <v>474</v>
+      </c>
+      <c r="F74" t="s">
         <v>475</v>
-      </c>
-      <c r="D74" t="s">
-        <v>476</v>
-      </c>
-      <c r="E74" t="s">
-        <v>477</v>
-      </c>
-      <c r="F74" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -4325,16 +4400,16 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D75" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E75" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F75" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -4342,16 +4417,16 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D76" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="E76" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="F76" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4359,16 +4434,16 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D77" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="E77" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="F77" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4376,16 +4451,16 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D78" t="s">
+        <v>505</v>
+      </c>
+      <c r="E78" t="s">
+        <v>506</v>
+      </c>
+      <c r="F78" t="s">
         <v>508</v>
-      </c>
-      <c r="E78" t="s">
-        <v>509</v>
-      </c>
-      <c r="F78" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -4393,13 +4468,13 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D79" t="s">
         <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -4410,16 +4485,16 @@
         <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D80" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E80" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F80" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4427,16 +4502,16 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="D81" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="E81" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F81" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4444,16 +4519,16 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="D82" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="E82" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="F82" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4461,16 +4536,16 @@
         <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D83" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E83" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="F83" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -4478,7 +4553,7 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D84" t="s">
         <v>17</v>
@@ -4487,7 +4562,7 @@
         <v>18</v>
       </c>
       <c r="F84" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -4495,16 +4570,16 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D85" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E85" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F85" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -4512,16 +4587,16 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D86" t="s">
-        <v>769</v>
+        <v>764</v>
       </c>
       <c r="E86" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="F86" t="s">
-        <v>771</v>
+        <v>766</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -4529,7 +4604,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -4538,7 +4613,7 @@
         <v>17</v>
       </c>
       <c r="F87" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -4546,16 +4621,16 @@
         <v>10</v>
       </c>
       <c r="B88" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D88" t="s">
-        <v>772</v>
+        <v>767</v>
       </c>
       <c r="E88" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
       <c r="F88" t="s">
-        <v>774</v>
+        <v>769</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -4563,16 +4638,16 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D89" t="s">
-        <v>785</v>
+        <v>780</v>
       </c>
       <c r="E89" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
       <c r="F89" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -4580,16 +4655,16 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D90" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E90" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F90" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -4597,16 +4672,16 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="D91" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="E91" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="F91" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -4614,16 +4689,16 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="D92" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="E92" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="F92" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -4631,16 +4706,16 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D93" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="E93" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="F93" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -4648,16 +4723,16 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
+        <v>558</v>
+      </c>
+      <c r="D94" t="s">
+        <v>559</v>
+      </c>
+      <c r="E94" t="s">
+        <v>560</v>
+      </c>
+      <c r="F94" t="s">
         <v>561</v>
-      </c>
-      <c r="D94" t="s">
-        <v>562</v>
-      </c>
-      <c r="E94" t="s">
-        <v>563</v>
-      </c>
-      <c r="F94" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -4668,13 +4743,13 @@
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D95" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E95" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F95" t="s">
         <v>45</v>
@@ -4688,13 +4763,13 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D96" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E96" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F96" t="s">
         <v>45</v>
@@ -4708,16 +4783,16 @@
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D97" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E97" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F97" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4725,16 +4800,16 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D98" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="E98" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F98" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -4742,16 +4817,16 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D99" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E99" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F99" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -4759,16 +4834,16 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D100" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E100" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="F100" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4776,16 +4851,16 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D101" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E101" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="F101" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4793,16 +4868,16 @@
         <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D102" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E102" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F102" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4810,16 +4885,16 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D103" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E103" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="F103" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4827,16 +4902,16 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D104" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E104" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F104" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4844,19 +4919,19 @@
         <v>10</v>
       </c>
       <c r="B105" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C105" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D105" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="E105" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="F105" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4864,16 +4939,16 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D106" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E106" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F106" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4881,16 +4956,16 @@
         <v>10</v>
       </c>
       <c r="B107" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D107" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="E107" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="F107" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4898,16 +4973,16 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D108" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E108" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="F108" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4915,16 +4990,16 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D109" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
       </c>
       <c r="F109" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4932,16 +5007,16 @@
         <v>10</v>
       </c>
       <c r="B110" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="D110" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="E110" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="F110" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4949,16 +5024,16 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D111" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="E111" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="F111" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4966,16 +5041,16 @@
         <v>10</v>
       </c>
       <c r="B112" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="D112" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="E112" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="F112" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -4983,16 +5058,16 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="D113" t="s">
         <v>279</v>
       </c>
       <c r="E113" t="s">
-        <v>791</v>
+        <v>786</v>
       </c>
       <c r="F113" t="s">
-        <v>790</v>
+        <v>785</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -5000,16 +5075,16 @@
         <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="D114" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="E114" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F114" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -5017,16 +5092,16 @@
         <v>10</v>
       </c>
       <c r="B115" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D115" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="E115" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="F115" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -5034,16 +5109,16 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="D116" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="E116" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="F116" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -5051,16 +5126,16 @@
         <v>10</v>
       </c>
       <c r="B117" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="D117" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="E117" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="F117" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -5068,16 +5143,16 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="D118" t="s">
-        <v>783</v>
+        <v>778</v>
       </c>
       <c r="E118" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="F118" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -5085,16 +5160,16 @@
         <v>10</v>
       </c>
       <c r="B119" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="D119" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="E119" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="F119" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -5102,16 +5177,16 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="D120" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="E120" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F120" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -5119,7 +5194,7 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="D121" s="2">
         <v>0.9</v>
@@ -5136,16 +5211,16 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="D122" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="E122" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="F122" t="s">
-        <v>777</v>
+        <v>772</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -5153,16 +5228,16 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="D123" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
       <c r="E123" t="s">
-        <v>775</v>
+        <v>770</v>
       </c>
       <c r="F123" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -5170,16 +5245,16 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D124" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="E124" t="s">
-        <v>781</v>
+        <v>776</v>
       </c>
       <c r="F124" t="s">
-        <v>782</v>
+        <v>777</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -5187,16 +5262,16 @@
         <v>10</v>
       </c>
       <c r="B125" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="D125" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="E125" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="F125" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -5204,16 +5279,16 @@
         <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="D126" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="E126" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="F126" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -5221,16 +5296,16 @@
         <v>10</v>
       </c>
       <c r="B127" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="D127" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E127" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="F127" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -5238,16 +5313,16 @@
         <v>10</v>
       </c>
       <c r="B128" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="D128" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="E128" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="F128" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -5255,16 +5330,16 @@
         <v>10</v>
       </c>
       <c r="B129" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="D129" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="E129" t="s">
-        <v>758</v>
+        <v>753</v>
       </c>
       <c r="F129" t="s">
-        <v>759</v>
+        <v>754</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -5272,16 +5347,16 @@
         <v>10</v>
       </c>
       <c r="B130" t="s">
-        <v>760</v>
+        <v>755</v>
       </c>
       <c r="D130" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="E130" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
       <c r="F130" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -5289,16 +5364,16 @@
         <v>10</v>
       </c>
       <c r="B131" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="D131" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="E131" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="F131" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -5306,7 +5381,7 @@
         <v>10</v>
       </c>
       <c r="B132" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="D132" s="2">
         <v>0.2</v>
@@ -5323,16 +5398,16 @@
         <v>10</v>
       </c>
       <c r="B133" t="s">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="D133" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="E133" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="F133" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -5340,16 +5415,16 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="D134" t="s">
-        <v>796</v>
+        <v>791</v>
       </c>
       <c r="E134" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
       <c r="F134" t="s">
-        <v>798</v>
+        <v>793</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -5357,16 +5432,16 @@
         <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>811</v>
+        <v>806</v>
       </c>
       <c r="D135" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="E135" t="s">
-        <v>812</v>
+        <v>807</v>
       </c>
       <c r="F135" t="s">
-        <v>813</v>
+        <v>808</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -5374,16 +5449,16 @@
         <v>10</v>
       </c>
       <c r="B136" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="D136" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="E136" t="s">
-        <v>817</v>
+        <v>812</v>
       </c>
       <c r="F136" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -5391,16 +5466,16 @@
         <v>10</v>
       </c>
       <c r="B137" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="D137" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="E137" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="F137" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -5408,16 +5483,16 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="D138" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="E138" t="s">
         <v>41</v>
       </c>
       <c r="F138" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -5425,16 +5500,16 @@
         <v>10</v>
       </c>
       <c r="B139" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="D139" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="E139" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="F139" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -5442,16 +5517,16 @@
         <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="D140" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="E140" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="F140" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -5459,16 +5534,16 @@
         <v>10</v>
       </c>
       <c r="B141" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="D141" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="E141" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="F141" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -5476,16 +5551,16 @@
         <v>10</v>
       </c>
       <c r="B142" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="D142" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="E142" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="F142" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -5493,16 +5568,16 @@
         <v>10</v>
       </c>
       <c r="B143" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="D143" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="E143" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="F143" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -5510,16 +5585,16 @@
         <v>10</v>
       </c>
       <c r="B144" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="D144" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="E144" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="F144" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -5527,16 +5602,16 @@
         <v>10</v>
       </c>
       <c r="B145" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="D145" t="s">
+        <v>845</v>
+      </c>
+      <c r="E145" t="s">
+        <v>846</v>
+      </c>
+      <c r="F145" t="s">
         <v>851</v>
-      </c>
-      <c r="E145" t="s">
-        <v>852</v>
-      </c>
-      <c r="F145" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -5544,16 +5619,16 @@
         <v>10</v>
       </c>
       <c r="B146" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="D146" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="E146" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="F146" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -5561,7 +5636,7 @@
         <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="D147" t="s">
         <v>250</v>
@@ -5570,7 +5645,7 @@
         <v>249</v>
       </c>
       <c r="F147" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -5578,16 +5653,16 @@
         <v>10</v>
       </c>
       <c r="B148" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="D148" t="s">
         <v>250</v>
       </c>
       <c r="E148" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="F148" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5595,16 +5670,16 @@
         <v>10</v>
       </c>
       <c r="B149" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="D149" t="s">
-        <v>865</v>
+        <v>886</v>
       </c>
       <c r="E149" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="F149" t="s">
-        <v>866</v>
+        <v>885</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -5612,13 +5687,13 @@
         <v>10</v>
       </c>
       <c r="B150" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="D150" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="E150" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="F150" t="s">
         <v>249</v>
@@ -5629,13 +5704,13 @@
         <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="D151" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="E151" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="F151" t="s">
         <v>250</v>
@@ -5646,13 +5721,13 @@
         <v>10</v>
       </c>
       <c r="B152" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="D152" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="E152" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="F152" t="s">
         <v>75</v>
@@ -5663,16 +5738,19 @@
         <v>10</v>
       </c>
       <c r="B153" t="s">
-        <v>873</v>
+        <v>8</v>
+      </c>
+      <c r="C153" t="s">
+        <v>876</v>
       </c>
       <c r="D153" t="s">
-        <v>75</v>
+        <v>875</v>
       </c>
       <c r="E153" t="s">
-        <v>871</v>
+        <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>872</v>
+        <v>813</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -5680,61 +5758,16 @@
         <v>10</v>
       </c>
       <c r="B154" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="D154" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E154" t="s">
         <v>250</v>
       </c>
       <c r="F154" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155">
-        <v>10</v>
-      </c>
-      <c r="B155" t="s">
-        <v>875</v>
-      </c>
-      <c r="D155" t="s">
-        <v>876</v>
-      </c>
-      <c r="E155" t="s">
-        <v>630</v>
-      </c>
-      <c r="F155" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="B156" t="s">
-        <v>877</v>
-      </c>
-      <c r="D156" t="s">
-        <v>878</v>
-      </c>
-      <c r="E156" t="s">
-        <v>879</v>
-      </c>
-      <c r="F156" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="B157" t="s">
-        <v>881</v>
-      </c>
-      <c r="D157" t="s">
-        <v>882</v>
-      </c>
-      <c r="E157" t="s">
-        <v>876</v>
-      </c>
-      <c r="F157" t="s">
-        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -5744,10 +5777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5845,7 +5878,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -5984,7 +6017,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -6174,7 +6207,7 @@
         <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="E24" t="s">
         <v>192</v>
@@ -6188,16 +6221,16 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E25" t="s">
         <v>252</v>
       </c>
       <c r="F25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -6222,16 +6255,16 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
+        <v>314</v>
+      </c>
+      <c r="D27" t="s">
         <v>315</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>316</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>317</v>
-      </c>
-      <c r="F27" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -6239,16 +6272,16 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
+        <v>320</v>
+      </c>
+      <c r="D28" t="s">
         <v>321</v>
-      </c>
-      <c r="D28" t="s">
-        <v>322</v>
       </c>
       <c r="E28" t="s">
         <v>193</v>
       </c>
       <c r="F28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -6256,16 +6289,16 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" t="s">
         <v>327</v>
       </c>
-      <c r="D29" t="s">
-        <v>328</v>
-      </c>
       <c r="E29" t="s">
+        <v>324</v>
+      </c>
+      <c r="F29" t="s">
         <v>325</v>
-      </c>
-      <c r="F29" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -6273,16 +6306,16 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
+        <v>328</v>
+      </c>
+      <c r="D30" t="s">
         <v>329</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>330</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>331</v>
-      </c>
-      <c r="F30" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -6290,16 +6323,16 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D31" t="s">
+        <v>332</v>
+      </c>
+      <c r="E31" t="s">
         <v>333</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>334</v>
-      </c>
-      <c r="F31" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -6307,16 +6340,16 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
+        <v>338</v>
+      </c>
+      <c r="D32" t="s">
+        <v>336</v>
+      </c>
+      <c r="E32" t="s">
+        <v>337</v>
+      </c>
+      <c r="F32" t="s">
         <v>339</v>
-      </c>
-      <c r="D32" t="s">
-        <v>337</v>
-      </c>
-      <c r="E32" t="s">
-        <v>338</v>
-      </c>
-      <c r="F32" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -6324,7 +6357,7 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -6341,16 +6374,16 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
+        <v>358</v>
+      </c>
+      <c r="D34" t="s">
         <v>359</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>360</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>361</v>
-      </c>
-      <c r="F34" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -6361,16 +6394,16 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
+        <v>377</v>
+      </c>
+      <c r="D35" t="s">
         <v>378</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>379</v>
       </c>
-      <c r="E35" t="s">
-        <v>380</v>
-      </c>
       <c r="F35" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -6378,16 +6411,16 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
+        <v>384</v>
+      </c>
+      <c r="D36" t="s">
         <v>385</v>
       </c>
-      <c r="D36" t="s">
-        <v>386</v>
-      </c>
       <c r="E36" t="s">
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -6398,16 +6431,16 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F37" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -6415,16 +6448,16 @@
         <v>15</v>
       </c>
       <c r="B38" t="s">
+        <v>487</v>
+      </c>
+      <c r="D38" t="s">
         <v>490</v>
       </c>
-      <c r="D38" t="s">
-        <v>493</v>
-      </c>
       <c r="E38" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F38" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -6432,7 +6465,7 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="D39">
         <v>1998</v>
@@ -6449,16 +6482,16 @@
         <v>15</v>
       </c>
       <c r="B40" t="s">
+        <v>405</v>
+      </c>
+      <c r="D40" t="s">
+        <v>404</v>
+      </c>
+      <c r="E40" t="s">
+        <v>406</v>
+      </c>
+      <c r="F40" t="s">
         <v>407</v>
-      </c>
-      <c r="D40" t="s">
-        <v>406</v>
-      </c>
-      <c r="E40" t="s">
-        <v>408</v>
-      </c>
-      <c r="F40" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -6466,16 +6499,16 @@
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D41" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="E41" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="F41" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -6483,16 +6516,16 @@
         <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D42" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E42" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F42" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -6500,16 +6533,16 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D43" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E43" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F43" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -6517,16 +6550,16 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D44" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E44" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F44" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -6534,16 +6567,16 @@
         <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D45" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="E45" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="F45" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6551,16 +6584,16 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="D46" t="s">
-        <v>799</v>
+        <v>794</v>
       </c>
       <c r="E46" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="F46" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6571,16 +6604,16 @@
         <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D47" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E47" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F47" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -6588,16 +6621,16 @@
         <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D48" t="s">
         <v>138</v>
       </c>
       <c r="E48" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F48" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -6605,16 +6638,16 @@
         <v>15</v>
       </c>
       <c r="B49" t="s">
+        <v>460</v>
+      </c>
+      <c r="D49" t="s">
+        <v>461</v>
+      </c>
+      <c r="E49" t="s">
+        <v>462</v>
+      </c>
+      <c r="F49" t="s">
         <v>463</v>
-      </c>
-      <c r="D49" t="s">
-        <v>464</v>
-      </c>
-      <c r="E49" t="s">
-        <v>465</v>
-      </c>
-      <c r="F49" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -6622,16 +6655,16 @@
         <v>15</v>
       </c>
       <c r="B50" t="s">
+        <v>468</v>
+      </c>
+      <c r="D50" t="s">
+        <v>469</v>
+      </c>
+      <c r="E50" t="s">
+        <v>470</v>
+      </c>
+      <c r="F50" t="s">
         <v>471</v>
-      </c>
-      <c r="D50" t="s">
-        <v>472</v>
-      </c>
-      <c r="E50" t="s">
-        <v>473</v>
-      </c>
-      <c r="F50" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -6639,16 +6672,16 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D51" t="s">
+        <v>511</v>
+      </c>
+      <c r="E51" t="s">
+        <v>512</v>
+      </c>
+      <c r="F51" t="s">
         <v>514</v>
-      </c>
-      <c r="E51" t="s">
-        <v>515</v>
-      </c>
-      <c r="F51" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -6656,16 +6689,16 @@
         <v>15</v>
       </c>
       <c r="B52" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D52" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="E52" t="s">
+        <v>500</v>
+      </c>
+      <c r="F52" t="s">
         <v>503</v>
-      </c>
-      <c r="F52" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -6673,16 +6706,16 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="D53" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="E53" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="F53" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6693,16 +6726,16 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D54" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E54" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F54" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6713,16 +6746,16 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D55" t="s">
+        <v>550</v>
+      </c>
+      <c r="E55" t="s">
+        <v>551</v>
+      </c>
+      <c r="F55" t="s">
         <v>553</v>
-      </c>
-      <c r="E55" t="s">
-        <v>554</v>
-      </c>
-      <c r="F55" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6730,16 +6763,16 @@
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D56" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="E56" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="F56" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6747,16 +6780,16 @@
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D57" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="E57" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="F57" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6764,16 +6797,16 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D58" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="E58" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="F58" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6781,16 +6814,16 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D59" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="E59" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="F59" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6798,16 +6831,16 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="D60" t="s">
-        <v>807</v>
+        <v>802</v>
       </c>
       <c r="E60" t="s">
-        <v>808</v>
+        <v>803</v>
       </c>
       <c r="F60" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6815,16 +6848,16 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D61" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="E61" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="F61" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6832,16 +6865,16 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="D62" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="E62" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="F62" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -6849,10 +6882,10 @@
         <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D63" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="E63" t="s">
         <v>91</v>
@@ -6866,7 +6899,7 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="D64">
         <v>2007</v>
@@ -6883,16 +6916,16 @@
         <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="D65" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="E65" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="F65" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6900,16 +6933,16 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="D66" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="E66" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="F66" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -6917,16 +6950,16 @@
         <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="D67" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="E67" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="F67" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6934,26 +6967,104 @@
         <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="D68" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="E68" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="F68" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
     </row>
     <row r="69" spans="1:6">
+      <c r="A69">
+        <v>15</v>
+      </c>
       <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>877</v>
+      </c>
+      <c r="D69" t="s">
+        <v>813</v>
+      </c>
+      <c r="E69" t="s">
         <v>818</v>
       </c>
+      <c r="F69" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="70" spans="1:6">
+      <c r="A70">
+        <v>15</v>
+      </c>
       <c r="B70" t="s">
-        <v>819</v>
+        <v>881</v>
+      </c>
+      <c r="D70" t="s">
+        <v>882</v>
+      </c>
+      <c r="E70" t="s">
+        <v>883</v>
+      </c>
+      <c r="F70" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>15</v>
+      </c>
+      <c r="B71" t="s">
+        <v>867</v>
+      </c>
+      <c r="D71" t="s">
+        <v>868</v>
+      </c>
+      <c r="E71" t="s">
+        <v>626</v>
+      </c>
+      <c r="F71" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="B72" t="s">
+        <v>865</v>
+      </c>
+      <c r="D72" t="s">
+        <v>75</v>
+      </c>
+      <c r="E72" t="s">
+        <v>863</v>
+      </c>
+      <c r="F72" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>15</v>
+      </c>
+      <c r="B73" t="s">
+        <v>899</v>
+      </c>
+      <c r="D73" t="s">
+        <v>900</v>
+      </c>
+      <c r="E73" t="s">
+        <v>897</v>
+      </c>
+      <c r="F73" t="s">
+        <v>898</v>
       </c>
     </row>
   </sheetData>
@@ -6963,10 +7074,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7126,7 +7237,7 @@
         <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="E9" t="s">
         <v>222</v>
@@ -7174,10 +7285,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D12" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="E12" t="s">
         <v>242</v>
@@ -7191,16 +7302,16 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E13" t="s">
         <v>312</v>
       </c>
-      <c r="D13" t="s">
-        <v>311</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>313</v>
-      </c>
-      <c r="F13" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -7208,16 +7319,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E14" t="s">
         <v>366</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>367</v>
-      </c>
-      <c r="F14" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -7225,7 +7336,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>402</v>
+        <v>891</v>
+      </c>
+      <c r="D15" t="s">
+        <v>892</v>
+      </c>
+      <c r="E15" t="s">
+        <v>893</v>
+      </c>
+      <c r="F15" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7233,7 +7353,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>410</v>
+        <v>806</v>
+      </c>
+      <c r="D16" t="s">
+        <v>805</v>
+      </c>
+      <c r="E16" t="s">
+        <v>895</v>
+      </c>
+      <c r="F16" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -7241,16 +7370,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D17" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="E17" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="F17" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7258,16 +7387,16 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D18" t="s">
+        <v>446</v>
+      </c>
+      <c r="E18" t="s">
+        <v>447</v>
+      </c>
+      <c r="F18" t="s">
         <v>449</v>
-      </c>
-      <c r="E18" t="s">
-        <v>450</v>
-      </c>
-      <c r="F18" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -7275,16 +7404,16 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D19" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="E19" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F19" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -7292,16 +7421,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D20" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E20" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F20" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -7309,16 +7438,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D21" t="s">
+        <v>397</v>
+      </c>
+      <c r="E21" t="s">
         <v>398</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>399</v>
-      </c>
-      <c r="F21" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -7326,16 +7455,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D22" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E22" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="F22" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -7346,16 +7475,16 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
+        <v>456</v>
+      </c>
+      <c r="D23" t="s">
+        <v>457</v>
+      </c>
+      <c r="E23" t="s">
+        <v>458</v>
+      </c>
+      <c r="F23" t="s">
         <v>459</v>
-      </c>
-      <c r="D23" t="s">
-        <v>460</v>
-      </c>
-      <c r="E23" t="s">
-        <v>461</v>
-      </c>
-      <c r="F23" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -7363,16 +7492,16 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
+        <v>464</v>
+      </c>
+      <c r="D24" t="s">
+        <v>465</v>
+      </c>
+      <c r="E24" t="s">
+        <v>466</v>
+      </c>
+      <c r="F24" t="s">
         <v>467</v>
-      </c>
-      <c r="D24" t="s">
-        <v>468</v>
-      </c>
-      <c r="E24" t="s">
-        <v>469</v>
-      </c>
-      <c r="F24" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -7380,16 +7509,16 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
+        <v>483</v>
+      </c>
+      <c r="D25" t="s">
+        <v>484</v>
+      </c>
+      <c r="E25" t="s">
+        <v>485</v>
+      </c>
+      <c r="F25" t="s">
         <v>486</v>
-      </c>
-      <c r="D25" t="s">
-        <v>487</v>
-      </c>
-      <c r="E25" t="s">
-        <v>488</v>
-      </c>
-      <c r="F25" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -7397,7 +7526,16 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>565</v>
+        <v>901</v>
+      </c>
+      <c r="D26" t="s">
+        <v>902</v>
+      </c>
+      <c r="E26" t="s">
+        <v>903</v>
+      </c>
+      <c r="F26" t="s">
+        <v>904</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7405,16 +7543,16 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D27" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E27" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="F27" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7422,16 +7560,16 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="D28" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="E28" t="s">
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7439,7 +7577,16 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>632</v>
+        <v>887</v>
+      </c>
+      <c r="D29" t="s">
+        <v>888</v>
+      </c>
+      <c r="E29" t="s">
+        <v>889</v>
+      </c>
+      <c r="F29" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -7447,7 +7594,70 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>784</v>
+        <v>779</v>
+      </c>
+      <c r="D30">
+        <v>31.1</v>
+      </c>
+      <c r="E30">
+        <v>28.35</v>
+      </c>
+      <c r="F30">
+        <v>33.14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>879</v>
+      </c>
+      <c r="D31" t="s">
+        <v>880</v>
+      </c>
+      <c r="E31" t="s">
+        <v>813</v>
+      </c>
+      <c r="F31" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>873</v>
+      </c>
+      <c r="D32" t="s">
+        <v>874</v>
+      </c>
+      <c r="E32" t="s">
+        <v>868</v>
+      </c>
+      <c r="F32" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>869</v>
+      </c>
+      <c r="D33" t="s">
+        <v>870</v>
+      </c>
+      <c r="E33" t="s">
+        <v>871</v>
+      </c>
+      <c r="F33" t="s">
+        <v>872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections to the questions.
Adjustments to the interface so it also blinks when timer ends.

VerticalTextView class added to signal the ad banners when in the
transition layer (also added its style).

Unused imports removed.
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="908">
   <si>
     <t>Difficulty</t>
   </si>
@@ -1644,15 +1644,9 @@
     <t>A coin made of two bits</t>
   </si>
   <si>
-    <t>Papandeou</t>
-  </si>
-  <si>
     <t>papandeou1</t>
   </si>
   <si>
-    <t>Papademos</t>
-  </si>
-  <si>
     <t>lagarde1</t>
   </si>
   <si>
@@ -1677,9 +1671,6 @@
     <t>barroso1</t>
   </si>
   <si>
-    <t>Durao-Barroso</t>
-  </si>
-  <si>
     <t>What is the SEC?</t>
   </si>
   <si>
@@ -2109,9 +2100,6 @@
     <t>British Northern Rock</t>
   </si>
   <si>
-    <t>French Societé Generale</t>
-  </si>
-  <si>
     <t>American Goldman Sachs</t>
   </si>
   <si>
@@ -2538,9 +2526,6 @@
     <t>In New York City and priced in dollars</t>
   </si>
   <si>
-    <t>What can I pick up in Cushing, Ocklahoma?</t>
-  </si>
-  <si>
     <t>WTI barrels</t>
   </si>
   <si>
@@ -2737,6 +2722,24 @@
   </si>
   <si>
     <t>reales1</t>
+  </si>
+  <si>
+    <t>French Societe Generale</t>
+  </si>
+  <si>
+    <t>Jose M. Durao-Barroso</t>
+  </si>
+  <si>
+    <t>Lukanikos Papademos</t>
+  </si>
+  <si>
+    <t>Georgios Papandeou</t>
+  </si>
+  <si>
+    <t>J. M. Durao-Barroso</t>
+  </si>
+  <si>
+    <t>What can I pick up in Cushing, Oklahoma?</t>
   </si>
 </sst>
 </file>
@@ -3072,8 +3075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3637,7 +3640,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D31" t="s">
         <v>372</v>
@@ -3929,7 +3932,7 @@
         <v>285</v>
       </c>
       <c r="C48" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="D48" t="s">
         <v>287</v>
@@ -3983,7 +3986,7 @@
         <v>297</v>
       </c>
       <c r="D51" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="E51" t="s">
         <v>298</v>
@@ -4000,10 +4003,10 @@
         <v>300</v>
       </c>
       <c r="D52" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E52" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F52" t="s">
         <v>301</v>
@@ -4230,7 +4233,7 @@
         <v>400</v>
       </c>
       <c r="E65" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="F65" t="s">
         <v>422</v>
@@ -4366,13 +4369,13 @@
         <v>433</v>
       </c>
       <c r="D73" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="E73" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="F73" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4420,13 +4423,13 @@
         <v>498</v>
       </c>
       <c r="D76" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="E76" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="F76" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4437,13 +4440,13 @@
         <v>497</v>
       </c>
       <c r="D77" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="E77" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="F77" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4494,7 +4497,7 @@
         <v>501</v>
       </c>
       <c r="F80" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4502,16 +4505,16 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="D81" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="E81" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="F81" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4519,16 +4522,16 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
+        <v>637</v>
+      </c>
+      <c r="D82" t="s">
+        <v>638</v>
+      </c>
+      <c r="E82" t="s">
+        <v>639</v>
+      </c>
+      <c r="F82" t="s">
         <v>640</v>
-      </c>
-      <c r="D82" t="s">
-        <v>641</v>
-      </c>
-      <c r="E82" t="s">
-        <v>642</v>
-      </c>
-      <c r="F82" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4542,10 +4545,10 @@
         <v>518</v>
       </c>
       <c r="E83" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="F83" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -4590,13 +4593,13 @@
         <v>520</v>
       </c>
       <c r="D86" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="E86" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="F86" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -4624,13 +4627,13 @@
         <v>526</v>
       </c>
       <c r="D88" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="E88" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="F88" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -4641,13 +4644,13 @@
         <v>525</v>
       </c>
       <c r="D89" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="E89" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="F89" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -4664,7 +4667,7 @@
         <v>516</v>
       </c>
       <c r="F90" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -4672,16 +4675,16 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="D91" t="s">
+        <v>707</v>
+      </c>
+      <c r="E91" t="s">
+        <v>709</v>
+      </c>
+      <c r="F91" t="s">
         <v>711</v>
-      </c>
-      <c r="E91" t="s">
-        <v>713</v>
-      </c>
-      <c r="F91" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -4689,16 +4692,16 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="D92" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="E92" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="F92" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -4706,13 +4709,13 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D93" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="E93" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="F93" t="s">
         <v>446</v>
@@ -4723,16 +4726,16 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
+        <v>555</v>
+      </c>
+      <c r="D94" t="s">
+        <v>556</v>
+      </c>
+      <c r="E94" t="s">
+        <v>557</v>
+      </c>
+      <c r="F94" t="s">
         <v>558</v>
-      </c>
-      <c r="D94" t="s">
-        <v>559</v>
-      </c>
-      <c r="E94" t="s">
-        <v>560</v>
-      </c>
-      <c r="F94" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -4743,13 +4746,13 @@
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D95" t="s">
-        <v>542</v>
+        <v>905</v>
       </c>
       <c r="E95" t="s">
-        <v>544</v>
+        <v>906</v>
       </c>
       <c r="F95" t="s">
         <v>45</v>
@@ -4763,13 +4766,13 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D96" t="s">
-        <v>553</v>
+        <v>903</v>
       </c>
       <c r="E96" t="s">
-        <v>544</v>
+        <v>904</v>
       </c>
       <c r="F96" t="s">
         <v>45</v>
@@ -4783,16 +4786,16 @@
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D97" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E97" t="s">
         <v>501</v>
       </c>
       <c r="F97" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4800,16 +4803,16 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D98" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="E98" t="s">
         <v>446</v>
       </c>
       <c r="F98" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -4817,16 +4820,16 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D99" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E99" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F99" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -4834,16 +4837,16 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
+        <v>567</v>
+      </c>
+      <c r="D100" t="s">
+        <v>568</v>
+      </c>
+      <c r="E100" t="s">
+        <v>569</v>
+      </c>
+      <c r="F100" t="s">
         <v>570</v>
-      </c>
-      <c r="D100" t="s">
-        <v>571</v>
-      </c>
-      <c r="E100" t="s">
-        <v>572</v>
-      </c>
-      <c r="F100" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4851,16 +4854,16 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
+        <v>575</v>
+      </c>
+      <c r="D101" t="s">
+        <v>576</v>
+      </c>
+      <c r="E101" t="s">
+        <v>577</v>
+      </c>
+      <c r="F101" t="s">
         <v>578</v>
-      </c>
-      <c r="D101" t="s">
-        <v>579</v>
-      </c>
-      <c r="E101" t="s">
-        <v>580</v>
-      </c>
-      <c r="F101" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4868,16 +4871,16 @@
         <v>10</v>
       </c>
       <c r="B102" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D102" t="s">
+        <v>579</v>
+      </c>
+      <c r="E102" t="s">
+        <v>581</v>
+      </c>
+      <c r="F102" t="s">
         <v>582</v>
-      </c>
-      <c r="E102" t="s">
-        <v>584</v>
-      </c>
-      <c r="F102" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4885,16 +4888,16 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
+        <v>588</v>
+      </c>
+      <c r="D103" t="s">
+        <v>589</v>
+      </c>
+      <c r="E103" t="s">
+        <v>590</v>
+      </c>
+      <c r="F103" t="s">
         <v>591</v>
-      </c>
-      <c r="D103" t="s">
-        <v>592</v>
-      </c>
-      <c r="E103" t="s">
-        <v>593</v>
-      </c>
-      <c r="F103" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4902,16 +4905,16 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D104" t="s">
+        <v>594</v>
+      </c>
+      <c r="E104" t="s">
+        <v>596</v>
+      </c>
+      <c r="F104" t="s">
         <v>597</v>
-      </c>
-      <c r="E104" t="s">
-        <v>599</v>
-      </c>
-      <c r="F104" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4919,19 +4922,19 @@
         <v>10</v>
       </c>
       <c r="B105" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C105" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D105" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E105" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F105" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4939,16 +4942,16 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
+        <v>600</v>
+      </c>
+      <c r="D106" t="s">
+        <v>601</v>
+      </c>
+      <c r="E106" t="s">
+        <v>602</v>
+      </c>
+      <c r="F106" t="s">
         <v>603</v>
-      </c>
-      <c r="D106" t="s">
-        <v>604</v>
-      </c>
-      <c r="E106" t="s">
-        <v>605</v>
-      </c>
-      <c r="F106" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4956,16 +4959,16 @@
         <v>10</v>
       </c>
       <c r="B107" t="s">
+        <v>606</v>
+      </c>
+      <c r="D107" t="s">
+        <v>607</v>
+      </c>
+      <c r="E107" t="s">
+        <v>608</v>
+      </c>
+      <c r="F107" t="s">
         <v>609</v>
-      </c>
-      <c r="D107" t="s">
-        <v>610</v>
-      </c>
-      <c r="E107" t="s">
-        <v>611</v>
-      </c>
-      <c r="F107" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4973,16 +4976,16 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
+        <v>618</v>
+      </c>
+      <c r="D108" t="s">
+        <v>619</v>
+      </c>
+      <c r="E108" t="s">
+        <v>620</v>
+      </c>
+      <c r="F108" t="s">
         <v>621</v>
-      </c>
-      <c r="D108" t="s">
-        <v>622</v>
-      </c>
-      <c r="E108" t="s">
-        <v>623</v>
-      </c>
-      <c r="F108" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4990,16 +4993,16 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D109" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
       </c>
       <c r="F109" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -5007,16 +5010,16 @@
         <v>10</v>
       </c>
       <c r="B110" t="s">
+        <v>688</v>
+      </c>
+      <c r="D110" t="s">
+        <v>689</v>
+      </c>
+      <c r="E110" t="s">
+        <v>690</v>
+      </c>
+      <c r="F110" t="s">
         <v>691</v>
-      </c>
-      <c r="D110" t="s">
-        <v>692</v>
-      </c>
-      <c r="E110" t="s">
-        <v>693</v>
-      </c>
-      <c r="F110" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -5024,16 +5027,16 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
+        <v>641</v>
+      </c>
+      <c r="D111" t="s">
+        <v>642</v>
+      </c>
+      <c r="E111" t="s">
+        <v>643</v>
+      </c>
+      <c r="F111" t="s">
         <v>644</v>
-      </c>
-      <c r="D111" t="s">
-        <v>645</v>
-      </c>
-      <c r="E111" t="s">
-        <v>646</v>
-      </c>
-      <c r="F111" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -5041,16 +5044,16 @@
         <v>10</v>
       </c>
       <c r="B112" t="s">
+        <v>625</v>
+      </c>
+      <c r="D112" t="s">
+        <v>626</v>
+      </c>
+      <c r="E112" t="s">
         <v>628</v>
       </c>
-      <c r="D112" t="s">
-        <v>629</v>
-      </c>
-      <c r="E112" t="s">
-        <v>631</v>
-      </c>
       <c r="F112" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -5058,16 +5061,16 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="D113" t="s">
         <v>279</v>
       </c>
       <c r="E113" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="F113" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -5075,16 +5078,16 @@
         <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D114" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E114" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="F114" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -5092,16 +5095,16 @@
         <v>10</v>
       </c>
       <c r="B115" t="s">
+        <v>654</v>
+      </c>
+      <c r="D115" t="s">
+        <v>655</v>
+      </c>
+      <c r="E115" t="s">
+        <v>656</v>
+      </c>
+      <c r="F115" t="s">
         <v>657</v>
-      </c>
-      <c r="D115" t="s">
-        <v>658</v>
-      </c>
-      <c r="E115" t="s">
-        <v>659</v>
-      </c>
-      <c r="F115" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -5109,16 +5112,16 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
+        <v>658</v>
+      </c>
+      <c r="D116" t="s">
+        <v>659</v>
+      </c>
+      <c r="E116" t="s">
+        <v>660</v>
+      </c>
+      <c r="F116" t="s">
         <v>661</v>
-      </c>
-      <c r="D116" t="s">
-        <v>662</v>
-      </c>
-      <c r="E116" t="s">
-        <v>663</v>
-      </c>
-      <c r="F116" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -5126,16 +5129,16 @@
         <v>10</v>
       </c>
       <c r="B117" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D117" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="E117" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="F117" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -5143,16 +5146,16 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D118" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="E118" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="F118" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -5160,16 +5163,16 @@
         <v>10</v>
       </c>
       <c r="B119" t="s">
+        <v>666</v>
+      </c>
+      <c r="D119" t="s">
+        <v>667</v>
+      </c>
+      <c r="E119" t="s">
+        <v>668</v>
+      </c>
+      <c r="F119" t="s">
         <v>669</v>
-      </c>
-      <c r="D119" t="s">
-        <v>670</v>
-      </c>
-      <c r="E119" t="s">
-        <v>671</v>
-      </c>
-      <c r="F119" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -5177,16 +5180,16 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D120" t="s">
+        <v>670</v>
+      </c>
+      <c r="E120" t="s">
+        <v>671</v>
+      </c>
+      <c r="F120" t="s">
         <v>673</v>
-      </c>
-      <c r="E120" t="s">
-        <v>674</v>
-      </c>
-      <c r="F120" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -5194,7 +5197,7 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="D121" s="2">
         <v>0.9</v>
@@ -5211,16 +5214,16 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D122" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="E122" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F122" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -5228,16 +5231,16 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D123" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="E123" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="F123" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -5245,16 +5248,16 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D124" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="E124" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F124" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -5262,16 +5265,16 @@
         <v>10</v>
       </c>
       <c r="B125" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="D125" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="E125" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="F125" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -5279,16 +5282,16 @@
         <v>10</v>
       </c>
       <c r="B126" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D126" t="s">
+        <v>679</v>
+      </c>
+      <c r="E126" t="s">
+        <v>681</v>
+      </c>
+      <c r="F126" t="s">
         <v>682</v>
-      </c>
-      <c r="E126" t="s">
-        <v>684</v>
-      </c>
-      <c r="F126" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -5296,16 +5299,16 @@
         <v>10</v>
       </c>
       <c r="B127" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="D127" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E127" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="F127" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -5313,16 +5316,16 @@
         <v>10</v>
       </c>
       <c r="B128" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="D128" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="E128" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="F128" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -5330,16 +5333,16 @@
         <v>10</v>
       </c>
       <c r="B129" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="D129" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="E129" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="F129" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -5347,16 +5350,16 @@
         <v>10</v>
       </c>
       <c r="B130" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D130" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="E130" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="F130" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -5364,16 +5367,16 @@
         <v>10</v>
       </c>
       <c r="B131" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="D131" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="E131" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F131" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -5381,7 +5384,7 @@
         <v>10</v>
       </c>
       <c r="B132" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="D132" s="2">
         <v>0.2</v>
@@ -5398,16 +5401,16 @@
         <v>10</v>
       </c>
       <c r="B133" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="D133" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="E133" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="F133" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -5415,16 +5418,16 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="D134" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="E134" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="F134" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -5432,16 +5435,16 @@
         <v>10</v>
       </c>
       <c r="B135" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D135" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="E135" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="F135" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -5449,16 +5452,16 @@
         <v>10</v>
       </c>
       <c r="B136" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="D136" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="E136" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="F136" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -5466,16 +5469,16 @@
         <v>10</v>
       </c>
       <c r="B137" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="D137" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="E137" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="F137" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -5483,10 +5486,10 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="D138" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="E138" t="s">
         <v>41</v>
@@ -5500,16 +5503,16 @@
         <v>10</v>
       </c>
       <c r="B139" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="D139" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="E139" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="F139" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -5517,16 +5520,16 @@
         <v>10</v>
       </c>
       <c r="B140" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D140" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="E140" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="F140" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -5534,16 +5537,16 @@
         <v>10</v>
       </c>
       <c r="B141" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="D141" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="E141" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="F141" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -5551,16 +5554,16 @@
         <v>10</v>
       </c>
       <c r="B142" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="D142" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="E142" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="F142" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -5568,16 +5571,16 @@
         <v>10</v>
       </c>
       <c r="B143" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="D143" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="E143" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="F143" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -5585,16 +5588,16 @@
         <v>10</v>
       </c>
       <c r="B144" t="s">
-        <v>840</v>
+        <v>907</v>
       </c>
       <c r="D144" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="E144" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="F144" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -5602,16 +5605,16 @@
         <v>10</v>
       </c>
       <c r="B145" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="D145" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="E145" t="s">
+        <v>841</v>
+      </c>
+      <c r="F145" t="s">
         <v>846</v>
-      </c>
-      <c r="F145" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -5619,16 +5622,16 @@
         <v>10</v>
       </c>
       <c r="B146" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="D146" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="E146" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="F146" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -5636,7 +5639,7 @@
         <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
       <c r="D147" t="s">
         <v>250</v>
@@ -5645,7 +5648,7 @@
         <v>249</v>
       </c>
       <c r="F147" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -5653,16 +5656,16 @@
         <v>10</v>
       </c>
       <c r="B148" t="s">
-        <v>855</v>
+        <v>850</v>
       </c>
       <c r="D148" t="s">
         <v>250</v>
       </c>
       <c r="E148" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="F148" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5670,16 +5673,16 @@
         <v>10</v>
       </c>
       <c r="B149" t="s">
-        <v>858</v>
+        <v>853</v>
       </c>
       <c r="D149" t="s">
-        <v>886</v>
+        <v>881</v>
       </c>
       <c r="E149" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="F149" t="s">
-        <v>885</v>
+        <v>880</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -5687,13 +5690,13 @@
         <v>10</v>
       </c>
       <c r="B150" t="s">
-        <v>859</v>
+        <v>854</v>
       </c>
       <c r="D150" t="s">
-        <v>860</v>
+        <v>855</v>
       </c>
       <c r="E150" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="F150" t="s">
         <v>249</v>
@@ -5704,13 +5707,13 @@
         <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="D151" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
       <c r="E151" t="s">
-        <v>856</v>
+        <v>851</v>
       </c>
       <c r="F151" t="s">
         <v>250</v>
@@ -5721,13 +5724,13 @@
         <v>10</v>
       </c>
       <c r="B152" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="D152" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="E152" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="F152" t="s">
         <v>75</v>
@@ -5741,16 +5744,16 @@
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="D153" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="E153" t="s">
         <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -5758,10 +5761,10 @@
         <v>10</v>
       </c>
       <c r="B154" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="D154" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E154" t="s">
         <v>250</v>
@@ -5779,8 +5782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6207,7 +6210,7 @@
         <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E24" t="s">
         <v>192</v>
@@ -6221,7 +6224,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D25" t="s">
         <v>318</v>
@@ -6465,7 +6468,7 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D39">
         <v>1998</v>
@@ -6570,13 +6573,13 @@
         <v>434</v>
       </c>
       <c r="D45" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="E45" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="F45" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6584,16 +6587,16 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="D46" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="E46" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="F46" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6706,16 +6709,16 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D53" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="E53" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="F53" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6726,16 +6729,16 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D54" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E54" t="s">
         <v>501</v>
       </c>
       <c r="F54" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6746,16 +6749,16 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
+        <v>547</v>
+      </c>
+      <c r="D55" t="s">
+        <v>548</v>
+      </c>
+      <c r="E55" t="s">
         <v>549</v>
       </c>
-      <c r="D55" t="s">
-        <v>550</v>
-      </c>
-      <c r="E55" t="s">
-        <v>551</v>
-      </c>
       <c r="F55" t="s">
-        <v>553</v>
+        <v>903</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6763,16 +6766,16 @@
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D56" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E56" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F56" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6780,16 +6783,16 @@
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D57" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="E57" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="F57" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6797,16 +6800,16 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D58" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="E58" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F58" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6814,16 +6817,16 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
+        <v>614</v>
+      </c>
+      <c r="D59" t="s">
+        <v>615</v>
+      </c>
+      <c r="E59" t="s">
+        <v>616</v>
+      </c>
+      <c r="F59" t="s">
         <v>617</v>
-      </c>
-      <c r="D59" t="s">
-        <v>618</v>
-      </c>
-      <c r="E59" t="s">
-        <v>619</v>
-      </c>
-      <c r="F59" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6831,16 +6834,16 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="D60" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="E60" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="F60" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6848,16 +6851,16 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
+        <v>629</v>
+      </c>
+      <c r="D61" t="s">
+        <v>630</v>
+      </c>
+      <c r="E61" t="s">
+        <v>631</v>
+      </c>
+      <c r="F61" t="s">
         <v>632</v>
-      </c>
-      <c r="D61" t="s">
-        <v>633</v>
-      </c>
-      <c r="E61" t="s">
-        <v>634</v>
-      </c>
-      <c r="F61" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6865,16 +6868,16 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
+        <v>645</v>
+      </c>
+      <c r="D62" t="s">
+        <v>646</v>
+      </c>
+      <c r="E62" t="s">
+        <v>647</v>
+      </c>
+      <c r="F62" t="s">
         <v>648</v>
-      </c>
-      <c r="D62" t="s">
-        <v>649</v>
-      </c>
-      <c r="E62" t="s">
-        <v>650</v>
-      </c>
-      <c r="F62" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -6882,10 +6885,10 @@
         <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D63" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="E63" t="s">
         <v>91</v>
@@ -6899,7 +6902,7 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D64">
         <v>2007</v>
@@ -6916,16 +6919,16 @@
         <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D65" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="E65" t="s">
-        <v>697</v>
+        <v>902</v>
       </c>
       <c r="F65" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6933,16 +6936,16 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D66" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="E66" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="F66" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -6950,16 +6953,16 @@
         <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="D67" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="E67" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="F67" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6967,16 +6970,16 @@
         <v>15</v>
       </c>
       <c r="B68" t="s">
+        <v>684</v>
+      </c>
+      <c r="D68" t="s">
+        <v>685</v>
+      </c>
+      <c r="E68" t="s">
+        <v>686</v>
+      </c>
+      <c r="F68" t="s">
         <v>687</v>
-      </c>
-      <c r="D68" t="s">
-        <v>688</v>
-      </c>
-      <c r="E68" t="s">
-        <v>689</v>
-      </c>
-      <c r="F68" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -6987,16 +6990,16 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="D69" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="E69" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="F69" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -7004,16 +7007,16 @@
         <v>15</v>
       </c>
       <c r="B70" t="s">
-        <v>881</v>
+        <v>876</v>
       </c>
       <c r="D70" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="E70" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="F70" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -7021,16 +7024,16 @@
         <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="D71" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="E71" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F71" t="s">
-        <v>857</v>
+        <v>852</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -7038,16 +7041,16 @@
         <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="D72" t="s">
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="F72" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -7055,16 +7058,16 @@
         <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="D73" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="E73" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="F73" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
     </row>
   </sheetData>
@@ -7237,7 +7240,7 @@
         <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="E9" t="s">
         <v>222</v>
@@ -7336,16 +7339,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>891</v>
+        <v>886</v>
       </c>
       <c r="D15" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="E15" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="F15" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7353,16 +7356,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="D16" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="E16" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="F16" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -7373,13 +7376,13 @@
         <v>402</v>
       </c>
       <c r="D17" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E17" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F17" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7438,7 +7441,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D21" t="s">
         <v>397</v>
@@ -7455,7 +7458,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D22" t="s">
         <v>453</v>
@@ -7526,16 +7529,16 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="D26" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
       <c r="E26" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="F26" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7543,7 +7546,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D27" t="s">
         <v>501</v>
@@ -7552,7 +7555,7 @@
         <v>502</v>
       </c>
       <c r="F27" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7560,7 +7563,7 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D28" t="s">
         <v>501</v>
@@ -7569,7 +7572,7 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7577,16 +7580,16 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="D29" t="s">
-        <v>888</v>
+        <v>883</v>
       </c>
       <c r="E29" t="s">
-        <v>889</v>
+        <v>884</v>
       </c>
       <c r="F29" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -7594,7 +7597,7 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="D30">
         <v>31.1</v>
@@ -7614,13 +7617,13 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="D31" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="E31" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="F31" t="s">
         <v>394</v>
@@ -7631,16 +7634,16 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="D32" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="E32" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="F32" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -7648,16 +7651,16 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="D33" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="E33" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="F33" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed MoPub stuff and added AdMob libraries.
Fixed some issues with the gameover and congratulation screens.

Changed the papandreou png name, which was not appearing.

Fixed some questions.
</commit_message>
<xml_diff>
--- a/CrisisTrivia/qa.xlsx
+++ b/CrisisTrivia/qa.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="907">
   <si>
     <t>Difficulty</t>
   </si>
@@ -1548,9 +1548,6 @@
     <t>Which bank was the target of the 2010 Max Kaiser's campaign?</t>
   </si>
   <si>
-    <t>Scotia Moccata</t>
-  </si>
-  <si>
     <t>A trader buys cattle futures and forgets to close its position so he has to go and feed the cattle himself</t>
   </si>
   <si>
@@ -2589,9 +2586,6 @@
     <t>Who said "If congress has the right under the Constitution to issue paper money, it was  given them to use themselves, not to be delegated to individuals or corporations"?</t>
   </si>
   <si>
-    <t>The words "I am a most unhappy man. I have unwittingly ruined my country…" were written by. . .</t>
-  </si>
-  <si>
     <t>Woodrow Wilson</t>
   </si>
   <si>
@@ -2740,6 +2734,9 @@
   </si>
   <si>
     <t>What can I pick up in Cushing, Oklahoma?</t>
+  </si>
+  <si>
+    <t>The words "I am a most unhappy man. I have unwittingly ruined my country" were written by. . .</t>
   </si>
 </sst>
 </file>
@@ -3075,8 +3072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3591,6 +3588,9 @@
       <c r="B28" t="s">
         <v>226</v>
       </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
       <c r="D28" t="s">
         <v>225</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D31" t="s">
         <v>372</v>
@@ -3932,7 +3932,7 @@
         <v>285</v>
       </c>
       <c r="C48" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D48" t="s">
         <v>287</v>
@@ -3986,7 +3986,7 @@
         <v>297</v>
       </c>
       <c r="D51" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E51" t="s">
         <v>298</v>
@@ -4003,10 +4003,10 @@
         <v>300</v>
       </c>
       <c r="D52" t="s">
+        <v>603</v>
+      </c>
+      <c r="E52" t="s">
         <v>604</v>
-      </c>
-      <c r="E52" t="s">
-        <v>605</v>
       </c>
       <c r="F52" t="s">
         <v>301</v>
@@ -4233,7 +4233,7 @@
         <v>400</v>
       </c>
       <c r="E65" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F65" t="s">
         <v>422</v>
@@ -4247,13 +4247,13 @@
         <v>411</v>
       </c>
       <c r="D66" t="s">
+        <v>528</v>
+      </c>
+      <c r="E66" t="s">
+        <v>530</v>
+      </c>
+      <c r="F66" t="s">
         <v>529</v>
-      </c>
-      <c r="E66" t="s">
-        <v>531</v>
-      </c>
-      <c r="F66" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4264,13 +4264,13 @@
         <v>412</v>
       </c>
       <c r="D67" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E67" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F67" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4281,13 +4281,13 @@
         <v>413</v>
       </c>
       <c r="D68" t="s">
+        <v>532</v>
+      </c>
+      <c r="E68" t="s">
         <v>533</v>
       </c>
-      <c r="E68" t="s">
-        <v>534</v>
-      </c>
       <c r="F68" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4335,13 +4335,13 @@
         <v>421</v>
       </c>
       <c r="D71" t="s">
+        <v>534</v>
+      </c>
+      <c r="E71" t="s">
         <v>535</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>536</v>
-      </c>
-      <c r="F71" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -4369,13 +4369,13 @@
         <v>433</v>
       </c>
       <c r="D73" t="s">
+        <v>719</v>
+      </c>
+      <c r="E73" t="s">
         <v>720</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>721</v>
-      </c>
-      <c r="F73" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4423,13 +4423,13 @@
         <v>498</v>
       </c>
       <c r="D76" t="s">
+        <v>730</v>
+      </c>
+      <c r="E76" t="s">
+        <v>733</v>
+      </c>
+      <c r="F76" t="s">
         <v>731</v>
-      </c>
-      <c r="E76" t="s">
-        <v>734</v>
-      </c>
-      <c r="F76" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4440,13 +4440,13 @@
         <v>497</v>
       </c>
       <c r="D77" t="s">
+        <v>732</v>
+      </c>
+      <c r="E77" t="s">
         <v>733</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>734</v>
-      </c>
-      <c r="F77" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4477,7 +4477,7 @@
         <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>510</v>
+        <v>523</v>
       </c>
       <c r="F79" t="s">
         <v>17</v>
@@ -4497,7 +4497,7 @@
         <v>501</v>
       </c>
       <c r="F80" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4505,16 +4505,16 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
+        <v>735</v>
+      </c>
+      <c r="D81" t="s">
         <v>736</v>
       </c>
-      <c r="D81" t="s">
-        <v>737</v>
-      </c>
       <c r="E81" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F81" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4522,16 +4522,16 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
+        <v>636</v>
+      </c>
+      <c r="D82" t="s">
         <v>637</v>
       </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>638</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>639</v>
-      </c>
-      <c r="F82" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4539,16 +4539,16 @@
         <v>10</v>
       </c>
       <c r="B83" t="s">
+        <v>516</v>
+      </c>
+      <c r="D83" t="s">
         <v>517</v>
       </c>
-      <c r="D83" t="s">
-        <v>518</v>
-      </c>
       <c r="E83" t="s">
+        <v>737</v>
+      </c>
+      <c r="F83" t="s">
         <v>738</v>
-      </c>
-      <c r="F83" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -4556,7 +4556,7 @@
         <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D84" t="s">
         <v>17</v>
@@ -4565,7 +4565,7 @@
         <v>18</v>
       </c>
       <c r="F84" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -4573,16 +4573,16 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D85" t="s">
+        <v>538</v>
+      </c>
+      <c r="E85" t="s">
         <v>539</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>540</v>
-      </c>
-      <c r="F85" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -4590,16 +4590,16 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D86" t="s">
+        <v>759</v>
+      </c>
+      <c r="E86" t="s">
         <v>760</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>761</v>
-      </c>
-      <c r="F86" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -4607,7 +4607,7 @@
         <v>10</v>
       </c>
       <c r="B87" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D87" t="s">
         <v>18</v>
@@ -4616,7 +4616,7 @@
         <v>17</v>
       </c>
       <c r="F87" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -4624,16 +4624,16 @@
         <v>10</v>
       </c>
       <c r="B88" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D88" t="s">
+        <v>762</v>
+      </c>
+      <c r="E88" t="s">
         <v>763</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>764</v>
-      </c>
-      <c r="F88" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -4641,16 +4641,16 @@
         <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D89" t="s">
+        <v>775</v>
+      </c>
+      <c r="E89" t="s">
         <v>776</v>
       </c>
-      <c r="E89" t="s">
+      <c r="F89" t="s">
         <v>777</v>
-      </c>
-      <c r="F89" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -4658,16 +4658,16 @@
         <v>10</v>
       </c>
       <c r="B90" t="s">
+        <v>526</v>
+      </c>
+      <c r="D90" t="s">
         <v>527</v>
       </c>
-      <c r="D90" t="s">
-        <v>528</v>
-      </c>
       <c r="E90" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F90" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -4675,16 +4675,16 @@
         <v>10</v>
       </c>
       <c r="B91" t="s">
+        <v>709</v>
+      </c>
+      <c r="D91" t="s">
+        <v>706</v>
+      </c>
+      <c r="E91" t="s">
+        <v>708</v>
+      </c>
+      <c r="F91" t="s">
         <v>710</v>
-      </c>
-      <c r="D91" t="s">
-        <v>707</v>
-      </c>
-      <c r="E91" t="s">
-        <v>709</v>
-      </c>
-      <c r="F91" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -4692,16 +4692,16 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
+        <v>711</v>
+      </c>
+      <c r="D92" t="s">
         <v>712</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>713</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>714</v>
-      </c>
-      <c r="F92" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -4709,13 +4709,13 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D93" t="s">
+        <v>715</v>
+      </c>
+      <c r="E93" t="s">
         <v>716</v>
-      </c>
-      <c r="E93" t="s">
-        <v>717</v>
       </c>
       <c r="F93" t="s">
         <v>446</v>
@@ -4726,16 +4726,16 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
+        <v>554</v>
+      </c>
+      <c r="D94" t="s">
         <v>555</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>556</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F94" t="s">
         <v>557</v>
-      </c>
-      <c r="F94" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -4746,13 +4746,13 @@
         <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D95" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E95" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F95" t="s">
         <v>45</v>
@@ -4766,13 +4766,13 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D96" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E96" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="F96" t="s">
         <v>45</v>
@@ -4786,16 +4786,16 @@
         <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D97" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E97" t="s">
         <v>501</v>
       </c>
       <c r="F97" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -4803,16 +4803,16 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D98" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E98" t="s">
         <v>446</v>
       </c>
       <c r="F98" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -4820,16 +4820,16 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
+        <v>551</v>
+      </c>
+      <c r="D99" t="s">
         <v>552</v>
       </c>
-      <c r="D99" t="s">
-        <v>553</v>
-      </c>
       <c r="E99" t="s">
+        <v>571</v>
+      </c>
+      <c r="F99" t="s">
         <v>572</v>
-      </c>
-      <c r="F99" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -4837,16 +4837,16 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
+        <v>566</v>
+      </c>
+      <c r="D100" t="s">
         <v>567</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>568</v>
       </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>569</v>
-      </c>
-      <c r="F100" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -4854,16 +4854,16 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
+        <v>574</v>
+      </c>
+      <c r="D101" t="s">
         <v>575</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>576</v>
       </c>
-      <c r="E101" t="s">
+      <c r="F101" t="s">
         <v>577</v>
-      </c>
-      <c r="F101" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -4871,16 +4871,16 @@
         <v>10</v>
       </c>
       <c r="B102" t="s">
+        <v>579</v>
+      </c>
+      <c r="D102" t="s">
+        <v>578</v>
+      </c>
+      <c r="E102" t="s">
         <v>580</v>
       </c>
-      <c r="D102" t="s">
-        <v>579</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="F102" t="s">
         <v>581</v>
-      </c>
-      <c r="F102" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -4888,16 +4888,16 @@
         <v>10</v>
       </c>
       <c r="B103" t="s">
+        <v>587</v>
+      </c>
+      <c r="D103" t="s">
         <v>588</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" t="s">
         <v>589</v>
       </c>
-      <c r="E103" t="s">
+      <c r="F103" t="s">
         <v>590</v>
-      </c>
-      <c r="F103" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4905,16 +4905,16 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
+        <v>594</v>
+      </c>
+      <c r="D104" t="s">
+        <v>593</v>
+      </c>
+      <c r="E104" t="s">
         <v>595</v>
       </c>
-      <c r="D104" t="s">
-        <v>594</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="F104" t="s">
         <v>596</v>
-      </c>
-      <c r="F104" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -4922,19 +4922,19 @@
         <v>10</v>
       </c>
       <c r="B105" t="s">
+        <v>597</v>
+      </c>
+      <c r="C105" t="s">
         <v>598</v>
       </c>
-      <c r="C105" t="s">
-        <v>599</v>
-      </c>
       <c r="D105" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E105" t="s">
+        <v>610</v>
+      </c>
+      <c r="F105" t="s">
         <v>611</v>
-      </c>
-      <c r="F105" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4942,16 +4942,16 @@
         <v>10</v>
       </c>
       <c r="B106" t="s">
+        <v>599</v>
+      </c>
+      <c r="D106" t="s">
         <v>600</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
         <v>601</v>
       </c>
-      <c r="E106" t="s">
+      <c r="F106" t="s">
         <v>602</v>
-      </c>
-      <c r="F106" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4959,16 +4959,16 @@
         <v>10</v>
       </c>
       <c r="B107" t="s">
+        <v>605</v>
+      </c>
+      <c r="D107" t="s">
         <v>606</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" t="s">
         <v>607</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F107" t="s">
         <v>608</v>
-      </c>
-      <c r="F107" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4976,16 +4976,16 @@
         <v>10</v>
       </c>
       <c r="B108" t="s">
+        <v>617</v>
+      </c>
+      <c r="D108" t="s">
         <v>618</v>
       </c>
-      <c r="D108" t="s">
+      <c r="E108" t="s">
         <v>619</v>
       </c>
-      <c r="E108" t="s">
+      <c r="F108" t="s">
         <v>620</v>
-      </c>
-      <c r="F108" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4993,16 +4993,16 @@
         <v>10</v>
       </c>
       <c r="B109" t="s">
+        <v>621</v>
+      </c>
+      <c r="D109" t="s">
         <v>622</v>
-      </c>
-      <c r="D109" t="s">
-        <v>623</v>
       </c>
       <c r="E109" t="s">
         <v>14</v>
       </c>
       <c r="F109" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -5010,16 +5010,16 @@
         <v>10</v>
       </c>
       <c r="B110" t="s">
+        <v>687</v>
+      </c>
+      <c r="D110" t="s">
         <v>688</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E110" t="s">
         <v>689</v>
       </c>
-      <c r="E110" t="s">
+      <c r="F110" t="s">
         <v>690</v>
-      </c>
-      <c r="F110" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -5027,16 +5027,16 @@
         <v>10</v>
       </c>
       <c r="B111" t="s">
+        <v>640</v>
+      </c>
+      <c r="D111" t="s">
         <v>641</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>642</v>
       </c>
-      <c r="E111" t="s">
+      <c r="F111" t="s">
         <v>643</v>
-      </c>
-      <c r="F111" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -5044,16 +5044,16 @@
         <v>10</v>
       </c>
       <c r="B112" t="s">
+        <v>624</v>
+      </c>
+      <c r="D112" t="s">
         <v>625</v>
       </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
+        <v>627</v>
+      </c>
+      <c r="F112" t="s">
         <v>626</v>
-      </c>
-      <c r="E112" t="s">
-        <v>628</v>
-      </c>
-      <c r="F112" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -5061,16 +5061,16 @@
         <v>10</v>
       </c>
       <c r="B113" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D113" t="s">
         <v>279</v>
       </c>
       <c r="E113" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F113" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -5078,16 +5078,16 @@
         <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D114" t="s">
+        <v>632</v>
+      </c>
+      <c r="E114" t="s">
         <v>633</v>
       </c>
-      <c r="E114" t="s">
+      <c r="F114" t="s">
         <v>634</v>
-      </c>
-      <c r="F114" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -5095,16 +5095,16 @@
         <v>10</v>
       </c>
       <c r="B115" t="s">
+        <v>653</v>
+      </c>
+      <c r="D115" t="s">
         <v>654</v>
       </c>
-      <c r="D115" t="s">
+      <c r="E115" t="s">
         <v>655</v>
       </c>
-      <c r="E115" t="s">
+      <c r="F115" t="s">
         <v>656</v>
-      </c>
-      <c r="F115" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -5112,16 +5112,16 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
+        <v>657</v>
+      </c>
+      <c r="D116" t="s">
         <v>658</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E116" t="s">
         <v>659</v>
       </c>
-      <c r="E116" t="s">
+      <c r="F116" t="s">
         <v>660</v>
-      </c>
-      <c r="F116" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -5129,16 +5129,16 @@
         <v>10</v>
       </c>
       <c r="B117" t="s">
+        <v>661</v>
+      </c>
+      <c r="D117" t="s">
         <v>662</v>
       </c>
-      <c r="D117" t="s">
+      <c r="E117" t="s">
+        <v>654</v>
+      </c>
+      <c r="F117" t="s">
         <v>663</v>
-      </c>
-      <c r="E117" t="s">
-        <v>655</v>
-      </c>
-      <c r="F117" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -5146,16 +5146,16 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D118" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E118" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F118" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -5163,16 +5163,16 @@
         <v>10</v>
       </c>
       <c r="B119" t="s">
+        <v>665</v>
+      </c>
+      <c r="D119" t="s">
         <v>666</v>
       </c>
-      <c r="D119" t="s">
+      <c r="E119" t="s">
         <v>667</v>
       </c>
-      <c r="E119" t="s">
+      <c r="F119" t="s">
         <v>668</v>
-      </c>
-      <c r="F119" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -5180,16 +5180,16 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
+        <v>671</v>
+      </c>
+      <c r="D120" t="s">
+        <v>669</v>
+      </c>
+      <c r="E120" t="s">
+        <v>670</v>
+      </c>
+      <c r="F120" t="s">
         <v>672</v>
-      </c>
-      <c r="D120" t="s">
-        <v>670</v>
-      </c>
-      <c r="E120" t="s">
-        <v>671</v>
-      </c>
-      <c r="F120" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -5197,7 +5197,7 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D121" s="2">
         <v>0.9</v>
@@ -5214,16 +5214,16 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D122" t="s">
+        <v>765</v>
+      </c>
+      <c r="E122" t="s">
         <v>766</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>767</v>
-      </c>
-      <c r="F122" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -5231,16 +5231,16 @@
         <v>10</v>
       </c>
       <c r="B123" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D123" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E123" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F123" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -5248,16 +5248,16 @@
         <v>10</v>
       </c>
       <c r="B124" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D124" t="s">
+        <v>770</v>
+      </c>
+      <c r="E124" t="s">
         <v>771</v>
       </c>
-      <c r="E124" t="s">
+      <c r="F124" t="s">
         <v>772</v>
-      </c>
-      <c r="F124" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -5265,16 +5265,16 @@
         <v>10</v>
       </c>
       <c r="B125" t="s">
+        <v>726</v>
+      </c>
+      <c r="D125" t="s">
         <v>727</v>
       </c>
-      <c r="D125" t="s">
+      <c r="E125" t="s">
         <v>728</v>
       </c>
-      <c r="E125" t="s">
+      <c r="F125" t="s">
         <v>729</v>
-      </c>
-      <c r="F125" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -5282,16 +5282,16 @@
         <v>10</v>
       </c>
       <c r="B126" t="s">
+        <v>679</v>
+      </c>
+      <c r="D126" t="s">
+        <v>678</v>
+      </c>
+      <c r="E126" t="s">
         <v>680</v>
       </c>
-      <c r="D126" t="s">
-        <v>679</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="F126" t="s">
         <v>681</v>
-      </c>
-      <c r="F126" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -5299,16 +5299,16 @@
         <v>10</v>
       </c>
       <c r="B127" t="s">
+        <v>739</v>
+      </c>
+      <c r="D127" t="s">
+        <v>593</v>
+      </c>
+      <c r="E127" t="s">
         <v>740</v>
       </c>
-      <c r="D127" t="s">
-        <v>594</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="F127" t="s">
         <v>741</v>
-      </c>
-      <c r="F127" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -5316,16 +5316,16 @@
         <v>10</v>
       </c>
       <c r="B128" t="s">
+        <v>742</v>
+      </c>
+      <c r="D128" t="s">
         <v>743</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
         <v>744</v>
       </c>
-      <c r="E128" t="s">
+      <c r="F128" t="s">
         <v>745</v>
-      </c>
-      <c r="F128" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -5333,16 +5333,16 @@
         <v>10</v>
       </c>
       <c r="B129" t="s">
+        <v>746</v>
+      </c>
+      <c r="D129" t="s">
         <v>747</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" t="s">
         <v>748</v>
       </c>
-      <c r="E129" t="s">
+      <c r="F129" t="s">
         <v>749</v>
-      </c>
-      <c r="F129" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -5350,16 +5350,16 @@
         <v>10</v>
       </c>
       <c r="B130" t="s">
+        <v>750</v>
+      </c>
+      <c r="D130" t="s">
         <v>751</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" t="s">
         <v>752</v>
       </c>
-      <c r="E130" t="s">
+      <c r="F130" t="s">
         <v>753</v>
-      </c>
-      <c r="F130" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -5367,16 +5367,16 @@
         <v>10</v>
       </c>
       <c r="B131" t="s">
+        <v>754</v>
+      </c>
+      <c r="D131" t="s">
         <v>755</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131" t="s">
         <v>756</v>
       </c>
-      <c r="E131" t="s">
+      <c r="F131" t="s">
         <v>757</v>
-      </c>
-      <c r="F131" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -5384,7 +5384,7 @@
         <v>10</v>
       </c>
       <c r="B132" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D132" s="2">
         <v>0.2</v>
@@ -5401,16 +5401,16 @@
         <v>10</v>
       </c>
       <c r="B133" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D133" t="s">
+        <v>782</v>
+      </c>
+      <c r="E133" t="s">
         <v>783</v>
       </c>
-      <c r="E133" t="s">
+      <c r="F133" t="s">
         <v>784</v>
-      </c>
-      <c r="F133" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -5418,16 +5418,16 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
+        <v>785</v>
+      </c>
+      <c r="D134" t="s">
         <v>786</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" t="s">
         <v>787</v>
       </c>
-      <c r="E134" t="s">
+      <c r="F134" t="s">
         <v>788</v>
-      </c>
-      <c r="F134" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -5435,16 +5435,16 @@
         <v>10</v>
       </c>
       <c r="B135" t="s">
+        <v>801</v>
+      </c>
+      <c r="D135" t="s">
+        <v>800</v>
+      </c>
+      <c r="E135" t="s">
         <v>802</v>
       </c>
-      <c r="D135" t="s">
-        <v>801</v>
-      </c>
-      <c r="E135" t="s">
+      <c r="F135" t="s">
         <v>803</v>
-      </c>
-      <c r="F135" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -5452,16 +5452,16 @@
         <v>10</v>
       </c>
       <c r="B136" t="s">
+        <v>804</v>
+      </c>
+      <c r="D136" t="s">
         <v>805</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" t="s">
+        <v>807</v>
+      </c>
+      <c r="F136" t="s">
         <v>806</v>
-      </c>
-      <c r="E136" t="s">
-        <v>808</v>
-      </c>
-      <c r="F136" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -5469,16 +5469,16 @@
         <v>10</v>
       </c>
       <c r="B137" t="s">
+        <v>809</v>
+      </c>
+      <c r="D137" t="s">
         <v>810</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" t="s">
         <v>811</v>
       </c>
-      <c r="E137" t="s">
+      <c r="F137" t="s">
         <v>812</v>
-      </c>
-      <c r="F137" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -5486,10 +5486,10 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D138" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E138" t="s">
         <v>41</v>
@@ -5503,16 +5503,16 @@
         <v>10</v>
       </c>
       <c r="B139" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D139" t="s">
+        <v>815</v>
+      </c>
+      <c r="E139" t="s">
         <v>816</v>
       </c>
-      <c r="E139" t="s">
+      <c r="F139" t="s">
         <v>817</v>
-      </c>
-      <c r="F139" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -5520,16 +5520,16 @@
         <v>10</v>
       </c>
       <c r="B140" t="s">
+        <v>819</v>
+      </c>
+      <c r="D140" t="s">
         <v>820</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" t="s">
         <v>821</v>
       </c>
-      <c r="E140" t="s">
+      <c r="F140" t="s">
         <v>822</v>
-      </c>
-      <c r="F140" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -5537,16 +5537,16 @@
         <v>10</v>
       </c>
       <c r="B141" t="s">
+        <v>823</v>
+      </c>
+      <c r="D141" t="s">
         <v>824</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" t="s">
         <v>825</v>
       </c>
-      <c r="E141" t="s">
+      <c r="F141" t="s">
         <v>826</v>
-      </c>
-      <c r="F141" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -5554,16 +5554,16 @@
         <v>10</v>
       </c>
       <c r="B142" t="s">
+        <v>827</v>
+      </c>
+      <c r="D142" t="s">
         <v>828</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" t="s">
         <v>829</v>
       </c>
-      <c r="E142" t="s">
+      <c r="F142" t="s">
         <v>830</v>
-      </c>
-      <c r="F142" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -5571,16 +5571,16 @@
         <v>10</v>
       </c>
       <c r="B143" t="s">
+        <v>831</v>
+      </c>
+      <c r="D143" t="s">
         <v>832</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" t="s">
         <v>833</v>
       </c>
-      <c r="E143" t="s">
+      <c r="F143" t="s">
         <v>834</v>
-      </c>
-      <c r="F143" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -5588,16 +5588,16 @@
         <v>10</v>
       </c>
       <c r="B144" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D144" t="s">
+        <v>835</v>
+      </c>
+      <c r="E144" t="s">
         <v>836</v>
       </c>
-      <c r="E144" t="s">
+      <c r="F144" t="s">
         <v>837</v>
-      </c>
-      <c r="F144" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -5605,16 +5605,16 @@
         <v>10</v>
       </c>
       <c r="B145" t="s">
+        <v>838</v>
+      </c>
+      <c r="D145" t="s">
         <v>839</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" t="s">
         <v>840</v>
       </c>
-      <c r="E145" t="s">
-        <v>841</v>
-      </c>
       <c r="F145" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -5622,16 +5622,16 @@
         <v>10</v>
       </c>
       <c r="B146" t="s">
+        <v>841</v>
+      </c>
+      <c r="D146" t="s">
         <v>842</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" t="s">
         <v>843</v>
       </c>
-      <c r="E146" t="s">
+      <c r="F146" t="s">
         <v>844</v>
-      </c>
-      <c r="F146" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -5639,7 +5639,7 @@
         <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D147" t="s">
         <v>250</v>
@@ -5648,7 +5648,7 @@
         <v>249</v>
       </c>
       <c r="F147" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -5656,16 +5656,16 @@
         <v>10</v>
       </c>
       <c r="B148" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D148" t="s">
         <v>250</v>
       </c>
       <c r="E148" t="s">
+        <v>850</v>
+      </c>
+      <c r="F148" t="s">
         <v>851</v>
-      </c>
-      <c r="F148" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -5673,16 +5673,16 @@
         <v>10</v>
       </c>
       <c r="B149" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D149" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E149" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F149" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -5690,13 +5690,13 @@
         <v>10</v>
       </c>
       <c r="B150" t="s">
+        <v>853</v>
+      </c>
+      <c r="D150" t="s">
         <v>854</v>
       </c>
-      <c r="D150" t="s">
-        <v>855</v>
-      </c>
       <c r="E150" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F150" t="s">
         <v>249</v>
@@ -5707,13 +5707,13 @@
         <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D151" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E151" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F151" t="s">
         <v>250</v>
@@ -5724,13 +5724,13 @@
         <v>10</v>
       </c>
       <c r="B152" t="s">
+        <v>906</v>
+      </c>
+      <c r="D152" t="s">
+        <v>856</v>
+      </c>
+      <c r="E152" t="s">
         <v>857</v>
-      </c>
-      <c r="D152" t="s">
-        <v>858</v>
-      </c>
-      <c r="E152" t="s">
-        <v>859</v>
       </c>
       <c r="F152" t="s">
         <v>75</v>
@@ -5744,16 +5744,16 @@
         <v>8</v>
       </c>
       <c r="C153" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D153" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E153" t="s">
         <v>41</v>
       </c>
       <c r="F153" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -5761,10 +5761,10 @@
         <v>10</v>
       </c>
       <c r="B154" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D154" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="E154" t="s">
         <v>250</v>
@@ -6210,7 +6210,7 @@
         <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E24" t="s">
         <v>192</v>
@@ -6224,7 +6224,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D25" t="s">
         <v>318</v>
@@ -6468,7 +6468,7 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D39">
         <v>1998</v>
@@ -6573,13 +6573,13 @@
         <v>434</v>
       </c>
       <c r="D45" t="s">
+        <v>701</v>
+      </c>
+      <c r="E45" t="s">
         <v>702</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>703</v>
-      </c>
-      <c r="F45" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -6587,16 +6587,16 @@
         <v>15</v>
       </c>
       <c r="B46" t="s">
+        <v>791</v>
+      </c>
+      <c r="D46" t="s">
+        <v>789</v>
+      </c>
+      <c r="E46" t="s">
+        <v>790</v>
+      </c>
+      <c r="F46" t="s">
         <v>792</v>
-      </c>
-      <c r="D46" t="s">
-        <v>790</v>
-      </c>
-      <c r="E46" t="s">
-        <v>791</v>
-      </c>
-      <c r="F46" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -6607,10 +6607,10 @@
         <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E47" t="s">
         <v>438</v>
@@ -6675,16 +6675,16 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
+        <v>512</v>
+      </c>
+      <c r="D51" t="s">
+        <v>510</v>
+      </c>
+      <c r="E51" t="s">
+        <v>511</v>
+      </c>
+      <c r="F51" t="s">
         <v>513</v>
-      </c>
-      <c r="D51" t="s">
-        <v>511</v>
-      </c>
-      <c r="E51" t="s">
-        <v>512</v>
-      </c>
-      <c r="F51" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -6709,16 +6709,16 @@
         <v>15</v>
       </c>
       <c r="B53" t="s">
+        <v>704</v>
+      </c>
+      <c r="D53" t="s">
         <v>705</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>706</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>707</v>
-      </c>
-      <c r="F53" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -6729,16 +6729,16 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
+        <v>542</v>
+      </c>
+      <c r="D54" t="s">
         <v>543</v>
-      </c>
-      <c r="D54" t="s">
-        <v>544</v>
       </c>
       <c r="E54" t="s">
         <v>501</v>
       </c>
       <c r="F54" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -6749,16 +6749,16 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
+        <v>546</v>
+      </c>
+      <c r="D55" t="s">
         <v>547</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>548</v>
       </c>
-      <c r="E55" t="s">
-        <v>549</v>
-      </c>
       <c r="F55" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -6766,16 +6766,16 @@
         <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D56" t="s">
+        <v>562</v>
+      </c>
+      <c r="E56" t="s">
         <v>563</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>564</v>
-      </c>
-      <c r="F56" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -6783,16 +6783,16 @@
         <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D57" t="s">
+        <v>793</v>
+      </c>
+      <c r="E57" t="s">
         <v>794</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>795</v>
-      </c>
-      <c r="F57" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -6800,16 +6800,16 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
+        <v>585</v>
+      </c>
+      <c r="D58" t="s">
+        <v>592</v>
+      </c>
+      <c r="E58" t="s">
         <v>586</v>
       </c>
-      <c r="D58" t="s">
-        <v>593</v>
-      </c>
-      <c r="E58" t="s">
-        <v>587</v>
-      </c>
       <c r="F58" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -6817,16 +6817,16 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
+        <v>613</v>
+      </c>
+      <c r="D59" t="s">
         <v>614</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>615</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>616</v>
-      </c>
-      <c r="F59" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -6834,16 +6834,16 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
+        <v>796</v>
+      </c>
+      <c r="D60" t="s">
         <v>797</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>798</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>799</v>
-      </c>
-      <c r="F60" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -6851,16 +6851,16 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
+        <v>628</v>
+      </c>
+      <c r="D61" t="s">
         <v>629</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>630</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>631</v>
-      </c>
-      <c r="F61" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -6868,16 +6868,16 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
+        <v>644</v>
+      </c>
+      <c r="D62" t="s">
         <v>645</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>646</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>647</v>
-      </c>
-      <c r="F62" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -6885,10 +6885,10 @@
         <v>15</v>
       </c>
       <c r="B63" t="s">
+        <v>673</v>
+      </c>
+      <c r="D63" t="s">
         <v>674</v>
-      </c>
-      <c r="D63" t="s">
-        <v>675</v>
       </c>
       <c r="E63" t="s">
         <v>91</v>
@@ -6902,7 +6902,7 @@
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D64">
         <v>2007</v>
@@ -6919,16 +6919,16 @@
         <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D65" t="s">
+        <v>692</v>
+      </c>
+      <c r="E65" t="s">
+        <v>900</v>
+      </c>
+      <c r="F65" t="s">
         <v>693</v>
-      </c>
-      <c r="E65" t="s">
-        <v>902</v>
-      </c>
-      <c r="F65" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -6936,16 +6936,16 @@
         <v>15</v>
       </c>
       <c r="B66" t="s">
+        <v>697</v>
+      </c>
+      <c r="D66" t="s">
         <v>698</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>699</v>
       </c>
-      <c r="E66" t="s">
+      <c r="F66" t="s">
         <v>700</v>
-      </c>
-      <c r="F66" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -6953,16 +6953,16 @@
         <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D67" t="s">
+        <v>722</v>
+      </c>
+      <c r="E67" t="s">
         <v>723</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>724</v>
-      </c>
-      <c r="F67" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6970,16 +6970,16 @@
         <v>15</v>
       </c>
       <c r="B68" t="s">
+        <v>683</v>
+      </c>
+      <c r="D68" t="s">
         <v>684</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>685</v>
       </c>
-      <c r="E68" t="s">
+      <c r="F68" t="s">
         <v>686</v>
-      </c>
-      <c r="F68" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -6990,16 +6990,16 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D69" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E69" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F69" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -7007,16 +7007,16 @@
         <v>15</v>
       </c>
       <c r="B70" t="s">
+        <v>874</v>
+      </c>
+      <c r="D70" t="s">
+        <v>875</v>
+      </c>
+      <c r="E70" t="s">
         <v>876</v>
       </c>
-      <c r="D70" t="s">
+      <c r="F70" t="s">
         <v>877</v>
-      </c>
-      <c r="E70" t="s">
-        <v>878</v>
-      </c>
-      <c r="F70" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -7024,16 +7024,16 @@
         <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D71" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="E71" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F71" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -7041,16 +7041,16 @@
         <v>15</v>
       </c>
       <c r="B72" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D72" t="s">
         <v>75</v>
       </c>
       <c r="E72" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="F72" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -7058,16 +7058,16 @@
         <v>15</v>
       </c>
       <c r="B73" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="D73" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E73" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="F73" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
   </sheetData>
@@ -7240,7 +7240,7 @@
         <v>221</v>
       </c>
       <c r="D9" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E9" t="s">
         <v>222</v>
@@ -7339,16 +7339,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
+        <v>884</v>
+      </c>
+      <c r="D15" t="s">
+        <v>885</v>
+      </c>
+      <c r="E15" t="s">
         <v>886</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>887</v>
-      </c>
-      <c r="E15" t="s">
-        <v>888</v>
-      </c>
-      <c r="F15" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -7356,16 +7356,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D16" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E16" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="F16" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -7376,13 +7376,13 @@
         <v>402</v>
       </c>
       <c r="D17" t="s">
+        <v>648</v>
+      </c>
+      <c r="E17" t="s">
         <v>649</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>650</v>
-      </c>
-      <c r="F17" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -7441,7 +7441,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D21" t="s">
         <v>397</v>
@@ -7458,7 +7458,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D22" t="s">
         <v>453</v>
@@ -7529,16 +7529,16 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
+        <v>894</v>
+      </c>
+      <c r="D26" t="s">
+        <v>895</v>
+      </c>
+      <c r="E26" t="s">
         <v>896</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>897</v>
-      </c>
-      <c r="E26" t="s">
-        <v>898</v>
-      </c>
-      <c r="F26" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -7546,7 +7546,7 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D27" t="s">
         <v>501</v>
@@ -7555,7 +7555,7 @@
         <v>502</v>
       </c>
       <c r="F27" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -7563,7 +7563,7 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D28" t="s">
         <v>501</v>
@@ -7572,7 +7572,7 @@
         <v>41</v>
       </c>
       <c r="F28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -7580,16 +7580,16 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
+        <v>880</v>
+      </c>
+      <c r="D29" t="s">
+        <v>881</v>
+      </c>
+      <c r="E29" t="s">
         <v>882</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>883</v>
-      </c>
-      <c r="E29" t="s">
-        <v>884</v>
-      </c>
-      <c r="F29" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -7597,7 +7597,7 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D30">
         <v>31.1</v>
@@ -7617,13 +7617,13 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D31" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F31" t="s">
         <v>394</v>
@@ -7634,16 +7634,16 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D32" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E32" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F32" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -7651,16 +7651,16 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
+        <v>862</v>
+      </c>
+      <c r="D33" t="s">
+        <v>863</v>
+      </c>
+      <c r="E33" t="s">
         <v>864</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>865</v>
-      </c>
-      <c r="E33" t="s">
-        <v>866</v>
-      </c>
-      <c r="F33" t="s">
-        <v>867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>